<commit_message>
Added function to selection module. Added soft delete to user
</commit_message>
<xml_diff>
--- a/storage/PDS.xlsx
+++ b/storage/PDS.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="451">
   <si>
     <t xml:space="preserve">        </t>
   </si>
@@ -102,12 +102,21 @@
     <t>SURNAME</t>
   </si>
   <si>
+    <t>KIRK</t>
+  </si>
+  <si>
     <t>FIRST NAME</t>
   </si>
   <si>
+    <t>WALTER</t>
+  </si>
+  <si>
     <t xml:space="preserve">NAME EXTENSION (JR., SR)                                           </t>
   </si>
   <si>
+    <t>ALMA BEASLEY</t>
+  </si>
+  <si>
     <t>Married</t>
   </si>
   <si>
@@ -115,6 +124,9 @@
   </si>
   <si>
     <t>MIDDLE NAME</t>
+  </si>
+  <si>
+    <t>LOGAN YORK</t>
   </si>
   <si>
     <t>Widow/er</t>
@@ -130,6 +142,9 @@
 (mm/dd/yyyy)  </t>
   </si>
   <si>
+    <t>03-19-1977</t>
+  </si>
+  <si>
     <t>16. CITIZENSHIP</t>
   </si>
   <si>
@@ -145,6 +160,9 @@
     <t>PLACE OF BIRTH</t>
   </si>
   <si>
+    <t>INVENTORE AD IN QUID</t>
+  </si>
+  <si>
     <t xml:space="preserve">If holder of  dual citizenship, </t>
   </si>
   <si>
@@ -160,6 +178,9 @@
     <t>SEX</t>
   </si>
   <si>
+    <t>FEMALE</t>
+  </si>
+  <si>
     <t>please indicate the details.</t>
   </si>
   <si>
@@ -172,9 +193,18 @@
     <t>CIVIL STATUS</t>
   </si>
   <si>
+    <t xml:space="preserve">Others: </t>
+  </si>
+  <si>
     <t>17. RESIDENTIAL ADDRESS</t>
   </si>
   <si>
+    <t>AMET QUI QUI MOLLIT</t>
+  </si>
+  <si>
+    <t>AUT LABORUM POSSIMUS</t>
+  </si>
+  <si>
     <t>Angola</t>
   </si>
   <si>
@@ -187,6 +217,12 @@
     <t>Antigua and Barbuda</t>
   </si>
   <si>
+    <t>OFFICIA REPELLENDUS</t>
+  </si>
+  <si>
+    <t>CONSECTETUR ET DELE</t>
+  </si>
+  <si>
     <t>Argentina</t>
   </si>
   <si>
@@ -208,6 +244,15 @@
     <t>HEIGHT (m)</t>
   </si>
   <si>
+    <t>LIBERO QUI CUMQUE SA</t>
+  </si>
+  <si>
+    <t>NON EST VERO INCIDID</t>
+  </si>
+  <si>
+    <t>ASPERNATUR UT SIT C</t>
+  </si>
+  <si>
     <t>Australia</t>
   </si>
   <si>
@@ -226,9 +271,15 @@
     <t>WEIGHT (kg)</t>
   </si>
   <si>
+    <t>NESCIUNT EUM COMMOD</t>
+  </si>
+  <si>
     <t xml:space="preserve">ZIP CODE    </t>
   </si>
   <si>
+    <t>TEMPORE AUT CUPIDIT</t>
+  </si>
+  <si>
     <t>Azerbaijan</t>
   </si>
   <si>
@@ -238,9 +289,18 @@
     <t>BLOOD TYPE</t>
   </si>
   <si>
+    <t>SAPIENTE ID IUSTO DE</t>
+  </si>
+  <si>
     <t>18. PERMANENT ADDRESS</t>
   </si>
   <si>
+    <t>AMET NECESSITATIBUS</t>
+  </si>
+  <si>
+    <t>DIGNISSIMOS QUIA COM</t>
+  </si>
+  <si>
     <t>Bahamas, The</t>
   </si>
   <si>
@@ -253,6 +313,15 @@
     <t>GSIS ID NO.</t>
   </si>
   <si>
+    <t>UNDE TEMPOR OCCAECAT</t>
+  </si>
+  <si>
+    <t>DUCIMUS LABORE APER</t>
+  </si>
+  <si>
+    <t>FACERE QUI CUMQUE IU</t>
+  </si>
+  <si>
     <t>Bangladesh</t>
   </si>
   <si>
@@ -265,6 +334,15 @@
     <t>PAG-IBIG ID NO.</t>
   </si>
   <si>
+    <t>NULLA A ALIQUID OCCA</t>
+  </si>
+  <si>
+    <t>QUIS PARIATUR CONSE</t>
+  </si>
+  <si>
+    <t>EST IPSA DOLOR ASPE</t>
+  </si>
+  <si>
     <t>Belarus</t>
   </si>
   <si>
@@ -277,6 +355,9 @@
     <t>PHILHEALTH NO.</t>
   </si>
   <si>
+    <t>AUT UT VOLUPTATE NOS</t>
+  </si>
+  <si>
     <t>Belize</t>
   </si>
   <si>
@@ -286,27 +367,45 @@
     <t>SSS NO.</t>
   </si>
   <si>
+    <t>MINIMA CONSECTETUR</t>
+  </si>
+  <si>
     <t>19. TELEPHONE NO.</t>
   </si>
   <si>
+    <t>MAIORES CUPIDATAT QU</t>
+  </si>
+  <si>
     <t>Benin</t>
   </si>
   <si>
     <t>14. TIN NO.</t>
   </si>
   <si>
+    <t>DOLOR IMPEDIT AUTE</t>
+  </si>
+  <si>
     <t>20. MOBILE NO.</t>
   </si>
   <si>
+    <t>FUGA VEL IPSAM QUIA</t>
+  </si>
+  <si>
     <t>Bhutan</t>
   </si>
   <si>
     <t>15. AGENCY EMPLOYEE NO.</t>
   </si>
   <si>
+    <t>VOLUPTAS ESSE QUIA S</t>
+  </si>
+  <si>
     <t>21. E-MAIL ADDRESS (if any)</t>
   </si>
   <si>
+    <t>KOTYTI@MAILINATOR.COM</t>
+  </si>
+  <si>
     <t>Bolivia</t>
   </si>
   <si>
@@ -322,6 +421,9 @@
     <t>SPOUSE'S SURNAME</t>
   </si>
   <si>
+    <t>LABORE VOLUPTATE CUP (deceased)</t>
+  </si>
+  <si>
     <t>23. NAME of CHILDREN  (Write full name and list all)</t>
   </si>
   <si>
@@ -334,39 +436,60 @@
     <t xml:space="preserve">  FIRST NAME</t>
   </si>
   <si>
+    <t>IPSA ODIO EX AUT EX</t>
+  </si>
+  <si>
     <t xml:space="preserve">NAME EXTENSION (JR., SR)                                     </t>
   </si>
   <si>
+    <t>NUMQUAM IN ILLUM ET</t>
+  </si>
+  <si>
     <t>Brazil</t>
   </si>
   <si>
     <t xml:space="preserve">  MIDDLE NAME</t>
   </si>
   <si>
+    <t>AUT DISTINCTIO ULLA</t>
+  </si>
+  <si>
     <t>Brunei </t>
   </si>
   <si>
     <t>OCCUPATION</t>
   </si>
   <si>
+    <t>UT NON DEBITIS ISTE</t>
+  </si>
+  <si>
     <t>Bulgaria</t>
   </si>
   <si>
     <t>EMPLOYER/BUSINESS NAME</t>
   </si>
   <si>
+    <t>VOLUPTATEM DISTINCTI</t>
+  </si>
+  <si>
     <t>Burkina Faso</t>
   </si>
   <si>
     <t>BUSINESS ADDRESS</t>
   </si>
   <si>
+    <t>REM RERUM ULLAMCO AL</t>
+  </si>
+  <si>
     <t>Burma</t>
   </si>
   <si>
     <t>TELEPHONE NO.</t>
   </si>
   <si>
+    <t>REPREHENDERIT EXPEDI</t>
+  </si>
+  <si>
     <t>Burundi</t>
   </si>
   <si>
@@ -376,15 +499,27 @@
     <t>FATHER'S SURNAME</t>
   </si>
   <si>
+    <t>SUSCIPIT CONSEQUATUR (deceased)</t>
+  </si>
+  <si>
     <t>Cambodia</t>
   </si>
   <si>
+    <t>SED AMET UNDE DOLOR</t>
+  </si>
+  <si>
     <t xml:space="preserve">NAME EXTENSION (JR., SR)                                                  </t>
   </si>
   <si>
+    <t>SED DOLORE ADIPISICI</t>
+  </si>
+  <si>
     <t>Cameroon</t>
   </si>
   <si>
+    <t>LABORIOSAM NIHIL FU</t>
+  </si>
+  <si>
     <t>Canada</t>
   </si>
   <si>
@@ -397,10 +532,19 @@
     <t>Cape Verde</t>
   </si>
   <si>
+    <t>LOREM QUI SAPIENTE M</t>
+  </si>
+  <si>
     <t>Central African Republic</t>
   </si>
   <si>
+    <t>VOLUPTAS COMMODO NON</t>
+  </si>
+  <si>
     <t>Chad</t>
+  </si>
+  <si>
+    <t>NOSTRUM OPTIO ID FA</t>
   </si>
   <si>
     <t>(Continue on separate sheet if necessary)</t>
@@ -6934,7 +7078,9 @@
         <v>12</v>
       </c>
       <c r="C10" s="380"/>
-      <c r="D10" s="385"/>
+      <c r="D10" s="385" t="s">
+        <v>13</v>
+      </c>
       <c r="E10" s="385"/>
       <c r="F10" s="385"/>
       <c r="G10" s="385"/>
@@ -6950,10 +7096,12 @@
     <row r="11" spans="1:19" customHeight="1" ht="22.5">
       <c r="A11" s="163"/>
       <c r="B11" s="396" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" s="397"/>
-      <c r="D11" s="197"/>
+      <c r="D11" s="197" t="s">
+        <v>15</v>
+      </c>
       <c r="E11" s="198"/>
       <c r="F11" s="198"/>
       <c r="G11" s="198"/>
@@ -6962,24 +7110,28 @@
       <c r="J11" s="198"/>
       <c r="K11" s="198"/>
       <c r="L11" s="365" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M11" s="366"/>
-      <c r="N11" s="252"/>
+      <c r="N11" s="252" t="s">
+        <v>17</v>
+      </c>
       <c r="P11" s="96" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="Q11" s="143" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:19" customHeight="1" ht="21.75">
       <c r="A12" s="164"/>
       <c r="B12" s="398" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C12" s="399"/>
-      <c r="D12" s="194"/>
+      <c r="D12" s="194" t="s">
+        <v>21</v>
+      </c>
       <c r="E12" s="195"/>
       <c r="F12" s="195"/>
       <c r="G12" s="195"/>
@@ -6991,25 +7143,27 @@
       <c r="M12" s="199"/>
       <c r="N12" s="200"/>
       <c r="P12" s="96" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:19" customHeight="1" ht="24">
       <c r="A13" s="226" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B13" s="379" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C13" s="380"/>
-      <c r="D13" s="268"/>
+      <c r="D13" s="268" t="s">
+        <v>26</v>
+      </c>
       <c r="E13" s="268"/>
       <c r="F13" s="269"/>
       <c r="G13" s="102" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="H13" s="145"/>
       <c r="I13" s="145"/>
@@ -7019,10 +7173,10 @@
       <c r="M13" s="360"/>
       <c r="N13" s="361"/>
       <c r="P13" s="96" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:19" customHeight="1" ht="12">
@@ -7045,17 +7199,19 @@
     </row>
     <row r="15" spans="1:19" customHeight="1" ht="24.75">
       <c r="A15" s="165" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B15" s="97" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C15" s="97"/>
-      <c r="D15" s="371"/>
+      <c r="D15" s="371" t="s">
+        <v>32</v>
+      </c>
       <c r="E15" s="371"/>
       <c r="F15" s="372"/>
       <c r="G15" s="273" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="H15" s="274"/>
       <c r="I15" s="274"/>
@@ -7065,25 +7221,27 @@
       <c r="M15" s="284"/>
       <c r="N15" s="285"/>
       <c r="P15" s="96" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:19" customHeight="1" ht="24.75">
       <c r="A16" s="166" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B16" s="97" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C16" s="98"/>
-      <c r="D16" s="387"/>
+      <c r="D16" s="387" t="s">
+        <v>38</v>
+      </c>
       <c r="E16" s="387"/>
       <c r="F16" s="320"/>
       <c r="G16" s="270" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H16" s="271"/>
       <c r="I16" s="272"/>
@@ -7093,10 +7251,10 @@
       <c r="M16" s="287"/>
       <c r="N16" s="288"/>
       <c r="P16" s="96" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:19" customHeight="1" ht="15.75">
@@ -7104,24 +7262,30 @@
         <v>6</v>
       </c>
       <c r="B17" s="279" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C17" s="280"/>
-      <c r="D17" s="277"/>
+      <c r="D17" s="277" t="s">
+        <v>43</v>
+      </c>
       <c r="E17" s="277"/>
       <c r="F17" s="277"/>
       <c r="G17" s="103" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="H17" s="104"/>
-      <c r="I17" s="354"/>
+      <c r="I17" s="354" t="s">
+        <v>45</v>
+      </c>
       <c r="J17" s="355"/>
       <c r="K17" s="355"/>
-      <c r="L17" s="355"/>
+      <c r="L17" s="355" t="s">
+        <v>46</v>
+      </c>
       <c r="M17" s="355"/>
       <c r="N17" s="362"/>
       <c r="Q17" s="3" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:19" customHeight="1" ht="9">
@@ -7134,17 +7298,17 @@
       <c r="G18" s="151"/>
       <c r="H18" s="255"/>
       <c r="I18" s="363" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="J18" s="364"/>
       <c r="K18" s="364"/>
       <c r="L18" s="364" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="M18" s="364"/>
       <c r="N18" s="367"/>
       <c r="Q18" s="3" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:19" customHeight="1" ht="5.25">
@@ -7156,14 +7320,18 @@
       <c r="F19" s="257"/>
       <c r="G19" s="151"/>
       <c r="H19" s="255"/>
-      <c r="I19" s="377"/>
+      <c r="I19" s="377" t="s">
+        <v>51</v>
+      </c>
       <c r="J19" s="312"/>
       <c r="K19" s="312"/>
-      <c r="L19" s="311"/>
+      <c r="L19" s="311" t="s">
+        <v>52</v>
+      </c>
       <c r="M19" s="312"/>
       <c r="N19" s="313"/>
       <c r="Q19" s="3" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:19" customHeight="1" ht="9.75">
@@ -7182,7 +7350,7 @@
       <c r="M20" s="314"/>
       <c r="N20" s="315"/>
       <c r="Q20" s="3" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:19" customHeight="1" ht="9">
@@ -7195,40 +7363,46 @@
       <c r="G21" s="149"/>
       <c r="H21" s="251"/>
       <c r="I21" s="316" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="J21" s="317"/>
       <c r="K21" s="317"/>
       <c r="L21" s="430" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="M21" s="431"/>
       <c r="N21" s="432"/>
       <c r="Q21" s="3" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:19" customHeight="1" ht="15.75">
       <c r="A22" s="326" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B22" s="330" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C22" s="331"/>
-      <c r="D22" s="320"/>
+      <c r="D22" s="320" t="s">
+        <v>60</v>
+      </c>
       <c r="E22" s="277"/>
       <c r="F22" s="321"/>
       <c r="G22" s="149"/>
       <c r="H22" s="251"/>
-      <c r="I22" s="354"/>
+      <c r="I22" s="354" t="s">
+        <v>61</v>
+      </c>
       <c r="J22" s="355"/>
       <c r="K22" s="355"/>
-      <c r="L22" s="355"/>
+      <c r="L22" s="355" t="s">
+        <v>62</v>
+      </c>
       <c r="M22" s="355"/>
       <c r="N22" s="362"/>
       <c r="Q22" s="3" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:19" customHeight="1" ht="8.25">
@@ -7241,67 +7415,77 @@
       <c r="G23" s="149"/>
       <c r="H23" s="251"/>
       <c r="I23" s="435" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="J23" s="436"/>
       <c r="K23" s="436"/>
       <c r="L23" s="433" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="M23" s="433"/>
       <c r="N23" s="434"/>
       <c r="Q23" s="3" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:19" customHeight="1" ht="22.5">
       <c r="A24" s="163" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B24" s="334" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="C24" s="335"/>
-      <c r="D24" s="351"/>
+      <c r="D24" s="351" t="s">
+        <v>69</v>
+      </c>
       <c r="E24" s="352"/>
       <c r="F24" s="353"/>
       <c r="G24" s="400" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="H24" s="401"/>
-      <c r="I24" s="368"/>
+      <c r="I24" s="368" t="s">
+        <v>71</v>
+      </c>
       <c r="J24" s="369"/>
       <c r="K24" s="369"/>
       <c r="L24" s="369"/>
       <c r="M24" s="369"/>
       <c r="N24" s="370"/>
       <c r="Q24" s="3" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:19" customHeight="1" ht="15.75">
       <c r="A25" s="318" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="B25" s="330" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="C25" s="331"/>
-      <c r="D25" s="320"/>
+      <c r="D25" s="320" t="s">
+        <v>75</v>
+      </c>
       <c r="E25" s="277"/>
       <c r="F25" s="321"/>
       <c r="G25" s="109" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="H25" s="99"/>
-      <c r="I25" s="354"/>
+      <c r="I25" s="354" t="s">
+        <v>77</v>
+      </c>
       <c r="J25" s="355"/>
       <c r="K25" s="355"/>
-      <c r="L25" s="355"/>
+      <c r="L25" s="355" t="s">
+        <v>78</v>
+      </c>
       <c r="M25" s="355"/>
       <c r="N25" s="362"/>
       <c r="Q25" s="3" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:19" customHeight="1" ht="9">
@@ -7314,40 +7498,46 @@
       <c r="G26" s="149"/>
       <c r="H26" s="251"/>
       <c r="I26" s="363" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="J26" s="364"/>
       <c r="K26" s="364"/>
       <c r="L26" s="364" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="M26" s="364"/>
       <c r="N26" s="367"/>
       <c r="Q26" s="3" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:19" customHeight="1" ht="15.75">
       <c r="A27" s="318" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="B27" s="330" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="C27" s="331"/>
-      <c r="D27" s="320"/>
+      <c r="D27" s="320" t="s">
+        <v>83</v>
+      </c>
       <c r="E27" s="277"/>
       <c r="F27" s="321"/>
       <c r="G27" s="151"/>
       <c r="H27" s="255"/>
-      <c r="I27" s="354"/>
+      <c r="I27" s="354" t="s">
+        <v>84</v>
+      </c>
       <c r="J27" s="355"/>
       <c r="K27" s="355"/>
-      <c r="L27" s="355"/>
+      <c r="L27" s="355" t="s">
+        <v>85</v>
+      </c>
       <c r="M27" s="355"/>
       <c r="N27" s="362"/>
       <c r="Q27" s="3" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:19" customHeight="1" ht="9">
@@ -7360,40 +7550,46 @@
       <c r="G28" s="151"/>
       <c r="H28" s="255"/>
       <c r="I28" s="412" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="J28" s="410"/>
       <c r="K28" s="410"/>
       <c r="L28" s="409" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="M28" s="410"/>
       <c r="N28" s="411"/>
       <c r="Q28" s="3" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:19" customHeight="1" ht="15.75">
       <c r="A29" s="318" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="B29" s="330" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="C29" s="331"/>
-      <c r="D29" s="320"/>
+      <c r="D29" s="320" t="s">
+        <v>90</v>
+      </c>
       <c r="E29" s="277"/>
       <c r="F29" s="321"/>
       <c r="G29" s="151"/>
       <c r="H29" s="156"/>
-      <c r="I29" s="407"/>
+      <c r="I29" s="407" t="s">
+        <v>91</v>
+      </c>
       <c r="J29" s="408"/>
       <c r="K29" s="408"/>
-      <c r="L29" s="408"/>
+      <c r="L29" s="408" t="s">
+        <v>92</v>
+      </c>
       <c r="M29" s="408"/>
       <c r="N29" s="441"/>
       <c r="Q29" s="3" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:19" customHeight="1" ht="9.75">
@@ -7406,32 +7602,34 @@
       <c r="G30" s="151"/>
       <c r="H30" s="156"/>
       <c r="I30" s="437" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="J30" s="437"/>
       <c r="K30" s="437"/>
       <c r="L30" s="437" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="M30" s="437"/>
       <c r="N30" s="438"/>
       <c r="Q30" s="3" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:19" customHeight="1" ht="24.75">
       <c r="A31" s="165" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="B31" s="97" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="C31" s="98"/>
-      <c r="D31" s="351"/>
+      <c r="D31" s="351" t="s">
+        <v>97</v>
+      </c>
       <c r="E31" s="352"/>
       <c r="F31" s="353"/>
       <c r="G31" s="439" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="H31" s="440"/>
       <c r="I31" s="356"/>
@@ -7441,83 +7639,95 @@
       <c r="M31" s="357"/>
       <c r="N31" s="358"/>
       <c r="Q31" s="3" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:19" customHeight="1" ht="24.75">
       <c r="A32" s="163" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="B32" s="97" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="C32" s="98"/>
-      <c r="D32" s="351"/>
+      <c r="D32" s="351" t="s">
+        <v>101</v>
+      </c>
       <c r="E32" s="352"/>
       <c r="F32" s="353"/>
       <c r="G32" s="373" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="H32" s="335"/>
-      <c r="I32" s="356"/>
+      <c r="I32" s="356" t="s">
+        <v>103</v>
+      </c>
       <c r="J32" s="357"/>
       <c r="K32" s="357"/>
       <c r="L32" s="357"/>
       <c r="M32" s="357"/>
       <c r="N32" s="358"/>
       <c r="Q32" s="3" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:19" customHeight="1" ht="24.75">
       <c r="A33" s="402" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="B33" s="335"/>
       <c r="C33" s="403"/>
-      <c r="D33" s="351"/>
+      <c r="D33" s="351" t="s">
+        <v>106</v>
+      </c>
       <c r="E33" s="352"/>
       <c r="F33" s="353"/>
       <c r="G33" s="196" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="H33" s="150"/>
-      <c r="I33" s="356"/>
+      <c r="I33" s="356" t="s">
+        <v>108</v>
+      </c>
       <c r="J33" s="357"/>
       <c r="K33" s="357"/>
       <c r="L33" s="357"/>
       <c r="M33" s="357"/>
       <c r="N33" s="358"/>
       <c r="Q33" s="3" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:19" customHeight="1" ht="24.75">
       <c r="A34" s="168" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="B34" s="254"/>
       <c r="C34" s="152"/>
-      <c r="D34" s="390"/>
+      <c r="D34" s="390" t="s">
+        <v>111</v>
+      </c>
       <c r="E34" s="391"/>
       <c r="F34" s="392"/>
       <c r="G34" s="109" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="H34" s="99"/>
-      <c r="I34" s="356"/>
+      <c r="I34" s="356" t="s">
+        <v>113</v>
+      </c>
       <c r="J34" s="357"/>
       <c r="K34" s="357"/>
       <c r="L34" s="357"/>
       <c r="M34" s="357"/>
       <c r="N34" s="358"/>
       <c r="Q34" s="3" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:19" customHeight="1" ht="16.5">
       <c r="A35" s="205" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="B35" s="206"/>
       <c r="C35" s="206"/>
@@ -7533,49 +7743,55 @@
       <c r="M35" s="206"/>
       <c r="N35" s="207"/>
       <c r="Q35" s="3" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:19" customHeight="1" ht="21">
       <c r="A36" s="102" t="s">
-        <v>84</v>
+        <v>117</v>
       </c>
       <c r="B36" s="215" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="C36" s="216"/>
-      <c r="D36" s="309"/>
+      <c r="D36" s="309" t="s">
+        <v>119</v>
+      </c>
       <c r="E36" s="309"/>
       <c r="F36" s="309"/>
       <c r="G36" s="309"/>
       <c r="H36" s="309"/>
       <c r="I36" s="291" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="J36" s="291"/>
       <c r="K36" s="291"/>
       <c r="L36" s="292"/>
       <c r="M36" s="328" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="N36" s="329"/>
       <c r="Q36" s="3" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:19" customHeight="1" ht="21">
       <c r="A37" s="149"/>
       <c r="B37" s="255" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="C37" s="156"/>
-      <c r="D37" s="404"/>
+      <c r="D37" s="404" t="s">
+        <v>124</v>
+      </c>
       <c r="E37" s="405"/>
       <c r="F37" s="406"/>
       <c r="G37" s="247" t="s">
-        <v>90</v>
-      </c>
-      <c r="H37" s="248"/>
+        <v>125</v>
+      </c>
+      <c r="H37" s="248" t="s">
+        <v>126</v>
+      </c>
       <c r="I37" s="293"/>
       <c r="J37" s="266"/>
       <c r="K37" s="266"/>
@@ -7583,16 +7799,18 @@
       <c r="M37" s="289"/>
       <c r="N37" s="290"/>
       <c r="Q37" s="3" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:19" customHeight="1" ht="21">
       <c r="A38" s="169"/>
       <c r="B38" s="210" t="s">
-        <v>92</v>
+        <v>128</v>
       </c>
       <c r="C38" s="209"/>
-      <c r="D38" s="404"/>
+      <c r="D38" s="404" t="s">
+        <v>129</v>
+      </c>
       <c r="E38" s="405"/>
       <c r="F38" s="405"/>
       <c r="G38" s="405"/>
@@ -7604,16 +7822,18 @@
       <c r="M38" s="289"/>
       <c r="N38" s="290"/>
       <c r="Q38" s="3" t="s">
-        <v>93</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:19" customHeight="1" ht="21">
       <c r="A39" s="170"/>
       <c r="B39" s="97" t="s">
-        <v>94</v>
+        <v>131</v>
       </c>
       <c r="C39" s="98"/>
-      <c r="D39" s="310"/>
+      <c r="D39" s="310" t="s">
+        <v>132</v>
+      </c>
       <c r="E39" s="310"/>
       <c r="F39" s="310"/>
       <c r="G39" s="310"/>
@@ -7625,16 +7845,18 @@
       <c r="M39" s="289"/>
       <c r="N39" s="290"/>
       <c r="Q39" s="3" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:19" customHeight="1" ht="21">
       <c r="A40" s="170"/>
       <c r="B40" s="97" t="s">
-        <v>96</v>
+        <v>134</v>
       </c>
       <c r="C40" s="98"/>
-      <c r="D40" s="310"/>
+      <c r="D40" s="310" t="s">
+        <v>135</v>
+      </c>
       <c r="E40" s="310"/>
       <c r="F40" s="310"/>
       <c r="G40" s="310"/>
@@ -7646,16 +7868,18 @@
       <c r="M40" s="289"/>
       <c r="N40" s="290"/>
       <c r="Q40" s="3" t="s">
-        <v>97</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:19" customHeight="1" ht="21">
       <c r="A41" s="170"/>
       <c r="B41" s="97" t="s">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="C41" s="98"/>
-      <c r="D41" s="310"/>
+      <c r="D41" s="310" t="s">
+        <v>138</v>
+      </c>
       <c r="E41" s="310"/>
       <c r="F41" s="310"/>
       <c r="G41" s="310"/>
@@ -7667,16 +7891,18 @@
       <c r="M41" s="289"/>
       <c r="N41" s="290"/>
       <c r="Q41" s="3" t="s">
-        <v>99</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:19" customHeight="1" ht="21">
       <c r="A42" s="103"/>
       <c r="B42" s="104" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="C42" s="137"/>
-      <c r="D42" s="310"/>
+      <c r="D42" s="310" t="s">
+        <v>141</v>
+      </c>
       <c r="E42" s="310"/>
       <c r="F42" s="310"/>
       <c r="G42" s="310"/>
@@ -7688,18 +7914,20 @@
       <c r="M42" s="289"/>
       <c r="N42" s="290"/>
       <c r="Q42" s="3" t="s">
-        <v>101</v>
+        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:19" customHeight="1" ht="21">
       <c r="A43" s="208" t="s">
-        <v>102</v>
+        <v>143</v>
       </c>
       <c r="B43" s="213" t="s">
-        <v>103</v>
+        <v>144</v>
       </c>
       <c r="C43" s="104"/>
-      <c r="D43" s="310"/>
+      <c r="D43" s="310" t="s">
+        <v>145</v>
+      </c>
       <c r="E43" s="310"/>
       <c r="F43" s="310"/>
       <c r="G43" s="310"/>
@@ -7711,22 +7939,26 @@
       <c r="M43" s="289"/>
       <c r="N43" s="290"/>
       <c r="Q43" s="3" t="s">
-        <v>104</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:19" customHeight="1" ht="21">
       <c r="A44" s="149"/>
       <c r="B44" s="251" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C44" s="251"/>
-      <c r="D44" s="404"/>
+      <c r="D44" s="404" t="s">
+        <v>147</v>
+      </c>
       <c r="E44" s="405"/>
       <c r="F44" s="406"/>
       <c r="G44" s="247" t="s">
-        <v>105</v>
-      </c>
-      <c r="H44" s="248"/>
+        <v>148</v>
+      </c>
+      <c r="H44" s="248" t="s">
+        <v>149</v>
+      </c>
       <c r="I44" s="266"/>
       <c r="J44" s="266"/>
       <c r="K44" s="266"/>
@@ -7734,16 +7966,18 @@
       <c r="M44" s="289"/>
       <c r="N44" s="290"/>
       <c r="Q44" s="3" t="s">
-        <v>106</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="1:19" customHeight="1" ht="21">
       <c r="A45" s="169"/>
       <c r="B45" s="203" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C45" s="203"/>
-      <c r="D45" s="404"/>
+      <c r="D45" s="404" t="s">
+        <v>151</v>
+      </c>
       <c r="E45" s="405"/>
       <c r="F45" s="405"/>
       <c r="G45" s="405"/>
@@ -7755,15 +7989,15 @@
       <c r="M45" s="289"/>
       <c r="N45" s="290"/>
       <c r="Q45" s="3" t="s">
-        <v>107</v>
+        <v>152</v>
       </c>
     </row>
     <row r="46" spans="1:19" customHeight="1" ht="21">
       <c r="A46" s="149" t="s">
-        <v>108</v>
+        <v>153</v>
       </c>
       <c r="B46" s="104" t="s">
-        <v>109</v>
+        <v>154</v>
       </c>
       <c r="C46" s="104"/>
       <c r="D46" s="308"/>
@@ -7778,7 +8012,7 @@
       <c r="M46" s="289"/>
       <c r="N46" s="290"/>
       <c r="Q46" s="3" t="s">
-        <v>110</v>
+        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:19" customHeight="1" ht="21">
@@ -7787,7 +8021,9 @@
         <v>12</v>
       </c>
       <c r="C47" s="251"/>
-      <c r="D47" s="461"/>
+      <c r="D47" s="461" t="s">
+        <v>156</v>
+      </c>
       <c r="E47" s="461"/>
       <c r="F47" s="461"/>
       <c r="G47" s="461"/>
@@ -7799,16 +8035,18 @@
       <c r="M47" s="289"/>
       <c r="N47" s="290"/>
       <c r="Q47" s="3" t="s">
-        <v>111</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:19" customHeight="1" ht="21">
       <c r="A48" s="149"/>
       <c r="B48" s="251" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C48" s="251"/>
-      <c r="D48" s="461"/>
+      <c r="D48" s="461" t="s">
+        <v>158</v>
+      </c>
       <c r="E48" s="461"/>
       <c r="F48" s="461"/>
       <c r="G48" s="461"/>
@@ -7820,22 +8058,24 @@
       <c r="M48" s="289"/>
       <c r="N48" s="290"/>
       <c r="Q48" s="3" t="s">
-        <v>112</v>
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:19" customHeight="1" ht="21">
       <c r="A49" s="171"/>
       <c r="B49" s="204" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C49" s="204"/>
-      <c r="D49" s="301"/>
+      <c r="D49" s="301" t="s">
+        <v>160</v>
+      </c>
       <c r="E49" s="301"/>
       <c r="F49" s="301"/>
       <c r="G49" s="301"/>
       <c r="H49" s="301"/>
       <c r="I49" s="299" t="s">
-        <v>113</v>
+        <v>161</v>
       </c>
       <c r="J49" s="299"/>
       <c r="K49" s="299"/>
@@ -7843,12 +8083,12 @@
       <c r="M49" s="299"/>
       <c r="N49" s="300"/>
       <c r="Q49" s="3" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
     </row>
     <row r="50" spans="1:19" customHeight="1" ht="15.75">
       <c r="A50" s="172" t="s">
-        <v>115</v>
+        <v>163</v>
       </c>
       <c r="B50" s="172"/>
       <c r="C50" s="100"/>
@@ -7858,7 +8098,7 @@
       <c r="G50" s="101"/>
       <c r="H50" s="101"/>
       <c r="I50" s="388" t="s">
-        <v>116</v>
+        <v>164</v>
       </c>
       <c r="J50" s="388"/>
       <c r="K50" s="388"/>
@@ -7866,42 +8106,42 @@
       <c r="M50" s="388"/>
       <c r="N50" s="389"/>
       <c r="Q50" s="3" t="s">
-        <v>117</v>
+        <v>165</v>
       </c>
     </row>
     <row r="51" spans="1:19" customHeight="1" ht="14.25">
       <c r="A51" s="381" t="s">
-        <v>118</v>
+        <v>166</v>
       </c>
       <c r="B51" s="413" t="s">
-        <v>119</v>
+        <v>167</v>
       </c>
       <c r="C51" s="413"/>
       <c r="D51" s="416" t="s">
-        <v>120</v>
+        <v>168</v>
       </c>
       <c r="E51" s="417"/>
       <c r="F51" s="418"/>
       <c r="G51" s="416" t="s">
-        <v>121</v>
+        <v>169</v>
       </c>
       <c r="H51" s="417"/>
       <c r="I51" s="462"/>
       <c r="J51" s="302" t="s">
-        <v>122</v>
+        <v>170</v>
       </c>
       <c r="K51" s="303"/>
       <c r="L51" s="459" t="s">
-        <v>123</v>
+        <v>171</v>
       </c>
       <c r="M51" s="383" t="s">
-        <v>124</v>
+        <v>172</v>
       </c>
       <c r="N51" s="306" t="s">
-        <v>125</v>
+        <v>173</v>
       </c>
       <c r="Q51" s="3" t="s">
-        <v>126</v>
+        <v>174</v>
       </c>
     </row>
     <row r="52" spans="1:19" customHeight="1" ht="19.5">
@@ -7920,7 +8160,7 @@
       <c r="M52" s="383"/>
       <c r="N52" s="306"/>
       <c r="Q52" s="3" t="s">
-        <v>127</v>
+        <v>175</v>
       </c>
     </row>
     <row r="53" spans="1:19" customHeight="1" ht="14.25">
@@ -7934,10 +8174,10 @@
       <c r="H53" s="423"/>
       <c r="I53" s="464"/>
       <c r="J53" s="105" t="s">
-        <v>128</v>
+        <v>176</v>
       </c>
       <c r="K53" s="106" t="s">
-        <v>129</v>
+        <v>177</v>
       </c>
       <c r="L53" s="460"/>
       <c r="M53" s="384"/>
@@ -7945,13 +8185,13 @@
       <c r="O53" s="107"/>
       <c r="P53" s="107"/>
       <c r="Q53" s="3" t="s">
-        <v>130</v>
+        <v>178</v>
       </c>
     </row>
     <row r="54" spans="1:19" customHeight="1" ht="28.5">
       <c r="A54" s="217"/>
       <c r="B54" s="218" t="s">
-        <v>131</v>
+        <v>179</v>
       </c>
       <c r="C54" s="218"/>
       <c r="D54" s="424"/>
@@ -7966,13 +8206,13 @@
       <c r="M54" s="18"/>
       <c r="N54" s="153"/>
       <c r="Q54" s="3" t="s">
-        <v>132</v>
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:19" customHeight="1" ht="28.5">
       <c r="A55" s="217"/>
       <c r="B55" s="218" t="s">
-        <v>133</v>
+        <v>181</v>
       </c>
       <c r="C55" s="218"/>
       <c r="D55" s="424"/>
@@ -7987,13 +8227,13 @@
       <c r="M55" s="19"/>
       <c r="N55" s="153"/>
       <c r="Q55" s="3" t="s">
-        <v>134</v>
+        <v>182</v>
       </c>
     </row>
     <row r="56" spans="1:19" customHeight="1" ht="28.5">
       <c r="A56" s="217"/>
       <c r="B56" s="218" t="s">
-        <v>135</v>
+        <v>183</v>
       </c>
       <c r="C56" s="218"/>
       <c r="D56" s="424"/>
@@ -8008,13 +8248,13 @@
       <c r="M56" s="18"/>
       <c r="N56" s="153"/>
       <c r="Q56" s="3" t="s">
-        <v>136</v>
+        <v>184</v>
       </c>
     </row>
     <row r="57" spans="1:19" customHeight="1" ht="28.5">
       <c r="A57" s="217"/>
       <c r="B57" s="218" t="s">
-        <v>137</v>
+        <v>185</v>
       </c>
       <c r="C57" s="218"/>
       <c r="D57" s="424"/>
@@ -8029,13 +8269,13 @@
       <c r="M57" s="19"/>
       <c r="N57" s="153"/>
       <c r="Q57" s="3" t="s">
-        <v>138</v>
+        <v>186</v>
       </c>
     </row>
     <row r="58" spans="1:19" customHeight="1" ht="28.5">
       <c r="A58" s="219"/>
       <c r="B58" s="220" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="C58" s="220"/>
       <c r="D58" s="427"/>
@@ -8050,12 +8290,12 @@
       <c r="M58" s="21"/>
       <c r="N58" s="153"/>
       <c r="Q58" s="3" t="s">
-        <v>140</v>
+        <v>188</v>
       </c>
     </row>
     <row r="59" spans="1:19" customHeight="1" ht="12">
       <c r="A59" s="448" t="s">
-        <v>113</v>
+        <v>161</v>
       </c>
       <c r="B59" s="449"/>
       <c r="C59" s="449"/>
@@ -8071,12 +8311,12 @@
       <c r="M59" s="449"/>
       <c r="N59" s="450"/>
       <c r="Q59" s="3" t="s">
-        <v>141</v>
+        <v>189</v>
       </c>
     </row>
     <row r="60" spans="1:19" customHeight="1" ht="27.75">
       <c r="A60" s="445" t="s">
-        <v>142</v>
+        <v>190</v>
       </c>
       <c r="B60" s="446"/>
       <c r="C60" s="447"/>
@@ -8087,19 +8327,19 @@
       <c r="H60" s="455"/>
       <c r="I60" s="456"/>
       <c r="J60" s="457" t="s">
-        <v>143</v>
+        <v>191</v>
       </c>
       <c r="K60" s="458"/>
       <c r="L60" s="451"/>
       <c r="M60" s="452"/>
       <c r="N60" s="453"/>
       <c r="Q60" s="3" t="s">
-        <v>144</v>
+        <v>192</v>
       </c>
     </row>
     <row r="61" spans="1:19" customHeight="1" ht="12" s="143" customFormat="1">
       <c r="A61" s="442" t="s">
-        <v>145</v>
+        <v>193</v>
       </c>
       <c r="B61" s="443"/>
       <c r="C61" s="443"/>
@@ -8115,7 +8355,7 @@
       <c r="M61" s="443"/>
       <c r="N61" s="444"/>
       <c r="Q61" s="233" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
     </row>
     <row r="62" spans="1:19" customHeight="1" ht="14.25">
@@ -8134,7 +8374,7 @@
       <c r="M62" s="108"/>
       <c r="N62" s="108"/>
       <c r="Q62" s="3" t="s">
-        <v>147</v>
+        <v>195</v>
       </c>
     </row>
     <row r="63" spans="1:19" customHeight="1" ht="14.25">
@@ -8153,7 +8393,7 @@
       <c r="M63" s="108"/>
       <c r="N63" s="108"/>
       <c r="Q63" s="3" t="s">
-        <v>148</v>
+        <v>196</v>
       </c>
     </row>
     <row r="64" spans="1:19" customHeight="1" ht="28.5">
@@ -8172,7 +8412,7 @@
       <c r="M64" s="108"/>
       <c r="N64" s="108"/>
       <c r="Q64" s="3" t="s">
-        <v>149</v>
+        <v>197</v>
       </c>
     </row>
     <row r="65" spans="1:19" customHeight="1" ht="14.25">
@@ -8191,7 +8431,7 @@
       <c r="M65" s="108"/>
       <c r="N65" s="108"/>
       <c r="Q65" s="3" t="s">
-        <v>150</v>
+        <v>198</v>
       </c>
     </row>
     <row r="66" spans="1:19" customHeight="1" ht="14.25">
@@ -8210,7 +8450,7 @@
       <c r="M66" s="108"/>
       <c r="N66" s="108"/>
       <c r="Q66" s="3" t="s">
-        <v>151</v>
+        <v>199</v>
       </c>
     </row>
     <row r="67" spans="1:19" customHeight="1" ht="14.25">
@@ -8229,7 +8469,7 @@
       <c r="M67" s="108"/>
       <c r="N67" s="108"/>
       <c r="Q67" s="3" t="s">
-        <v>152</v>
+        <v>200</v>
       </c>
     </row>
     <row r="68" spans="1:19" customHeight="1" ht="14.25">
@@ -8248,7 +8488,7 @@
       <c r="M68" s="108"/>
       <c r="N68" s="108"/>
       <c r="Q68" s="3" t="s">
-        <v>153</v>
+        <v>201</v>
       </c>
     </row>
     <row r="69" spans="1:19" customHeight="1" ht="28.5">
@@ -8267,7 +8507,7 @@
       <c r="M69" s="108"/>
       <c r="N69" s="108"/>
       <c r="Q69" s="3" t="s">
-        <v>154</v>
+        <v>202</v>
       </c>
     </row>
     <row r="70" spans="1:19" customHeight="1" ht="14.25">
@@ -8286,7 +8526,7 @@
       <c r="M70" s="108"/>
       <c r="N70" s="108"/>
       <c r="Q70" s="3" t="s">
-        <v>155</v>
+        <v>203</v>
       </c>
     </row>
     <row r="71" spans="1:19" customHeight="1" ht="14.25">
@@ -8305,7 +8545,7 @@
       <c r="M71" s="108"/>
       <c r="N71" s="108"/>
       <c r="Q71" s="3" t="s">
-        <v>156</v>
+        <v>204</v>
       </c>
     </row>
     <row r="72" spans="1:19" customHeight="1" ht="14.25">
@@ -8324,7 +8564,7 @@
       <c r="M72" s="108"/>
       <c r="N72" s="108"/>
       <c r="Q72" s="3" t="s">
-        <v>157</v>
+        <v>205</v>
       </c>
     </row>
     <row r="73" spans="1:19" customHeight="1" ht="14.25">
@@ -8343,7 +8583,7 @@
       <c r="M73" s="108"/>
       <c r="N73" s="108"/>
       <c r="Q73" s="3" t="s">
-        <v>158</v>
+        <v>206</v>
       </c>
     </row>
     <row r="74" spans="1:19" customHeight="1" ht="14.25">
@@ -8362,7 +8602,7 @@
       <c r="M74" s="108"/>
       <c r="N74" s="108"/>
       <c r="Q74" s="3" t="s">
-        <v>159</v>
+        <v>207</v>
       </c>
     </row>
     <row r="75" spans="1:19" customHeight="1" ht="14.25">
@@ -8381,7 +8621,7 @@
       <c r="M75" s="108"/>
       <c r="N75" s="108"/>
       <c r="Q75" s="3" t="s">
-        <v>160</v>
+        <v>208</v>
       </c>
     </row>
     <row r="76" spans="1:19" customHeight="1" ht="14.25">
@@ -8400,7 +8640,7 @@
       <c r="M76" s="108"/>
       <c r="N76" s="108"/>
       <c r="Q76" s="3" t="s">
-        <v>161</v>
+        <v>209</v>
       </c>
     </row>
     <row r="77" spans="1:19" customHeight="1" ht="14.25">
@@ -8419,7 +8659,7 @@
       <c r="M77" s="108"/>
       <c r="N77" s="108"/>
       <c r="Q77" s="3" t="s">
-        <v>162</v>
+        <v>210</v>
       </c>
     </row>
     <row r="78" spans="1:19" customHeight="1" ht="14.25">
@@ -8438,7 +8678,7 @@
       <c r="M78" s="108"/>
       <c r="N78" s="108"/>
       <c r="Q78" s="3" t="s">
-        <v>163</v>
+        <v>211</v>
       </c>
     </row>
     <row r="79" spans="1:19" customHeight="1" ht="14.25">
@@ -8457,7 +8697,7 @@
       <c r="M79" s="108"/>
       <c r="N79" s="108"/>
       <c r="Q79" s="3" t="s">
-        <v>164</v>
+        <v>212</v>
       </c>
     </row>
     <row r="80" spans="1:19" customHeight="1" ht="14.25">
@@ -8476,7 +8716,7 @@
       <c r="M80" s="108"/>
       <c r="N80" s="108"/>
       <c r="Q80" s="3" t="s">
-        <v>165</v>
+        <v>213</v>
       </c>
     </row>
     <row r="81" spans="1:19" customHeight="1" ht="14.25">
@@ -8495,7 +8735,7 @@
       <c r="M81" s="108"/>
       <c r="N81" s="108"/>
       <c r="Q81" s="3" t="s">
-        <v>166</v>
+        <v>214</v>
       </c>
     </row>
     <row r="82" spans="1:19" customHeight="1" ht="14.25">
@@ -8514,7 +8754,7 @@
       <c r="M82" s="108"/>
       <c r="N82" s="108"/>
       <c r="Q82" s="3" t="s">
-        <v>167</v>
+        <v>215</v>
       </c>
     </row>
     <row r="83" spans="1:19" customHeight="1" ht="14.25">
@@ -8533,7 +8773,7 @@
       <c r="M83" s="108"/>
       <c r="N83" s="108"/>
       <c r="Q83" s="3" t="s">
-        <v>168</v>
+        <v>216</v>
       </c>
     </row>
     <row r="84" spans="1:19" customHeight="1" ht="14.25">
@@ -8552,7 +8792,7 @@
       <c r="M84" s="108"/>
       <c r="N84" s="108"/>
       <c r="Q84" s="3" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
     </row>
     <row r="85" spans="1:19" customHeight="1" ht="28.5">
@@ -8571,7 +8811,7 @@
       <c r="M85" s="108"/>
       <c r="N85" s="108"/>
       <c r="Q85" s="3" t="s">
-        <v>170</v>
+        <v>218</v>
       </c>
     </row>
     <row r="86" spans="1:19" customHeight="1" ht="14.25">
@@ -8590,7 +8830,7 @@
       <c r="M86" s="108"/>
       <c r="N86" s="108"/>
       <c r="Q86" s="3" t="s">
-        <v>171</v>
+        <v>219</v>
       </c>
     </row>
     <row r="87" spans="1:19" customHeight="1" ht="14.25">
@@ -8609,7 +8849,7 @@
       <c r="M87" s="108"/>
       <c r="N87" s="108"/>
       <c r="Q87" s="3" t="s">
-        <v>172</v>
+        <v>220</v>
       </c>
     </row>
     <row r="88" spans="1:19" customHeight="1" ht="14.25">
@@ -8628,7 +8868,7 @@
       <c r="M88" s="108"/>
       <c r="N88" s="108"/>
       <c r="Q88" s="3" t="s">
-        <v>173</v>
+        <v>221</v>
       </c>
     </row>
     <row r="89" spans="1:19" customHeight="1" ht="14.25">
@@ -8647,7 +8887,7 @@
       <c r="M89" s="108"/>
       <c r="N89" s="108"/>
       <c r="Q89" s="3" t="s">
-        <v>174</v>
+        <v>222</v>
       </c>
     </row>
     <row r="90" spans="1:19" customHeight="1" ht="14.25">
@@ -8666,7 +8906,7 @@
       <c r="M90" s="108"/>
       <c r="N90" s="108"/>
       <c r="Q90" s="3" t="s">
-        <v>175</v>
+        <v>223</v>
       </c>
     </row>
     <row r="91" spans="1:19" customHeight="1" ht="14.25">
@@ -8685,7 +8925,7 @@
       <c r="M91" s="108"/>
       <c r="N91" s="108"/>
       <c r="Q91" s="3" t="s">
-        <v>176</v>
+        <v>224</v>
       </c>
     </row>
     <row r="92" spans="1:19" customHeight="1" ht="14.25">
@@ -8704,7 +8944,7 @@
       <c r="M92" s="108"/>
       <c r="N92" s="108"/>
       <c r="Q92" s="3" t="s">
-        <v>177</v>
+        <v>225</v>
       </c>
     </row>
     <row r="93" spans="1:19" customHeight="1" ht="14.25">
@@ -8723,7 +8963,7 @@
       <c r="M93" s="108"/>
       <c r="N93" s="108"/>
       <c r="Q93" s="3" t="s">
-        <v>178</v>
+        <v>226</v>
       </c>
     </row>
     <row r="94" spans="1:19" customHeight="1" ht="14.25">
@@ -8742,7 +8982,7 @@
       <c r="M94" s="108"/>
       <c r="N94" s="108"/>
       <c r="Q94" s="3" t="s">
-        <v>179</v>
+        <v>227</v>
       </c>
     </row>
     <row r="95" spans="1:19" customHeight="1" ht="14.25">
@@ -8761,7 +9001,7 @@
       <c r="M95" s="108"/>
       <c r="N95" s="108"/>
       <c r="Q95" s="3" t="s">
-        <v>180</v>
+        <v>228</v>
       </c>
     </row>
     <row r="96" spans="1:19" customHeight="1" ht="14.25">
@@ -8780,7 +9020,7 @@
       <c r="M96" s="108"/>
       <c r="N96" s="108"/>
       <c r="Q96" s="3" t="s">
-        <v>181</v>
+        <v>229</v>
       </c>
     </row>
     <row r="97" spans="1:19" customHeight="1" ht="14.25">
@@ -8799,7 +9039,7 @@
       <c r="M97" s="108"/>
       <c r="N97" s="108"/>
       <c r="Q97" s="3" t="s">
-        <v>182</v>
+        <v>230</v>
       </c>
     </row>
     <row r="98" spans="1:19" customHeight="1" ht="14.25">
@@ -8818,7 +9058,7 @@
       <c r="M98" s="108"/>
       <c r="N98" s="108"/>
       <c r="Q98" s="3" t="s">
-        <v>183</v>
+        <v>231</v>
       </c>
     </row>
     <row r="99" spans="1:19" customHeight="1" ht="14.25">
@@ -8837,7 +9077,7 @@
       <c r="M99" s="108"/>
       <c r="N99" s="108"/>
       <c r="Q99" s="3" t="s">
-        <v>184</v>
+        <v>232</v>
       </c>
     </row>
     <row r="100" spans="1:19" customHeight="1" ht="14.25">
@@ -8856,7 +9096,7 @@
       <c r="M100" s="108"/>
       <c r="N100" s="108"/>
       <c r="Q100" s="3" t="s">
-        <v>185</v>
+        <v>233</v>
       </c>
     </row>
     <row r="101" spans="1:19" customHeight="1" ht="14.25">
@@ -8875,7 +9115,7 @@
       <c r="M101" s="108"/>
       <c r="N101" s="108"/>
       <c r="Q101" s="3" t="s">
-        <v>186</v>
+        <v>234</v>
       </c>
     </row>
     <row r="102" spans="1:19" customHeight="1" ht="14.25">
@@ -8894,7 +9134,7 @@
       <c r="M102" s="108"/>
       <c r="N102" s="108"/>
       <c r="Q102" s="3" t="s">
-        <v>187</v>
+        <v>235</v>
       </c>
     </row>
     <row r="103" spans="1:19" customHeight="1" ht="14.25">
@@ -8913,7 +9153,7 @@
       <c r="M103" s="108"/>
       <c r="N103" s="108"/>
       <c r="Q103" s="3" t="s">
-        <v>188</v>
+        <v>236</v>
       </c>
     </row>
     <row r="104" spans="1:19" customHeight="1" ht="14.25">
@@ -8932,7 +9172,7 @@
       <c r="M104" s="108"/>
       <c r="N104" s="108"/>
       <c r="Q104" s="3" t="s">
-        <v>189</v>
+        <v>237</v>
       </c>
     </row>
     <row r="105" spans="1:19" customHeight="1" ht="14.25">
@@ -8951,7 +9191,7 @@
       <c r="M105" s="108"/>
       <c r="N105" s="108"/>
       <c r="Q105" s="3" t="s">
-        <v>190</v>
+        <v>238</v>
       </c>
     </row>
     <row r="106" spans="1:19" customHeight="1" ht="14.25">
@@ -8970,7 +9210,7 @@
       <c r="M106" s="108"/>
       <c r="N106" s="108"/>
       <c r="Q106" s="3" t="s">
-        <v>191</v>
+        <v>239</v>
       </c>
     </row>
     <row r="107" spans="1:19" customHeight="1" ht="14.25">
@@ -8989,7 +9229,7 @@
       <c r="M107" s="108"/>
       <c r="N107" s="108"/>
       <c r="Q107" s="3" t="s">
-        <v>192</v>
+        <v>240</v>
       </c>
     </row>
     <row r="108" spans="1:19" customHeight="1" ht="14.25">
@@ -9008,7 +9248,7 @@
       <c r="M108" s="108"/>
       <c r="N108" s="108"/>
       <c r="Q108" s="3" t="s">
-        <v>193</v>
+        <v>241</v>
       </c>
     </row>
     <row r="109" spans="1:19" customHeight="1" ht="14.25">
@@ -9027,7 +9267,7 @@
       <c r="M109" s="108"/>
       <c r="N109" s="108"/>
       <c r="Q109" s="3" t="s">
-        <v>194</v>
+        <v>242</v>
       </c>
     </row>
     <row r="110" spans="1:19" customHeight="1" ht="14.25">
@@ -9046,7 +9286,7 @@
       <c r="M110" s="108"/>
       <c r="N110" s="108"/>
       <c r="Q110" s="3" t="s">
-        <v>195</v>
+        <v>243</v>
       </c>
     </row>
     <row r="111" spans="1:19" customHeight="1" ht="14.25">
@@ -9065,7 +9305,7 @@
       <c r="M111" s="108"/>
       <c r="N111" s="108"/>
       <c r="Q111" s="3" t="s">
-        <v>196</v>
+        <v>244</v>
       </c>
     </row>
     <row r="112" spans="1:19" customHeight="1" ht="14.25">
@@ -9084,7 +9324,7 @@
       <c r="M112" s="108"/>
       <c r="N112" s="108"/>
       <c r="Q112" s="3" t="s">
-        <v>197</v>
+        <v>245</v>
       </c>
     </row>
     <row r="113" spans="1:19" customHeight="1" ht="14.25">
@@ -9103,7 +9343,7 @@
       <c r="M113" s="108"/>
       <c r="N113" s="108"/>
       <c r="Q113" s="3" t="s">
-        <v>198</v>
+        <v>246</v>
       </c>
     </row>
     <row r="114" spans="1:19" customHeight="1" ht="14.25">
@@ -9122,7 +9362,7 @@
       <c r="M114" s="108"/>
       <c r="N114" s="108"/>
       <c r="Q114" s="3" t="s">
-        <v>199</v>
+        <v>247</v>
       </c>
     </row>
     <row r="115" spans="1:19" customHeight="1" ht="14.25">
@@ -9141,7 +9381,7 @@
       <c r="M115" s="108"/>
       <c r="N115" s="108"/>
       <c r="Q115" s="3" t="s">
-        <v>200</v>
+        <v>248</v>
       </c>
     </row>
     <row r="116" spans="1:19" customHeight="1" ht="14.25">
@@ -9160,7 +9400,7 @@
       <c r="M116" s="108"/>
       <c r="N116" s="108"/>
       <c r="Q116" s="3" t="s">
-        <v>201</v>
+        <v>249</v>
       </c>
     </row>
     <row r="117" spans="1:19" customHeight="1" ht="14.25">
@@ -9179,7 +9419,7 @@
       <c r="M117" s="108"/>
       <c r="N117" s="108"/>
       <c r="Q117" s="3" t="s">
-        <v>202</v>
+        <v>250</v>
       </c>
     </row>
     <row r="118" spans="1:19" customHeight="1" ht="14.25">
@@ -9198,7 +9438,7 @@
       <c r="M118" s="108"/>
       <c r="N118" s="108"/>
       <c r="Q118" s="3" t="s">
-        <v>203</v>
+        <v>251</v>
       </c>
     </row>
     <row r="119" spans="1:19" customHeight="1" ht="14.25">
@@ -9217,7 +9457,7 @@
       <c r="M119" s="108"/>
       <c r="N119" s="108"/>
       <c r="Q119" s="3" t="s">
-        <v>204</v>
+        <v>252</v>
       </c>
     </row>
     <row r="120" spans="1:19" customHeight="1" ht="14.25">
@@ -9236,7 +9476,7 @@
       <c r="M120" s="108"/>
       <c r="N120" s="108"/>
       <c r="Q120" s="3" t="s">
-        <v>205</v>
+        <v>253</v>
       </c>
     </row>
     <row r="121" spans="1:19" customHeight="1" ht="14.25">
@@ -9255,7 +9495,7 @@
       <c r="M121" s="108"/>
       <c r="N121" s="108"/>
       <c r="Q121" s="3" t="s">
-        <v>206</v>
+        <v>254</v>
       </c>
     </row>
     <row r="122" spans="1:19" customHeight="1" ht="14.25">
@@ -9274,7 +9514,7 @@
       <c r="M122" s="108"/>
       <c r="N122" s="108"/>
       <c r="Q122" s="3" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
     </row>
     <row r="123" spans="1:19" customHeight="1" ht="14.25">
@@ -9293,7 +9533,7 @@
       <c r="M123" s="108"/>
       <c r="N123" s="108"/>
       <c r="Q123" s="3" t="s">
-        <v>208</v>
+        <v>256</v>
       </c>
     </row>
     <row r="124" spans="1:19" customHeight="1" ht="14.25">
@@ -9312,7 +9552,7 @@
       <c r="M124" s="108"/>
       <c r="N124" s="108"/>
       <c r="Q124" s="3" t="s">
-        <v>209</v>
+        <v>257</v>
       </c>
     </row>
     <row r="125" spans="1:19" customHeight="1" ht="14.25">
@@ -9331,7 +9571,7 @@
       <c r="M125" s="108"/>
       <c r="N125" s="108"/>
       <c r="Q125" s="3" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
     </row>
     <row r="126" spans="1:19" customHeight="1" ht="14.25">
@@ -9350,7 +9590,7 @@
       <c r="M126" s="108"/>
       <c r="N126" s="108"/>
       <c r="Q126" s="3" t="s">
-        <v>211</v>
+        <v>259</v>
       </c>
     </row>
     <row r="127" spans="1:19" customHeight="1" ht="14.25">
@@ -9369,7 +9609,7 @@
       <c r="M127" s="108"/>
       <c r="N127" s="108"/>
       <c r="Q127" s="3" t="s">
-        <v>212</v>
+        <v>260</v>
       </c>
     </row>
     <row r="128" spans="1:19" customHeight="1" ht="28.5">
@@ -9388,7 +9628,7 @@
       <c r="M128" s="108"/>
       <c r="N128" s="108"/>
       <c r="Q128" s="3" t="s">
-        <v>213</v>
+        <v>261</v>
       </c>
     </row>
     <row r="129" spans="1:19" customHeight="1" ht="14.25">
@@ -9407,7 +9647,7 @@
       <c r="M129" s="108"/>
       <c r="N129" s="108"/>
       <c r="Q129" s="3" t="s">
-        <v>214</v>
+        <v>262</v>
       </c>
     </row>
     <row r="130" spans="1:19" customHeight="1" ht="14.25">
@@ -9426,7 +9666,7 @@
       <c r="M130" s="108"/>
       <c r="N130" s="108"/>
       <c r="Q130" s="3" t="s">
-        <v>215</v>
+        <v>263</v>
       </c>
     </row>
     <row r="131" spans="1:19" customHeight="1" ht="14.25">
@@ -9445,7 +9685,7 @@
       <c r="M131" s="108"/>
       <c r="N131" s="108"/>
       <c r="Q131" s="3" t="s">
-        <v>216</v>
+        <v>264</v>
       </c>
     </row>
     <row r="132" spans="1:19" customHeight="1" ht="14.25">
@@ -9464,7 +9704,7 @@
       <c r="M132" s="108"/>
       <c r="N132" s="108"/>
       <c r="Q132" s="3" t="s">
-        <v>217</v>
+        <v>265</v>
       </c>
     </row>
     <row r="133" spans="1:19" customHeight="1" ht="14.25">
@@ -9483,7 +9723,7 @@
       <c r="M133" s="108"/>
       <c r="N133" s="108"/>
       <c r="Q133" s="3" t="s">
-        <v>218</v>
+        <v>266</v>
       </c>
     </row>
     <row r="134" spans="1:19" customHeight="1" ht="14.25">
@@ -9502,7 +9742,7 @@
       <c r="M134" s="108"/>
       <c r="N134" s="108"/>
       <c r="Q134" s="3" t="s">
-        <v>219</v>
+        <v>267</v>
       </c>
     </row>
     <row r="135" spans="1:19" customHeight="1" ht="14.25">
@@ -9521,7 +9761,7 @@
       <c r="M135" s="108"/>
       <c r="N135" s="108"/>
       <c r="Q135" s="3" t="s">
-        <v>220</v>
+        <v>268</v>
       </c>
     </row>
     <row r="136" spans="1:19" customHeight="1" ht="14.25">
@@ -9540,7 +9780,7 @@
       <c r="M136" s="108"/>
       <c r="N136" s="108"/>
       <c r="Q136" s="3" t="s">
-        <v>221</v>
+        <v>269</v>
       </c>
     </row>
     <row r="137" spans="1:19" customHeight="1" ht="14.25">
@@ -9559,7 +9799,7 @@
       <c r="M137" s="108"/>
       <c r="N137" s="108"/>
       <c r="Q137" s="3" t="s">
-        <v>222</v>
+        <v>270</v>
       </c>
     </row>
     <row r="138" spans="1:19" customHeight="1" ht="14.25">
@@ -9578,7 +9818,7 @@
       <c r="M138" s="108"/>
       <c r="N138" s="108"/>
       <c r="Q138" s="3" t="s">
-        <v>223</v>
+        <v>271</v>
       </c>
     </row>
     <row r="139" spans="1:19" customHeight="1" ht="14.25">
@@ -9597,7 +9837,7 @@
       <c r="M139" s="108"/>
       <c r="N139" s="108"/>
       <c r="Q139" s="3" t="s">
-        <v>224</v>
+        <v>272</v>
       </c>
     </row>
     <row r="140" spans="1:19" customHeight="1" ht="14.25">
@@ -9616,7 +9856,7 @@
       <c r="M140" s="108"/>
       <c r="N140" s="108"/>
       <c r="Q140" s="3" t="s">
-        <v>225</v>
+        <v>273</v>
       </c>
     </row>
     <row r="141" spans="1:19" customHeight="1" ht="14.25">
@@ -9635,7 +9875,7 @@
       <c r="M141" s="108"/>
       <c r="N141" s="108"/>
       <c r="Q141" s="3" t="s">
-        <v>226</v>
+        <v>274</v>
       </c>
     </row>
     <row r="142" spans="1:19" customHeight="1" ht="14.25">
@@ -9654,7 +9894,7 @@
       <c r="M142" s="108"/>
       <c r="N142" s="108"/>
       <c r="Q142" s="3" t="s">
-        <v>227</v>
+        <v>275</v>
       </c>
     </row>
     <row r="143" spans="1:19" customHeight="1" ht="28.5">
@@ -9673,7 +9913,7 @@
       <c r="M143" s="108"/>
       <c r="N143" s="108"/>
       <c r="Q143" s="3" t="s">
-        <v>228</v>
+        <v>276</v>
       </c>
     </row>
     <row r="144" spans="1:19" customHeight="1" ht="14.25">
@@ -9692,7 +9932,7 @@
       <c r="M144" s="108"/>
       <c r="N144" s="108"/>
       <c r="Q144" s="3" t="s">
-        <v>229</v>
+        <v>277</v>
       </c>
     </row>
     <row r="145" spans="1:19" customHeight="1" ht="14.25">
@@ -9711,7 +9951,7 @@
       <c r="M145" s="108"/>
       <c r="N145" s="108"/>
       <c r="Q145" s="3" t="s">
-        <v>230</v>
+        <v>278</v>
       </c>
     </row>
     <row r="146" spans="1:19" customHeight="1" ht="14.25">
@@ -9730,7 +9970,7 @@
       <c r="M146" s="108"/>
       <c r="N146" s="108"/>
       <c r="Q146" s="3" t="s">
-        <v>231</v>
+        <v>279</v>
       </c>
     </row>
     <row r="147" spans="1:19" customHeight="1" ht="14.25">
@@ -9749,7 +9989,7 @@
       <c r="M147" s="108"/>
       <c r="N147" s="108"/>
       <c r="Q147" s="3" t="s">
-        <v>232</v>
+        <v>280</v>
       </c>
     </row>
     <row r="148" spans="1:19" customHeight="1" ht="14.25">
@@ -9768,7 +10008,7 @@
       <c r="M148" s="108"/>
       <c r="N148" s="108"/>
       <c r="Q148" s="3" t="s">
-        <v>233</v>
+        <v>281</v>
       </c>
     </row>
     <row r="149" spans="1:19" customHeight="1" ht="14.25">
@@ -9787,7 +10027,7 @@
       <c r="M149" s="108"/>
       <c r="N149" s="108"/>
       <c r="Q149" s="3" t="s">
-        <v>234</v>
+        <v>282</v>
       </c>
     </row>
     <row r="150" spans="1:19" customHeight="1" ht="14.25">
@@ -9806,7 +10046,7 @@
       <c r="M150" s="108"/>
       <c r="N150" s="108"/>
       <c r="Q150" s="3" t="s">
-        <v>235</v>
+        <v>283</v>
       </c>
     </row>
     <row r="151" spans="1:19" customHeight="1" ht="14.25">
@@ -9825,7 +10065,7 @@
       <c r="M151" s="108"/>
       <c r="N151" s="108"/>
       <c r="Q151" s="3" t="s">
-        <v>236</v>
+        <v>284</v>
       </c>
     </row>
     <row r="152" spans="1:19" customHeight="1" ht="14.25">
@@ -9844,7 +10084,7 @@
       <c r="M152" s="108"/>
       <c r="N152" s="108"/>
       <c r="Q152" s="3" t="s">
-        <v>237</v>
+        <v>285</v>
       </c>
     </row>
     <row r="153" spans="1:19" customHeight="1" ht="28.5">
@@ -9863,7 +10103,7 @@
       <c r="M153" s="108"/>
       <c r="N153" s="108"/>
       <c r="Q153" s="3" t="s">
-        <v>238</v>
+        <v>286</v>
       </c>
     </row>
     <row r="154" spans="1:19" customHeight="1" ht="14.25">
@@ -9882,7 +10122,7 @@
       <c r="M154" s="108"/>
       <c r="N154" s="108"/>
       <c r="Q154" s="3" t="s">
-        <v>239</v>
+        <v>287</v>
       </c>
     </row>
     <row r="155" spans="1:19" customHeight="1" ht="28.5">
@@ -9901,7 +10141,7 @@
       <c r="M155" s="108"/>
       <c r="N155" s="108"/>
       <c r="Q155" s="3" t="s">
-        <v>240</v>
+        <v>288</v>
       </c>
     </row>
     <row r="156" spans="1:19" customHeight="1" ht="14.25">
@@ -9920,7 +10160,7 @@
       <c r="M156" s="108"/>
       <c r="N156" s="108"/>
       <c r="Q156" s="3" t="s">
-        <v>241</v>
+        <v>289</v>
       </c>
     </row>
     <row r="157" spans="1:19" customHeight="1" ht="14.25">
@@ -9939,7 +10179,7 @@
       <c r="M157" s="108"/>
       <c r="N157" s="108"/>
       <c r="Q157" s="3" t="s">
-        <v>242</v>
+        <v>290</v>
       </c>
     </row>
     <row r="158" spans="1:19" customHeight="1" ht="14.25">
@@ -9958,7 +10198,7 @@
       <c r="M158" s="108"/>
       <c r="N158" s="108"/>
       <c r="Q158" s="3" t="s">
-        <v>243</v>
+        <v>291</v>
       </c>
     </row>
     <row r="159" spans="1:19" customHeight="1" ht="14.25">
@@ -9977,7 +10217,7 @@
       <c r="M159" s="108"/>
       <c r="N159" s="108"/>
       <c r="Q159" s="3" t="s">
-        <v>244</v>
+        <v>292</v>
       </c>
     </row>
     <row r="160" spans="1:19" customHeight="1" ht="14.25">
@@ -9996,7 +10236,7 @@
       <c r="M160" s="108"/>
       <c r="N160" s="108"/>
       <c r="Q160" s="3" t="s">
-        <v>245</v>
+        <v>293</v>
       </c>
     </row>
     <row r="161" spans="1:19" customHeight="1" ht="14.25">
@@ -10015,7 +10255,7 @@
       <c r="M161" s="108"/>
       <c r="N161" s="108"/>
       <c r="Q161" s="3" t="s">
-        <v>246</v>
+        <v>294</v>
       </c>
     </row>
     <row r="162" spans="1:19" customHeight="1" ht="14.25">
@@ -10034,7 +10274,7 @@
       <c r="M162" s="108"/>
       <c r="N162" s="108"/>
       <c r="Q162" s="3" t="s">
-        <v>247</v>
+        <v>295</v>
       </c>
     </row>
     <row r="163" spans="1:19" customHeight="1" ht="14.25">
@@ -10053,7 +10293,7 @@
       <c r="M163" s="108"/>
       <c r="N163" s="108"/>
       <c r="Q163" s="3" t="s">
-        <v>248</v>
+        <v>296</v>
       </c>
     </row>
     <row r="164" spans="1:19" customHeight="1" ht="14.25">
@@ -10072,7 +10312,7 @@
       <c r="M164" s="108"/>
       <c r="N164" s="108"/>
       <c r="Q164" s="3" t="s">
-        <v>249</v>
+        <v>297</v>
       </c>
     </row>
     <row r="165" spans="1:19" customHeight="1" ht="28.5">
@@ -10091,7 +10331,7 @@
       <c r="M165" s="108"/>
       <c r="N165" s="108"/>
       <c r="Q165" s="3" t="s">
-        <v>250</v>
+        <v>298</v>
       </c>
     </row>
     <row r="166" spans="1:19" customHeight="1" ht="14.25">
@@ -10110,7 +10350,7 @@
       <c r="M166" s="108"/>
       <c r="N166" s="108"/>
       <c r="Q166" s="3" t="s">
-        <v>251</v>
+        <v>299</v>
       </c>
     </row>
     <row r="167" spans="1:19" customHeight="1" ht="42.75">
@@ -10129,7 +10369,7 @@
       <c r="M167" s="108"/>
       <c r="N167" s="108"/>
       <c r="Q167" s="3" t="s">
-        <v>252</v>
+        <v>300</v>
       </c>
     </row>
     <row r="168" spans="1:19" customHeight="1" ht="14.25">
@@ -10148,7 +10388,7 @@
       <c r="M168" s="108"/>
       <c r="N168" s="108"/>
       <c r="Q168" s="3" t="s">
-        <v>253</v>
+        <v>301</v>
       </c>
     </row>
     <row r="169" spans="1:19" customHeight="1" ht="14.25">
@@ -10167,7 +10407,7 @@
       <c r="M169" s="108"/>
       <c r="N169" s="108"/>
       <c r="Q169" s="3" t="s">
-        <v>254</v>
+        <v>302</v>
       </c>
     </row>
     <row r="170" spans="1:19" customHeight="1" ht="28.5">
@@ -10186,7 +10426,7 @@
       <c r="M170" s="108"/>
       <c r="N170" s="108"/>
       <c r="Q170" s="3" t="s">
-        <v>255</v>
+        <v>303</v>
       </c>
     </row>
     <row r="171" spans="1:19" customHeight="1" ht="14.25">
@@ -10205,7 +10445,7 @@
       <c r="M171" s="108"/>
       <c r="N171" s="108"/>
       <c r="Q171" s="3" t="s">
-        <v>256</v>
+        <v>304</v>
       </c>
     </row>
     <row r="172" spans="1:19" customHeight="1" ht="14.25">
@@ -10224,7 +10464,7 @@
       <c r="M172" s="108"/>
       <c r="N172" s="108"/>
       <c r="Q172" s="3" t="s">
-        <v>257</v>
+        <v>305</v>
       </c>
     </row>
     <row r="173" spans="1:19" customHeight="1" ht="14.25">
@@ -10243,7 +10483,7 @@
       <c r="M173" s="108"/>
       <c r="N173" s="108"/>
       <c r="Q173" s="3" t="s">
-        <v>258</v>
+        <v>306</v>
       </c>
     </row>
     <row r="174" spans="1:19" customHeight="1" ht="14.25">
@@ -10262,7 +10502,7 @@
       <c r="M174" s="108"/>
       <c r="N174" s="108"/>
       <c r="Q174" s="3" t="s">
-        <v>259</v>
+        <v>307</v>
       </c>
     </row>
     <row r="175" spans="1:19" customHeight="1" ht="14.25">
@@ -10281,7 +10521,7 @@
       <c r="M175" s="108"/>
       <c r="N175" s="108"/>
       <c r="Q175" s="3" t="s">
-        <v>260</v>
+        <v>308</v>
       </c>
     </row>
     <row r="176" spans="1:19" customHeight="1" ht="14.25">
@@ -10300,7 +10540,7 @@
       <c r="M176" s="108"/>
       <c r="N176" s="108"/>
       <c r="Q176" s="3" t="s">
-        <v>261</v>
+        <v>309</v>
       </c>
     </row>
     <row r="177" spans="1:19" customHeight="1" ht="14.25">
@@ -10319,7 +10559,7 @@
       <c r="M177" s="108"/>
       <c r="N177" s="108"/>
       <c r="Q177" s="3" t="s">
-        <v>262</v>
+        <v>310</v>
       </c>
     </row>
     <row r="178" spans="1:19" customHeight="1" ht="14.25">
@@ -10338,7 +10578,7 @@
       <c r="M178" s="108"/>
       <c r="N178" s="108"/>
       <c r="Q178" s="3" t="s">
-        <v>263</v>
+        <v>311</v>
       </c>
     </row>
     <row r="179" spans="1:19" customHeight="1" ht="14.25">
@@ -10357,7 +10597,7 @@
       <c r="M179" s="108"/>
       <c r="N179" s="108"/>
       <c r="Q179" s="3" t="s">
-        <v>264</v>
+        <v>312</v>
       </c>
     </row>
     <row r="180" spans="1:19" customHeight="1" ht="28.5">
@@ -10376,7 +10616,7 @@
       <c r="M180" s="108"/>
       <c r="N180" s="108"/>
       <c r="Q180" s="3" t="s">
-        <v>265</v>
+        <v>313</v>
       </c>
     </row>
     <row r="181" spans="1:19" customHeight="1" ht="14.25">
@@ -10395,7 +10635,7 @@
       <c r="M181" s="108"/>
       <c r="N181" s="108"/>
       <c r="Q181" s="3" t="s">
-        <v>266</v>
+        <v>314</v>
       </c>
     </row>
     <row r="182" spans="1:19" customHeight="1" ht="14.25">
@@ -10414,7 +10654,7 @@
       <c r="M182" s="108"/>
       <c r="N182" s="108"/>
       <c r="Q182" s="3" t="s">
-        <v>267</v>
+        <v>315</v>
       </c>
     </row>
     <row r="183" spans="1:19" customHeight="1" ht="14.25">
@@ -10433,7 +10673,7 @@
       <c r="M183" s="108"/>
       <c r="N183" s="108"/>
       <c r="Q183" s="3" t="s">
-        <v>268</v>
+        <v>316</v>
       </c>
     </row>
     <row r="184" spans="1:19" customHeight="1" ht="14.25">
@@ -10452,7 +10692,7 @@
       <c r="M184" s="108"/>
       <c r="N184" s="108"/>
       <c r="Q184" s="3" t="s">
-        <v>269</v>
+        <v>317</v>
       </c>
     </row>
     <row r="185" spans="1:19" customHeight="1" ht="14.25">
@@ -10471,7 +10711,7 @@
       <c r="M185" s="108"/>
       <c r="N185" s="108"/>
       <c r="Q185" s="3" t="s">
-        <v>270</v>
+        <v>318</v>
       </c>
     </row>
     <row r="186" spans="1:19" customHeight="1" ht="14.25">
@@ -10490,7 +10730,7 @@
       <c r="M186" s="108"/>
       <c r="N186" s="108"/>
       <c r="Q186" s="3" t="s">
-        <v>271</v>
+        <v>319</v>
       </c>
     </row>
     <row r="187" spans="1:19" customHeight="1" ht="14.25">
@@ -10509,7 +10749,7 @@
       <c r="M187" s="108"/>
       <c r="N187" s="108"/>
       <c r="Q187" s="3" t="s">
-        <v>272</v>
+        <v>320</v>
       </c>
     </row>
     <row r="188" spans="1:19" customHeight="1" ht="14.25">
@@ -10528,7 +10768,7 @@
       <c r="M188" s="108"/>
       <c r="N188" s="108"/>
       <c r="Q188" s="3" t="s">
-        <v>273</v>
+        <v>321</v>
       </c>
     </row>
     <row r="189" spans="1:19" customHeight="1" ht="14.25">
@@ -10547,7 +10787,7 @@
       <c r="M189" s="108"/>
       <c r="N189" s="108"/>
       <c r="Q189" s="3" t="s">
-        <v>274</v>
+        <v>322</v>
       </c>
     </row>
     <row r="190" spans="1:19" customHeight="1" ht="14.25">
@@ -10566,7 +10806,7 @@
       <c r="M190" s="108"/>
       <c r="N190" s="108"/>
       <c r="Q190" s="3" t="s">
-        <v>275</v>
+        <v>323</v>
       </c>
     </row>
     <row r="191" spans="1:19" customHeight="1" ht="14.25">
@@ -10585,7 +10825,7 @@
       <c r="M191" s="108"/>
       <c r="N191" s="108"/>
       <c r="Q191" s="3" t="s">
-        <v>276</v>
+        <v>324</v>
       </c>
     </row>
     <row r="192" spans="1:19" customHeight="1" ht="14.25">
@@ -10604,7 +10844,7 @@
       <c r="M192" s="108"/>
       <c r="N192" s="108"/>
       <c r="Q192" s="3" t="s">
-        <v>277</v>
+        <v>325</v>
       </c>
     </row>
     <row r="193" spans="1:19" customHeight="1" ht="14.25">
@@ -10623,7 +10863,7 @@
       <c r="M193" s="108"/>
       <c r="N193" s="108"/>
       <c r="Q193" s="3" t="s">
-        <v>278</v>
+        <v>326</v>
       </c>
     </row>
     <row r="194" spans="1:19" customHeight="1" ht="14.25">
@@ -10642,7 +10882,7 @@
       <c r="M194" s="108"/>
       <c r="N194" s="108"/>
       <c r="Q194" s="3" t="s">
-        <v>279</v>
+        <v>327</v>
       </c>
     </row>
     <row r="195" spans="1:19" customHeight="1" ht="14.25">
@@ -10661,7 +10901,7 @@
       <c r="M195" s="108"/>
       <c r="N195" s="108"/>
       <c r="Q195" s="3" t="s">
-        <v>280</v>
+        <v>328</v>
       </c>
     </row>
     <row r="196" spans="1:19" customHeight="1" ht="14.25">
@@ -10680,7 +10920,7 @@
       <c r="M196" s="108"/>
       <c r="N196" s="108"/>
       <c r="Q196" s="3" t="s">
-        <v>281</v>
+        <v>329</v>
       </c>
     </row>
     <row r="197" spans="1:19" customHeight="1" ht="14.25">
@@ -10699,7 +10939,7 @@
       <c r="M197" s="108"/>
       <c r="N197" s="108"/>
       <c r="Q197" s="3" t="s">
-        <v>282</v>
+        <v>330</v>
       </c>
     </row>
     <row r="198" spans="1:19" customHeight="1" ht="14.25">
@@ -10718,7 +10958,7 @@
       <c r="M198" s="108"/>
       <c r="N198" s="108"/>
       <c r="Q198" s="3" t="s">
-        <v>283</v>
+        <v>331</v>
       </c>
     </row>
     <row r="199" spans="1:19" customHeight="1" ht="14.25">
@@ -10737,7 +10977,7 @@
       <c r="M199" s="108"/>
       <c r="N199" s="108"/>
       <c r="Q199" s="3" t="s">
-        <v>284</v>
+        <v>332</v>
       </c>
     </row>
     <row r="200" spans="1:19" customHeight="1" ht="28.5">
@@ -10756,7 +10996,7 @@
       <c r="M200" s="108"/>
       <c r="N200" s="108"/>
       <c r="Q200" s="3" t="s">
-        <v>285</v>
+        <v>333</v>
       </c>
     </row>
     <row r="201" spans="1:19" customHeight="1" ht="14.25">
@@ -10775,7 +11015,7 @@
       <c r="M201" s="108"/>
       <c r="N201" s="108"/>
       <c r="Q201" s="3" t="s">
-        <v>286</v>
+        <v>334</v>
       </c>
     </row>
     <row r="202" spans="1:19" customHeight="1" ht="14.25">
@@ -10794,7 +11034,7 @@
       <c r="M202" s="108"/>
       <c r="N202" s="108"/>
       <c r="Q202" s="3" t="s">
-        <v>287</v>
+        <v>335</v>
       </c>
     </row>
     <row r="203" spans="1:19" customHeight="1" ht="14.25">
@@ -10813,7 +11053,7 @@
       <c r="M203" s="108"/>
       <c r="N203" s="108"/>
       <c r="Q203" s="3" t="s">
-        <v>288</v>
+        <v>336</v>
       </c>
     </row>
     <row r="204" spans="1:19" customHeight="1" ht="14.25">
@@ -10832,7 +11072,7 @@
       <c r="M204" s="108"/>
       <c r="N204" s="108"/>
       <c r="Q204" s="3" t="s">
-        <v>289</v>
+        <v>337</v>
       </c>
     </row>
     <row r="205" spans="1:19" customHeight="1" ht="14.25">
@@ -10851,7 +11091,7 @@
       <c r="M205" s="108"/>
       <c r="N205" s="108"/>
       <c r="Q205" s="3" t="s">
-        <v>290</v>
+        <v>338</v>
       </c>
     </row>
     <row r="206" spans="1:19" customHeight="1" ht="14.25">
@@ -10870,7 +11110,7 @@
       <c r="M206" s="108"/>
       <c r="N206" s="108"/>
       <c r="Q206" s="3" t="s">
-        <v>291</v>
+        <v>339</v>
       </c>
     </row>
     <row r="207" spans="1:19" customHeight="1" ht="28.5">
@@ -10889,7 +11129,7 @@
       <c r="M207" s="108"/>
       <c r="N207" s="108"/>
       <c r="Q207" s="3" t="s">
-        <v>292</v>
+        <v>340</v>
       </c>
     </row>
     <row r="208" spans="1:19" customHeight="1" ht="28.5">
@@ -10908,7 +11148,7 @@
       <c r="M208" s="108"/>
       <c r="N208" s="108"/>
       <c r="Q208" s="3" t="s">
-        <v>293</v>
+        <v>341</v>
       </c>
     </row>
     <row r="209" spans="1:19" customHeight="1" ht="14.25">
@@ -10927,7 +11167,7 @@
       <c r="M209" s="108"/>
       <c r="N209" s="108"/>
       <c r="Q209" s="3" t="s">
-        <v>294</v>
+        <v>342</v>
       </c>
     </row>
     <row r="210" spans="1:19" customHeight="1" ht="14.25">
@@ -10946,7 +11186,7 @@
       <c r="M210" s="108"/>
       <c r="N210" s="108"/>
       <c r="Q210" s="3" t="s">
-        <v>295</v>
+        <v>343</v>
       </c>
     </row>
     <row r="211" spans="1:19" customHeight="1" ht="14.25">
@@ -10965,7 +11205,7 @@
       <c r="M211" s="108"/>
       <c r="N211" s="108"/>
       <c r="Q211" s="3" t="s">
-        <v>296</v>
+        <v>344</v>
       </c>
     </row>
     <row r="212" spans="1:19" customHeight="1" ht="14.25">
@@ -10984,7 +11224,7 @@
       <c r="M212" s="108"/>
       <c r="N212" s="108"/>
       <c r="Q212" s="3" t="s">
-        <v>297</v>
+        <v>345</v>
       </c>
     </row>
     <row r="213" spans="1:19" customHeight="1" ht="14.25">
@@ -11003,7 +11243,7 @@
       <c r="M213" s="108"/>
       <c r="N213" s="108"/>
       <c r="Q213" s="3" t="s">
-        <v>298</v>
+        <v>346</v>
       </c>
     </row>
     <row r="214" spans="1:19" customHeight="1" ht="14.25">
@@ -11022,7 +11262,7 @@
       <c r="M214" s="108"/>
       <c r="N214" s="108"/>
       <c r="Q214" s="3" t="s">
-        <v>299</v>
+        <v>347</v>
       </c>
     </row>
     <row r="215" spans="1:19" customHeight="1" ht="14.25">
@@ -11041,7 +11281,7 @@
       <c r="M215" s="108"/>
       <c r="N215" s="108"/>
       <c r="Q215" s="3" t="s">
-        <v>300</v>
+        <v>348</v>
       </c>
     </row>
     <row r="216" spans="1:19" customHeight="1" ht="14.25">
@@ -11060,7 +11300,7 @@
       <c r="M216" s="108"/>
       <c r="N216" s="108"/>
       <c r="Q216" s="3" t="s">
-        <v>301</v>
+        <v>349</v>
       </c>
     </row>
     <row r="217" spans="1:19">
@@ -12242,7 +12482,7 @@
     </row>
     <row r="2" spans="1:14" customHeight="1" ht="18">
       <c r="A2" s="514" t="s">
-        <v>302</v>
+        <v>350</v>
       </c>
       <c r="B2" s="515"/>
       <c r="C2" s="515"/>
@@ -12259,28 +12499,28 @@
     </row>
     <row r="3" spans="1:14" customHeight="1" ht="15">
       <c r="A3" s="140" t="s">
-        <v>303</v>
+        <v>351</v>
       </c>
       <c r="B3" s="507" t="s">
-        <v>304</v>
+        <v>352</v>
       </c>
       <c r="C3" s="507"/>
       <c r="D3" s="507"/>
       <c r="E3" s="508"/>
       <c r="F3" s="512" t="s">
-        <v>305</v>
+        <v>353</v>
       </c>
       <c r="G3" s="509" t="s">
-        <v>306</v>
+        <v>354</v>
       </c>
       <c r="H3" s="508"/>
       <c r="I3" s="509" t="s">
-        <v>307</v>
+        <v>355</v>
       </c>
       <c r="J3" s="507"/>
       <c r="K3" s="508"/>
       <c r="L3" s="510" t="s">
-        <v>308</v>
+        <v>356</v>
       </c>
       <c r="M3" s="511"/>
     </row>
@@ -12297,10 +12537,10 @@
       <c r="J4" s="483"/>
       <c r="K4" s="484"/>
       <c r="L4" s="5" t="s">
-        <v>309</v>
+        <v>357</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>310</v>
+        <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:14" customHeight="1" ht="27">
@@ -12410,7 +12650,7 @@
     </row>
     <row r="12" spans="1:14" customHeight="1" ht="12">
       <c r="A12" s="485" t="s">
-        <v>113</v>
+        <v>161</v>
       </c>
       <c r="B12" s="486"/>
       <c r="C12" s="486"/>
@@ -12427,7 +12667,7 @@
     </row>
     <row r="13" spans="1:14" customHeight="1" ht="18">
       <c r="A13" s="488" t="s">
-        <v>311</v>
+        <v>359</v>
       </c>
       <c r="B13" s="489"/>
       <c r="C13" s="489"/>
@@ -12444,7 +12684,7 @@
     </row>
     <row r="14" spans="1:14" customHeight="1" ht="12">
       <c r="A14" s="202" t="s">
-        <v>312</v>
+        <v>360</v>
       </c>
       <c r="B14" s="101"/>
       <c r="C14" s="101"/>
@@ -12461,33 +12701,33 @@
     </row>
     <row r="15" spans="1:14" customHeight="1" ht="18">
       <c r="A15" s="4" t="s">
-        <v>313</v>
+        <v>361</v>
       </c>
       <c r="B15" s="481" t="s">
-        <v>314</v>
+        <v>362</v>
       </c>
       <c r="C15" s="482"/>
       <c r="D15" s="494" t="s">
-        <v>315</v>
+        <v>363</v>
       </c>
       <c r="E15" s="481"/>
       <c r="F15" s="482"/>
       <c r="G15" s="494" t="s">
-        <v>316</v>
+        <v>364</v>
       </c>
       <c r="H15" s="481"/>
       <c r="I15" s="482"/>
       <c r="J15" s="498" t="s">
-        <v>317</v>
+        <v>365</v>
       </c>
       <c r="K15" s="519" t="s">
-        <v>318</v>
+        <v>366</v>
       </c>
       <c r="L15" s="473" t="s">
-        <v>319</v>
+        <v>367</v>
       </c>
       <c r="M15" s="517" t="s">
-        <v>320</v>
+        <v>368</v>
       </c>
     </row>
     <row r="16" spans="1:14" customHeight="1" ht="15">
@@ -12507,11 +12747,11 @@
     </row>
     <row r="17" spans="1:14" customHeight="1" ht="18.75">
       <c r="A17" s="521" t="s">
-        <v>128</v>
+        <v>176</v>
       </c>
       <c r="B17" s="522"/>
       <c r="C17" s="8" t="s">
-        <v>129</v>
+        <v>177</v>
       </c>
       <c r="D17" s="495"/>
       <c r="E17" s="483"/>
@@ -12946,7 +13186,7 @@
     </row>
     <row r="46" spans="1:14" customHeight="1" ht="9.75">
       <c r="A46" s="476" t="s">
-        <v>113</v>
+        <v>161</v>
       </c>
       <c r="B46" s="477"/>
       <c r="C46" s="477"/>
@@ -12963,7 +13203,7 @@
     </row>
     <row r="47" spans="1:14" customHeight="1" ht="27.75">
       <c r="A47" s="445" t="s">
-        <v>142</v>
+        <v>190</v>
       </c>
       <c r="B47" s="446"/>
       <c r="C47" s="447"/>
@@ -12973,7 +13213,7 @@
       <c r="G47" s="502"/>
       <c r="H47" s="503"/>
       <c r="I47" s="228" t="s">
-        <v>143</v>
+        <v>191</v>
       </c>
       <c r="J47" s="229"/>
       <c r="K47" s="230"/>
@@ -12983,7 +13223,7 @@
     </row>
     <row r="48" spans="1:14" customHeight="1" ht="9">
       <c r="A48" s="500" t="s">
-        <v>321</v>
+        <v>369</v>
       </c>
       <c r="B48" s="500"/>
       <c r="C48" s="500"/>
@@ -13187,7 +13427,7 @@
     </row>
     <row r="2" spans="1:13" customHeight="1" ht="22.5">
       <c r="A2" s="571" t="s">
-        <v>322</v>
+        <v>370</v>
       </c>
       <c r="B2" s="572"/>
       <c r="C2" s="572"/>
@@ -13202,22 +13442,22 @@
     </row>
     <row r="3" spans="1:13" customHeight="1" ht="15">
       <c r="A3" s="555" t="s">
-        <v>323</v>
+        <v>371</v>
       </c>
       <c r="B3" s="556" t="s">
-        <v>324</v>
+        <v>372</v>
       </c>
       <c r="C3" s="556"/>
       <c r="D3" s="557"/>
       <c r="E3" s="507" t="s">
-        <v>325</v>
+        <v>373</v>
       </c>
       <c r="F3" s="508"/>
       <c r="G3" s="576" t="s">
-        <v>326</v>
+        <v>374</v>
       </c>
       <c r="H3" s="509" t="s">
-        <v>327</v>
+        <v>375</v>
       </c>
       <c r="I3" s="566"/>
       <c r="J3" s="566"/>
@@ -13242,10 +13482,10 @@
       <c r="C5" s="574"/>
       <c r="D5" s="575"/>
       <c r="E5" s="27" t="s">
-        <v>128</v>
+        <v>176</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>129</v>
+        <v>177</v>
       </c>
       <c r="G5" s="520"/>
       <c r="H5" s="570"/>
@@ -13346,7 +13586,7 @@
     </row>
     <row r="13" spans="1:13" customHeight="1" ht="11.25">
       <c r="A13" s="485" t="s">
-        <v>113</v>
+        <v>161</v>
       </c>
       <c r="B13" s="486"/>
       <c r="C13" s="486"/>
@@ -13361,7 +13601,7 @@
     </row>
     <row r="14" spans="1:13" customHeight="1" ht="18">
       <c r="A14" s="528" t="s">
-        <v>328</v>
+        <v>376</v>
       </c>
       <c r="B14" s="529"/>
       <c r="C14" s="529"/>
@@ -13376,25 +13616,25 @@
     </row>
     <row r="15" spans="1:13" customHeight="1" ht="18">
       <c r="A15" s="543" t="s">
-        <v>329</v>
+        <v>377</v>
       </c>
       <c r="B15" s="481" t="s">
-        <v>330</v>
+        <v>378</v>
       </c>
       <c r="C15" s="549"/>
       <c r="D15" s="550"/>
       <c r="E15" s="481" t="s">
-        <v>331</v>
+        <v>379</v>
       </c>
       <c r="F15" s="482"/>
       <c r="G15" s="519" t="s">
-        <v>326</v>
+        <v>374</v>
       </c>
       <c r="H15" s="498" t="s">
-        <v>332</v>
+        <v>380</v>
       </c>
       <c r="I15" s="494" t="s">
-        <v>333</v>
+        <v>381</v>
       </c>
       <c r="J15" s="549"/>
       <c r="K15" s="569"/>
@@ -13418,10 +13658,10 @@
       <c r="C17" s="431"/>
       <c r="D17" s="551"/>
       <c r="E17" s="27" t="s">
-        <v>128</v>
+        <v>176</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>129</v>
+        <v>177</v>
       </c>
       <c r="G17" s="520"/>
       <c r="H17" s="499"/>
@@ -13704,7 +13944,7 @@
     </row>
     <row r="39" spans="1:13" customHeight="1" ht="13.5">
       <c r="A39" s="448" t="s">
-        <v>113</v>
+        <v>161</v>
       </c>
       <c r="B39" s="449"/>
       <c r="C39" s="449"/>
@@ -13719,7 +13959,7 @@
     </row>
     <row r="40" spans="1:13" customHeight="1" ht="22.5">
       <c r="A40" s="585" t="s">
-        <v>334</v>
+        <v>382</v>
       </c>
       <c r="B40" s="586"/>
       <c r="C40" s="586"/>
@@ -13734,26 +13974,26 @@
     </row>
     <row r="41" spans="1:13" customHeight="1" ht="33.75">
       <c r="A41" s="141" t="s">
-        <v>335</v>
+        <v>383</v>
       </c>
       <c r="B41" s="146" t="s">
-        <v>336</v>
+        <v>384</v>
       </c>
       <c r="C41" s="142" t="s">
-        <v>337</v>
+        <v>385</v>
       </c>
       <c r="D41" s="577" t="s">
-        <v>338</v>
+        <v>386</v>
       </c>
       <c r="E41" s="577"/>
       <c r="F41" s="577"/>
       <c r="G41" s="577"/>
       <c r="H41" s="578"/>
       <c r="I41" s="142" t="s">
-        <v>339</v>
+        <v>387</v>
       </c>
       <c r="J41" s="577" t="s">
-        <v>340</v>
+        <v>388</v>
       </c>
       <c r="K41" s="584"/>
     </row>
@@ -13850,7 +14090,7 @@
     </row>
     <row r="49" spans="1:13" customHeight="1" ht="11.25">
       <c r="A49" s="448" t="s">
-        <v>113</v>
+        <v>161</v>
       </c>
       <c r="B49" s="449"/>
       <c r="C49" s="449"/>
@@ -13865,7 +14105,7 @@
     </row>
     <row r="50" spans="1:13" customHeight="1" ht="28.5">
       <c r="A50" s="445" t="s">
-        <v>142</v>
+        <v>190</v>
       </c>
       <c r="B50" s="447"/>
       <c r="C50" s="501"/>
@@ -13873,7 +14113,7 @@
       <c r="E50" s="502"/>
       <c r="F50" s="503"/>
       <c r="G50" s="588" t="s">
-        <v>143</v>
+        <v>191</v>
       </c>
       <c r="H50" s="589"/>
       <c r="I50" s="501"/>
@@ -13884,7 +14124,7 @@
     </row>
     <row r="51" spans="1:13" customHeight="1" ht="9.75">
       <c r="K51" s="236" t="s">
-        <v>341</v>
+        <v>389</v>
       </c>
     </row>
     <row r="52" spans="1:13" customHeight="1" ht="3"/>
@@ -14054,11 +14294,11 @@
     </row>
     <row r="2" spans="1:14" customHeight="1" ht="13.5">
       <c r="A2" s="624" t="s">
-        <v>342</v>
+        <v>390</v>
       </c>
       <c r="B2" s="625"/>
       <c r="C2" s="603" t="s">
-        <v>343</v>
+        <v>391</v>
       </c>
       <c r="D2" s="603"/>
       <c r="E2" s="603"/>
@@ -14075,7 +14315,7 @@
       <c r="A3" s="39"/>
       <c r="B3" s="40"/>
       <c r="C3" s="607" t="s">
-        <v>344</v>
+        <v>392</v>
       </c>
       <c r="D3" s="607"/>
       <c r="E3" s="607"/>
@@ -14092,7 +14332,7 @@
       <c r="A4" s="39"/>
       <c r="B4" s="40"/>
       <c r="C4" s="607" t="s">
-        <v>345</v>
+        <v>393</v>
       </c>
       <c r="D4" s="607"/>
       <c r="E4" s="607"/>
@@ -14118,7 +14358,7 @@
       <c r="A6" s="39"/>
       <c r="B6" s="40"/>
       <c r="C6" s="607" t="s">
-        <v>346</v>
+        <v>394</v>
       </c>
       <c r="D6" s="607"/>
       <c r="E6" s="607"/>
@@ -14150,7 +14390,7 @@
       <c r="A8" s="39"/>
       <c r="B8" s="40"/>
       <c r="C8" s="607" t="s">
-        <v>347</v>
+        <v>395</v>
       </c>
       <c r="D8" s="607"/>
       <c r="E8" s="607"/>
@@ -14180,7 +14420,7 @@
       <c r="E10" s="607"/>
       <c r="F10" s="608"/>
       <c r="G10" s="592" t="s">
-        <v>348</v>
+        <v>396</v>
       </c>
       <c r="H10" s="592"/>
       <c r="I10" s="592"/>
@@ -14221,11 +14461,11 @@
     </row>
     <row r="13" spans="1:14" customHeight="1" ht="18">
       <c r="A13" s="622" t="s">
-        <v>349</v>
+        <v>397</v>
       </c>
       <c r="B13" s="623"/>
       <c r="C13" s="590" t="s">
-        <v>350</v>
+        <v>398</v>
       </c>
       <c r="D13" s="590"/>
       <c r="E13" s="549"/>
@@ -14246,7 +14486,7 @@
       <c r="E14" s="549"/>
       <c r="F14" s="550"/>
       <c r="G14" s="591" t="s">
-        <v>348</v>
+        <v>396</v>
       </c>
       <c r="H14" s="592"/>
       <c r="I14" s="592"/>
@@ -14304,7 +14544,7 @@
       <c r="A18" s="51"/>
       <c r="B18" s="52"/>
       <c r="C18" s="737" t="s">
-        <v>351</v>
+        <v>399</v>
       </c>
       <c r="D18" s="737"/>
       <c r="E18" s="738"/>
@@ -14325,7 +14565,7 @@
       <c r="E19" s="738"/>
       <c r="F19" s="739"/>
       <c r="G19" s="591" t="s">
-        <v>348</v>
+        <v>396</v>
       </c>
       <c r="H19" s="592"/>
       <c r="I19" s="592"/>
@@ -14343,7 +14583,7 @@
       <c r="F20" s="739"/>
       <c r="G20" s="56"/>
       <c r="H20" s="733" t="s">
-        <v>352</v>
+        <v>400</v>
       </c>
       <c r="I20" s="733"/>
       <c r="J20" s="246"/>
@@ -14359,7 +14599,7 @@
       <c r="E21" s="738"/>
       <c r="F21" s="739"/>
       <c r="G21" s="734" t="s">
-        <v>353</v>
+        <v>401</v>
       </c>
       <c r="H21" s="735"/>
       <c r="I21" s="735"/>
@@ -14376,7 +14616,7 @@
       <c r="E22" s="740"/>
       <c r="F22" s="741"/>
       <c r="G22" s="125" t="s">
-        <v>354</v>
+        <v>402</v>
       </c>
       <c r="H22" s="237"/>
       <c r="I22" s="685"/>
@@ -14387,11 +14627,11 @@
     </row>
     <row r="23" spans="1:14" customHeight="1" ht="18">
       <c r="A23" s="636" t="s">
-        <v>355</v>
+        <v>403</v>
       </c>
       <c r="B23" s="637"/>
       <c r="C23" s="618" t="s">
-        <v>356</v>
+        <v>404</v>
       </c>
       <c r="D23" s="618"/>
       <c r="E23" s="618"/>
@@ -14412,7 +14652,7 @@
       <c r="E24" s="610"/>
       <c r="F24" s="609"/>
       <c r="G24" s="591" t="s">
-        <v>348</v>
+        <v>396</v>
       </c>
       <c r="H24" s="592"/>
       <c r="I24" s="592"/>
@@ -14453,11 +14693,11 @@
     </row>
     <row r="27" spans="1:14" customHeight="1" ht="14.25">
       <c r="A27" s="636" t="s">
-        <v>357</v>
+        <v>405</v>
       </c>
       <c r="B27" s="637"/>
       <c r="C27" s="618" t="s">
-        <v>358</v>
+        <v>406</v>
       </c>
       <c r="D27" s="618"/>
       <c r="E27" s="618"/>
@@ -14478,7 +14718,7 @@
       <c r="E28" s="610"/>
       <c r="F28" s="609"/>
       <c r="G28" s="591" t="s">
-        <v>348</v>
+        <v>396</v>
       </c>
       <c r="H28" s="592"/>
       <c r="I28" s="592"/>
@@ -14518,11 +14758,11 @@
     </row>
     <row r="31" spans="1:14" customHeight="1" ht="18">
       <c r="A31" s="636" t="s">
-        <v>359</v>
+        <v>407</v>
       </c>
       <c r="B31" s="637"/>
       <c r="C31" s="618" t="s">
-        <v>360</v>
+        <v>408</v>
       </c>
       <c r="D31" s="618"/>
       <c r="E31" s="618"/>
@@ -14543,7 +14783,7 @@
       <c r="E32" s="610"/>
       <c r="F32" s="609"/>
       <c r="G32" s="672" t="s">
-        <v>361</v>
+        <v>409</v>
       </c>
       <c r="H32" s="673"/>
       <c r="I32" s="673"/>
@@ -14571,7 +14811,7 @@
       <c r="A34" s="49"/>
       <c r="B34" s="50"/>
       <c r="C34" s="610" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="D34" s="610"/>
       <c r="E34" s="610"/>
@@ -14592,7 +14832,7 @@
       <c r="E35" s="610"/>
       <c r="F35" s="609"/>
       <c r="G35" s="672" t="s">
-        <v>361</v>
+        <v>409</v>
       </c>
       <c r="H35" s="673"/>
       <c r="I35" s="673"/>
@@ -14617,11 +14857,11 @@
     </row>
     <row r="37" spans="1:14" customHeight="1" ht="18">
       <c r="A37" s="636" t="s">
-        <v>363</v>
+        <v>411</v>
       </c>
       <c r="B37" s="637"/>
       <c r="C37" s="613" t="s">
-        <v>364</v>
+        <v>412</v>
       </c>
       <c r="D37" s="613"/>
       <c r="E37" s="613"/>
@@ -14642,7 +14882,7 @@
       <c r="E38" s="590"/>
       <c r="F38" s="615"/>
       <c r="G38" s="591" t="s">
-        <v>365</v>
+        <v>413</v>
       </c>
       <c r="H38" s="592"/>
       <c r="I38" s="592"/>
@@ -14683,11 +14923,11 @@
     </row>
     <row r="41" spans="1:14" customHeight="1" ht="28.5">
       <c r="A41" s="611" t="s">
-        <v>366</v>
+        <v>414</v>
       </c>
       <c r="B41" s="612"/>
       <c r="C41" s="610" t="s">
-        <v>367</v>
+        <v>415</v>
       </c>
       <c r="D41" s="610"/>
       <c r="E41" s="610"/>
@@ -14717,11 +14957,11 @@
     </row>
     <row r="43" spans="1:14" customHeight="1" ht="13.5">
       <c r="A43" s="64" t="s">
-        <v>368</v>
+        <v>416</v>
       </c>
       <c r="B43" s="65"/>
       <c r="C43" s="610" t="s">
-        <v>369</v>
+        <v>417</v>
       </c>
       <c r="D43" s="610"/>
       <c r="E43" s="610"/>
@@ -14742,7 +14982,7 @@
       <c r="E44" s="610"/>
       <c r="F44" s="609"/>
       <c r="G44" s="187" t="s">
-        <v>370</v>
+        <v>418</v>
       </c>
       <c r="H44" s="239"/>
       <c r="I44" s="118"/>
@@ -14753,11 +14993,11 @@
     </row>
     <row r="45" spans="1:14" customHeight="1" ht="13.5">
       <c r="A45" s="64" t="s">
-        <v>371</v>
+        <v>419</v>
       </c>
       <c r="B45" s="65"/>
       <c r="C45" s="609" t="s">
-        <v>372</v>
+        <v>420</v>
       </c>
       <c r="D45" s="609"/>
       <c r="E45" s="609"/>
@@ -14778,7 +15018,7 @@
       <c r="E46" s="609"/>
       <c r="F46" s="609"/>
       <c r="G46" s="188" t="s">
-        <v>373</v>
+        <v>421</v>
       </c>
       <c r="H46" s="240"/>
       <c r="I46" s="118"/>
@@ -14790,11 +15030,11 @@
     </row>
     <row r="47" spans="1:14" customHeight="1" ht="13.5">
       <c r="A47" s="64" t="s">
-        <v>374</v>
+        <v>422</v>
       </c>
       <c r="B47" s="65"/>
       <c r="C47" s="610" t="s">
-        <v>375</v>
+        <v>423</v>
       </c>
       <c r="D47" s="610"/>
       <c r="E47" s="115"/>
@@ -14815,7 +15055,7 @@
       <c r="E48" s="652"/>
       <c r="F48" s="653"/>
       <c r="G48" s="189" t="s">
-        <v>373</v>
+        <v>421</v>
       </c>
       <c r="H48" s="241"/>
       <c r="I48" s="120"/>
@@ -14843,11 +15083,11 @@
     </row>
     <row r="50" spans="1:14" customHeight="1" ht="23.25">
       <c r="A50" s="725" t="s">
-        <v>376</v>
+        <v>424</v>
       </c>
       <c r="B50" s="726"/>
       <c r="C50" s="185" t="s">
-        <v>377</v>
+        <v>425</v>
       </c>
       <c r="D50" s="185"/>
       <c r="E50" s="185"/>
@@ -14862,17 +15102,17 @@
     </row>
     <row r="51" spans="1:14" customHeight="1" ht="18">
       <c r="A51" s="648" t="s">
-        <v>378</v>
+        <v>426</v>
       </c>
       <c r="B51" s="649"/>
       <c r="C51" s="649"/>
       <c r="D51" s="649"/>
       <c r="E51" s="650"/>
       <c r="F51" s="177" t="s">
-        <v>379</v>
+        <v>427</v>
       </c>
       <c r="G51" s="657" t="s">
-        <v>380</v>
+        <v>428</v>
       </c>
       <c r="H51" s="577"/>
       <c r="I51" s="584"/>
@@ -14928,11 +15168,11 @@
     </row>
     <row r="55" spans="1:14" customHeight="1" ht="39.75">
       <c r="A55" s="624" t="s">
-        <v>381</v>
+        <v>429</v>
       </c>
       <c r="B55" s="625"/>
       <c r="C55" s="670" t="s">
-        <v>382</v>
+        <v>430</v>
       </c>
       <c r="D55" s="670"/>
       <c r="E55" s="670"/>
@@ -14957,7 +15197,7 @@
       <c r="I56" s="243"/>
       <c r="J56" s="192"/>
       <c r="K56" s="605" t="s">
-        <v>383</v>
+        <v>431</v>
       </c>
       <c r="L56" s="605"/>
       <c r="M56" s="176"/>
@@ -15007,7 +15247,7 @@
     <row r="60" spans="1:14" customHeight="1" ht="25.5">
       <c r="A60" s="75"/>
       <c r="B60" s="677" t="s">
-        <v>384</v>
+        <v>432</v>
       </c>
       <c r="C60" s="678"/>
       <c r="D60" s="679"/>
@@ -15022,7 +15262,7 @@
     <row r="61" spans="1:14" customHeight="1" ht="20.25">
       <c r="A61" s="75"/>
       <c r="B61" s="712" t="s">
-        <v>385</v>
+        <v>433</v>
       </c>
       <c r="C61" s="713"/>
       <c r="D61" s="131"/>
@@ -15037,7 +15277,7 @@
     <row r="62" spans="1:14" customHeight="1" ht="9">
       <c r="A62" s="75"/>
       <c r="B62" s="701" t="s">
-        <v>386</v>
+        <v>434</v>
       </c>
       <c r="C62" s="702"/>
       <c r="D62" s="680"/>
@@ -15055,7 +15295,7 @@
       <c r="C63" s="715"/>
       <c r="D63" s="681"/>
       <c r="F63" s="682" t="s">
-        <v>387</v>
+        <v>435</v>
       </c>
       <c r="G63" s="683"/>
       <c r="H63" s="683"/>
@@ -15067,7 +15307,7 @@
     <row r="64" spans="1:14" customHeight="1" ht="10.5">
       <c r="A64" s="75"/>
       <c r="B64" s="701" t="s">
-        <v>388</v>
+        <v>436</v>
       </c>
       <c r="C64" s="702"/>
       <c r="D64" s="680"/>
@@ -15086,14 +15326,14 @@
       <c r="C65" s="704"/>
       <c r="D65" s="705"/>
       <c r="F65" s="698" t="s">
-        <v>389</v>
+        <v>437</v>
       </c>
       <c r="G65" s="699"/>
       <c r="H65" s="699"/>
       <c r="I65" s="700"/>
       <c r="J65" s="78"/>
       <c r="K65" s="696" t="s">
-        <v>390</v>
+        <v>438</v>
       </c>
       <c r="L65" s="697"/>
       <c r="M65" s="76"/>
@@ -15115,7 +15355,7 @@
     </row>
     <row r="67" spans="1:14" customHeight="1" ht="28.5">
       <c r="A67" s="693" t="s">
-        <v>391</v>
+        <v>439</v>
       </c>
       <c r="B67" s="694"/>
       <c r="C67" s="694"/>
@@ -15150,7 +15390,7 @@
       <c r="C69" s="227"/>
       <c r="D69" s="227"/>
       <c r="E69" s="687" t="s">
-        <v>392</v>
+        <v>440</v>
       </c>
       <c r="F69" s="688"/>
       <c r="G69" s="688"/>
@@ -15178,7 +15418,7 @@
     </row>
     <row r="71" spans="1:14" customHeight="1" ht="10.5">
       <c r="A71" s="686" t="s">
-        <v>393</v>
+        <v>441</v>
       </c>
       <c r="B71" s="686"/>
       <c r="C71" s="686"/>
@@ -15357,45 +15597,45 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>394</v>
+        <v>442</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>395</v>
+        <v>443</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>396</v>
+        <v>444</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>397</v>
+        <v>445</v>
       </c>
       <c r="B2" t="s">
-        <v>398</v>
+        <v>446</v>
       </c>
       <c r="C2" t="s">
-        <v>399</v>
+        <v>447</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>400</v>
+        <v>448</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>401</v>
+        <v>449</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="B4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="B5" t="s">
-        <v>402</v>
+        <v>450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix some modules, and improved ui
</commit_message>
<xml_diff>
--- a/storage/PDS.xlsx
+++ b/storage/PDS.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="468">
   <si>
     <t xml:space="preserve">        </t>
   </si>
@@ -102,21 +102,18 @@
     <t>SURNAME</t>
   </si>
   <si>
-    <t>KIRK</t>
+    <t>JOHNS</t>
   </si>
   <si>
     <t>FIRST NAME</t>
   </si>
   <si>
-    <t>WALTER</t>
+    <t>ELDORA</t>
   </si>
   <si>
     <t xml:space="preserve">NAME EXTENSION (JR., SR)                                           </t>
   </si>
   <si>
-    <t>ALMA BEASLEY</t>
-  </si>
-  <si>
     <t>Married</t>
   </si>
   <si>
@@ -126,7 +123,7 @@
     <t>MIDDLE NAME</t>
   </si>
   <si>
-    <t>LOGAN YORK</t>
+    <t>CRONIN</t>
   </si>
   <si>
     <t>Widow/er</t>
@@ -142,12 +139,15 @@
 (mm/dd/yyyy)  </t>
   </si>
   <si>
-    <t>03-19-1977</t>
+    <t>02-02-2000</t>
   </si>
   <si>
     <t>16. CITIZENSHIP</t>
   </si>
   <si>
+    <t>Filipino</t>
+  </si>
+  <si>
     <t>Separated</t>
   </si>
   <si>
@@ -160,7 +160,7 @@
     <t>PLACE OF BIRTH</t>
   </si>
   <si>
-    <t>INVENTORE AD IN QUID</t>
+    <t>TUGUEGARAO CITY</t>
   </si>
   <si>
     <t xml:space="preserve">If holder of  dual citizenship, </t>
@@ -178,7 +178,7 @@
     <t>SEX</t>
   </si>
   <si>
-    <t>FEMALE</t>
+    <t>MALE</t>
   </si>
   <si>
     <t>please indicate the details.</t>
@@ -199,10 +199,7 @@
     <t>17. RESIDENTIAL ADDRESS</t>
   </si>
   <si>
-    <t>AMET QUI QUI MOLLIT</t>
-  </si>
-  <si>
-    <t>AUT LABORUM POSSIMUS</t>
+    <t>ASDF</t>
   </si>
   <si>
     <t>Angola</t>
@@ -217,10 +214,10 @@
     <t>Antigua and Barbuda</t>
   </si>
   <si>
-    <t>OFFICIA REPELLENDUS</t>
-  </si>
-  <si>
-    <t>CONSECTETUR ET DELE</t>
+    <t>SUBDIVISION</t>
+  </si>
+  <si>
+    <t>ATULAYAN</t>
   </si>
   <si>
     <t>Argentina</t>
@@ -244,13 +241,10 @@
     <t>HEIGHT (m)</t>
   </si>
   <si>
-    <t>LIBERO QUI CUMQUE SA</t>
-  </si>
-  <si>
-    <t>NON EST VERO INCIDID</t>
-  </si>
-  <si>
-    <t>ASPERNATUR UT SIT C</t>
+    <t>TUGUEGARAO</t>
+  </si>
+  <si>
+    <t>CAGAYAN</t>
   </si>
   <si>
     <t>Australia</t>
@@ -271,15 +265,9 @@
     <t>WEIGHT (kg)</t>
   </si>
   <si>
-    <t>NESCIUNT EUM COMMOD</t>
-  </si>
-  <si>
     <t xml:space="preserve">ZIP CODE    </t>
   </si>
   <si>
-    <t>TEMPORE AUT CUPIDIT</t>
-  </si>
-  <si>
     <t>Azerbaijan</t>
   </si>
   <si>
@@ -289,18 +277,12 @@
     <t>BLOOD TYPE</t>
   </si>
   <si>
-    <t>SAPIENTE ID IUSTO DE</t>
+    <t>O</t>
   </si>
   <si>
     <t>18. PERMANENT ADDRESS</t>
   </si>
   <si>
-    <t>AMET NECESSITATIBUS</t>
-  </si>
-  <si>
-    <t>DIGNISSIMOS QUIA COM</t>
-  </si>
-  <si>
     <t>Bahamas, The</t>
   </si>
   <si>
@@ -313,15 +295,6 @@
     <t>GSIS ID NO.</t>
   </si>
   <si>
-    <t>UNDE TEMPOR OCCAECAT</t>
-  </si>
-  <si>
-    <t>DUCIMUS LABORE APER</t>
-  </si>
-  <si>
-    <t>FACERE QUI CUMQUE IU</t>
-  </si>
-  <si>
     <t>Bangladesh</t>
   </si>
   <si>
@@ -334,15 +307,6 @@
     <t>PAG-IBIG ID NO.</t>
   </si>
   <si>
-    <t>NULLA A ALIQUID OCCA</t>
-  </si>
-  <si>
-    <t>QUIS PARIATUR CONSE</t>
-  </si>
-  <si>
-    <t>EST IPSA DOLOR ASPE</t>
-  </si>
-  <si>
     <t>Belarus</t>
   </si>
   <si>
@@ -355,9 +319,6 @@
     <t>PHILHEALTH NO.</t>
   </si>
   <si>
-    <t>AUT UT VOLUPTATE NOS</t>
-  </si>
-  <si>
     <t>Belize</t>
   </si>
   <si>
@@ -367,43 +328,28 @@
     <t>SSS NO.</t>
   </si>
   <si>
-    <t>MINIMA CONSECTETUR</t>
-  </si>
-  <si>
     <t>19. TELEPHONE NO.</t>
   </si>
   <si>
-    <t>MAIORES CUPIDATAT QU</t>
-  </si>
-  <si>
     <t>Benin</t>
   </si>
   <si>
     <t>14. TIN NO.</t>
   </si>
   <si>
-    <t>DOLOR IMPEDIT AUTE</t>
-  </si>
-  <si>
     <t>20. MOBILE NO.</t>
   </si>
   <si>
-    <t>FUGA VEL IPSAM QUIA</t>
-  </si>
-  <si>
     <t>Bhutan</t>
   </si>
   <si>
     <t>15. AGENCY EMPLOYEE NO.</t>
   </si>
   <si>
-    <t>VOLUPTAS ESSE QUIA S</t>
-  </si>
-  <si>
     <t>21. E-MAIL ADDRESS (if any)</t>
   </si>
   <si>
-    <t>KOTYTI@MAILINATOR.COM</t>
+    <t>JESTERADDURU@GMAIL.COM</t>
   </si>
   <si>
     <t>Bolivia</t>
@@ -421,7 +367,7 @@
     <t>SPOUSE'S SURNAME</t>
   </si>
   <si>
-    <t>LABORE VOLUPTATE CUP (deceased)</t>
+    <t>DUCIMUS FUGA POSSI</t>
   </si>
   <si>
     <t>23. NAME of CHILDREN  (Write full name and list all)</t>
@@ -436,13 +382,13 @@
     <t xml:space="preserve">  FIRST NAME</t>
   </si>
   <si>
-    <t>IPSA ODIO EX AUT EX</t>
+    <t>EXPEDITA REICIENDIS</t>
   </si>
   <si>
     <t xml:space="preserve">NAME EXTENSION (JR., SR)                                     </t>
   </si>
   <si>
-    <t>NUMQUAM IN ILLUM ET</t>
+    <t>QUASI REICIENDIS SIM</t>
   </si>
   <si>
     <t>Brazil</t>
@@ -451,7 +397,7 @@
     <t xml:space="preserve">  MIDDLE NAME</t>
   </si>
   <si>
-    <t>AUT DISTINCTIO ULLA</t>
+    <t>MOLESTIAE QUI QUI AU</t>
   </si>
   <si>
     <t>Brunei </t>
@@ -460,7 +406,7 @@
     <t>OCCUPATION</t>
   </si>
   <si>
-    <t>UT NON DEBITIS ISTE</t>
+    <t>DOLOR EXPEDITA ET FA</t>
   </si>
   <si>
     <t>Bulgaria</t>
@@ -469,7 +415,7 @@
     <t>EMPLOYER/BUSINESS NAME</t>
   </si>
   <si>
-    <t>VOLUPTATEM DISTINCTI</t>
+    <t>SINT QUAE SUNT QUIS</t>
   </si>
   <si>
     <t>Burkina Faso</t>
@@ -478,7 +424,7 @@
     <t>BUSINESS ADDRESS</t>
   </si>
   <si>
-    <t>REM RERUM ULLAMCO AL</t>
+    <t>RATIONE HARUM SUNT</t>
   </si>
   <si>
     <t>Burma</t>
@@ -487,7 +433,7 @@
     <t>TELEPHONE NO.</t>
   </si>
   <si>
-    <t>REPREHENDERIT EXPEDI</t>
+    <t>MODI EIUS UT LABORIO</t>
   </si>
   <si>
     <t>Burundi</t>
@@ -499,25 +445,25 @@
     <t>FATHER'S SURNAME</t>
   </si>
   <si>
-    <t>SUSCIPIT CONSEQUATUR (deceased)</t>
+    <t>OFFICIA CORPORIS AUT</t>
   </si>
   <si>
     <t>Cambodia</t>
   </si>
   <si>
-    <t>SED AMET UNDE DOLOR</t>
+    <t>ET ODIT CONSEQUUNTUR</t>
   </si>
   <si>
     <t xml:space="preserve">NAME EXTENSION (JR., SR)                                                  </t>
   </si>
   <si>
-    <t>SED DOLORE ADIPISICI</t>
+    <t>OFFICIA VENIAM ULLA</t>
   </si>
   <si>
     <t>Cameroon</t>
   </si>
   <si>
-    <t>LABORIOSAM NIHIL FU</t>
+    <t>IURE PLACEAT LABORE</t>
   </si>
   <si>
     <t>Canada</t>
@@ -532,19 +478,19 @@
     <t>Cape Verde</t>
   </si>
   <si>
-    <t>LOREM QUI SAPIENTE M</t>
+    <t>PROIDENT SIT EIUS N</t>
   </si>
   <si>
     <t>Central African Republic</t>
   </si>
   <si>
-    <t>VOLUPTAS COMMODO NON</t>
+    <t>EARUM ET CORPORIS EA</t>
   </si>
   <si>
     <t>Chad</t>
   </si>
   <si>
-    <t>NOSTRUM OPTIO ID FA</t>
+    <t>CONSEQUUNTUR OFFICIA</t>
   </si>
   <si>
     <t>(Continue on separate sheet if necessary)</t>
@@ -605,16 +551,31 @@
     <t>ELEMENTARY</t>
   </si>
   <si>
+    <t>TEST SCHOOL</t>
+  </si>
+  <si>
     <t>Congo, Republic of the</t>
   </si>
   <si>
     <t>SECONDARY</t>
   </si>
   <si>
+    <t>TEST HIGH SCHOOL</t>
+  </si>
+  <si>
+    <t>HIGH SCHOOL</t>
+  </si>
+  <si>
     <t>Costa Rica</t>
   </si>
   <si>
     <t>VOCATIONAL /                                                                                                                                                                                                        TRADE COURSE</t>
+  </si>
+  <si>
+    <t>TEST UNIVERSITY</t>
+  </si>
+  <si>
+    <t>BSIT</t>
   </si>
   <si>
     <t>Cote d'Ivoire</t>
@@ -1144,6 +1105,33 @@
 Validity</t>
   </si>
   <si>
+    <t>CS PROF</t>
+  </si>
+  <si>
+    <t>12/12/2012</t>
+  </si>
+  <si>
+    <t>12/31/2024</t>
+  </si>
+  <si>
+    <t>03/01/2020</t>
+  </si>
+  <si>
+    <t>TO PRESENT</t>
+  </si>
+  <si>
+    <t>ECONOMIC DEVELOPMENT SPECIALIST I</t>
+  </si>
+  <si>
+    <t>NEDA</t>
+  </si>
+  <si>
+    <t>PERMANENT</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
     <t xml:space="preserve">V.  WORK EXPERIENCE </t>
   </si>
   <si>
@@ -1193,6 +1181,30 @@
   </si>
   <si>
     <t>POSITION / NATURE OF WORK</t>
+  </si>
+  <si>
+    <t>TEST ORG</t>
+  </si>
+  <si>
+    <t>12/31/2018</t>
+  </si>
+  <si>
+    <t>12/31/2021</t>
+  </si>
+  <si>
+    <t>POSITION</t>
+  </si>
+  <si>
+    <t>TEST TRAINING</t>
+  </si>
+  <si>
+    <t>07/29/2024</t>
+  </si>
+  <si>
+    <t>TECHNICAL</t>
+  </si>
+  <si>
+    <t>DICT</t>
   </si>
   <si>
     <t>VII.  LEARNING AND DEVELOPMENT (L&amp;D) INTERVENTIONS/TRAINING PROGRAMS ATTENDED</t>
@@ -1236,6 +1248,9 @@
     <t>MEMBERSHIP IN ASSOCIATION/ORGANIZATION                                                                                         (Write in full)</t>
   </si>
   <si>
+    <t>GAWAD NG DIREKTOR</t>
+  </si>
+  <si>
     <t xml:space="preserve"> CS FORM 212 (Revised 2017), Page 3 of 4</t>
   </si>
   <si>
@@ -1252,6 +1267,9 @@
   </si>
   <si>
     <t>a. within the third degree?</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
   <si>
     <t>b. within the fourth degree (for Local Government Unit - Career Employees)?</t>
@@ -1386,6 +1404,33 @@
     <t>TEL. NO.</t>
   </si>
   <si>
+    <t>RIA COOK</t>
+  </si>
+  <si>
+    <t>CHESTER ADKINS</t>
+  </si>
+  <si>
+    <t>DEXTER POPE</t>
+  </si>
+  <si>
+    <t>WARREN SINGLETON</t>
+  </si>
+  <si>
+    <t>HEDWIG GENTRY</t>
+  </si>
+  <si>
+    <t>QUINTESSA HOWARD</t>
+  </si>
+  <si>
+    <t>RAYA GILMORE</t>
+  </si>
+  <si>
+    <t>CAILIN HARRIS</t>
+  </si>
+  <si>
+    <t>ECHO KIRKLAND</t>
+  </si>
+  <si>
     <t>42.</t>
   </si>
   <si>
@@ -1460,6 +1505,9 @@
     <t xml:space="preserve">Government Issued ID: </t>
   </si>
   <si>
+    <t>MATTHEW SHARPE</t>
+  </si>
+  <si>
     <t xml:space="preserve">ID/License/Passport No.: </t>
   </si>
   <si>
@@ -1467,6 +1515,9 @@
   </si>
   <si>
     <t>Date/Place of Issuance:</t>
+  </si>
+  <si>
+    <t>DECEMBER 25, 2023</t>
   </si>
   <si>
     <t>Date Accomplished</t>
@@ -7113,24 +7164,22 @@
         <v>16</v>
       </c>
       <c r="M11" s="366"/>
-      <c r="N11" s="252" t="s">
+      <c r="N11" s="252"/>
+      <c r="P11" s="96" t="s">
         <v>17</v>
       </c>
-      <c r="P11" s="96" t="s">
+      <c r="Q11" s="143" t="s">
         <v>18</v>
-      </c>
-      <c r="Q11" s="143" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:19" customHeight="1" ht="21.75">
       <c r="A12" s="164"/>
       <c r="B12" s="398" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="399"/>
       <c r="D12" s="194" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" s="195"/>
       <c r="F12" s="195"/>
@@ -7143,31 +7192,33 @@
       <c r="M12" s="199"/>
       <c r="N12" s="200"/>
       <c r="P12" s="96" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q12" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="Q12" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:19" customHeight="1" ht="24">
       <c r="A13" s="226" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="379" t="s">
         <v>24</v>
-      </c>
-      <c r="B13" s="379" t="s">
-        <v>25</v>
       </c>
       <c r="C13" s="380"/>
       <c r="D13" s="268" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="268"/>
       <c r="F13" s="269"/>
       <c r="G13" s="102" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H13" s="145"/>
       <c r="I13" s="145"/>
-      <c r="J13" s="359"/>
+      <c r="J13" s="359" t="s">
+        <v>27</v>
+      </c>
       <c r="K13" s="360"/>
       <c r="L13" s="360"/>
       <c r="M13" s="360"/>
@@ -7274,18 +7325,18 @@
         <v>44</v>
       </c>
       <c r="H17" s="104"/>
-      <c r="I17" s="354" t="s">
-        <v>45</v>
+      <c r="I17" s="354">
+        <v>321231</v>
       </c>
       <c r="J17" s="355"/>
       <c r="K17" s="355"/>
       <c r="L17" s="355" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M17" s="355"/>
       <c r="N17" s="362"/>
       <c r="Q17" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:19" customHeight="1" ht="9">
@@ -7298,17 +7349,17 @@
       <c r="G18" s="151"/>
       <c r="H18" s="255"/>
       <c r="I18" s="363" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J18" s="364"/>
       <c r="K18" s="364"/>
       <c r="L18" s="364" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M18" s="364"/>
       <c r="N18" s="367"/>
       <c r="Q18" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:19" customHeight="1" ht="5.25">
@@ -7321,17 +7372,17 @@
       <c r="G19" s="151"/>
       <c r="H19" s="255"/>
       <c r="I19" s="377" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J19" s="312"/>
       <c r="K19" s="312"/>
       <c r="L19" s="311" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M19" s="312"/>
       <c r="N19" s="313"/>
       <c r="Q19" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:19" customHeight="1" ht="9.75">
@@ -7350,7 +7401,7 @@
       <c r="M20" s="314"/>
       <c r="N20" s="315"/>
       <c r="Q20" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:19" customHeight="1" ht="9">
@@ -7363,46 +7414,46 @@
       <c r="G21" s="149"/>
       <c r="H21" s="251"/>
       <c r="I21" s="316" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J21" s="317"/>
       <c r="K21" s="317"/>
       <c r="L21" s="430" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M21" s="431"/>
       <c r="N21" s="432"/>
       <c r="Q21" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:19" customHeight="1" ht="15.75">
       <c r="A22" s="326" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="330" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="330" t="s">
-        <v>59</v>
-      </c>
       <c r="C22" s="331"/>
-      <c r="D22" s="320" t="s">
-        <v>60</v>
+      <c r="D22" s="320">
+        <v>100</v>
       </c>
       <c r="E22" s="277"/>
       <c r="F22" s="321"/>
       <c r="G22" s="149"/>
       <c r="H22" s="251"/>
       <c r="I22" s="354" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J22" s="355"/>
       <c r="K22" s="355"/>
       <c r="L22" s="355" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M22" s="355"/>
       <c r="N22" s="362"/>
       <c r="Q22" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:19" customHeight="1" ht="8.25">
@@ -7415,38 +7466,38 @@
       <c r="G23" s="149"/>
       <c r="H23" s="251"/>
       <c r="I23" s="435" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J23" s="436"/>
       <c r="K23" s="436"/>
       <c r="L23" s="433" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M23" s="433"/>
       <c r="N23" s="434"/>
       <c r="Q23" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:19" customHeight="1" ht="22.5">
       <c r="A24" s="163" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B24" s="334" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C24" s="335"/>
-      <c r="D24" s="351" t="s">
-        <v>69</v>
+      <c r="D24" s="351">
+        <v>100</v>
       </c>
       <c r="E24" s="352"/>
       <c r="F24" s="353"/>
       <c r="G24" s="400" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H24" s="401"/>
-      <c r="I24" s="368" t="s">
-        <v>71</v>
+      <c r="I24" s="368">
+        <v>3500</v>
       </c>
       <c r="J24" s="369"/>
       <c r="K24" s="369"/>
@@ -7454,38 +7505,34 @@
       <c r="M24" s="369"/>
       <c r="N24" s="370"/>
       <c r="Q24" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:19" customHeight="1" ht="15.75">
       <c r="A25" s="318" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B25" s="330" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C25" s="331"/>
       <c r="D25" s="320" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E25" s="277"/>
       <c r="F25" s="321"/>
       <c r="G25" s="109" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H25" s="99"/>
-      <c r="I25" s="354" t="s">
-        <v>77</v>
-      </c>
+      <c r="I25" s="354"/>
       <c r="J25" s="355"/>
       <c r="K25" s="355"/>
-      <c r="L25" s="355" t="s">
-        <v>78</v>
-      </c>
+      <c r="L25" s="355"/>
       <c r="M25" s="355"/>
       <c r="N25" s="362"/>
       <c r="Q25" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:19" customHeight="1" ht="9">
@@ -7498,46 +7545,42 @@
       <c r="G26" s="149"/>
       <c r="H26" s="251"/>
       <c r="I26" s="363" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J26" s="364"/>
       <c r="K26" s="364"/>
       <c r="L26" s="364" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M26" s="364"/>
       <c r="N26" s="367"/>
       <c r="Q26" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:19" customHeight="1" ht="15.75">
       <c r="A27" s="318" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B27" s="330" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C27" s="331"/>
-      <c r="D27" s="320" t="s">
-        <v>83</v>
+      <c r="D27" s="320">
+        <v>1324</v>
       </c>
       <c r="E27" s="277"/>
       <c r="F27" s="321"/>
       <c r="G27" s="151"/>
       <c r="H27" s="255"/>
-      <c r="I27" s="354" t="s">
-        <v>84</v>
-      </c>
+      <c r="I27" s="354"/>
       <c r="J27" s="355"/>
       <c r="K27" s="355"/>
-      <c r="L27" s="355" t="s">
-        <v>85</v>
-      </c>
+      <c r="L27" s="355"/>
       <c r="M27" s="355"/>
       <c r="N27" s="362"/>
       <c r="Q27" s="3" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:19" customHeight="1" ht="9">
@@ -7550,46 +7593,42 @@
       <c r="G28" s="151"/>
       <c r="H28" s="255"/>
       <c r="I28" s="412" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J28" s="410"/>
       <c r="K28" s="410"/>
       <c r="L28" s="409" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M28" s="410"/>
       <c r="N28" s="411"/>
       <c r="Q28" s="3" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:19" customHeight="1" ht="15.75">
       <c r="A29" s="318" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B29" s="330" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C29" s="331"/>
-      <c r="D29" s="320" t="s">
-        <v>90</v>
+      <c r="D29" s="320">
+        <v>1234</v>
       </c>
       <c r="E29" s="277"/>
       <c r="F29" s="321"/>
       <c r="G29" s="151"/>
       <c r="H29" s="156"/>
-      <c r="I29" s="407" t="s">
-        <v>91</v>
-      </c>
+      <c r="I29" s="407"/>
       <c r="J29" s="408"/>
       <c r="K29" s="408"/>
-      <c r="L29" s="408" t="s">
-        <v>92</v>
-      </c>
+      <c r="L29" s="408"/>
       <c r="M29" s="408"/>
       <c r="N29" s="441"/>
       <c r="Q29" s="3" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:19" customHeight="1" ht="9.75">
@@ -7602,34 +7641,34 @@
       <c r="G30" s="151"/>
       <c r="H30" s="156"/>
       <c r="I30" s="437" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J30" s="437"/>
       <c r="K30" s="437"/>
       <c r="L30" s="437" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M30" s="437"/>
       <c r="N30" s="438"/>
       <c r="Q30" s="3" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:19" customHeight="1" ht="24.75">
       <c r="A31" s="165" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B31" s="97" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C31" s="98"/>
-      <c r="D31" s="351" t="s">
-        <v>97</v>
+      <c r="D31" s="351">
+        <v>12345313</v>
       </c>
       <c r="E31" s="352"/>
       <c r="F31" s="353"/>
       <c r="G31" s="439" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H31" s="440"/>
       <c r="I31" s="356"/>
@@ -7639,28 +7678,28 @@
       <c r="M31" s="357"/>
       <c r="N31" s="358"/>
       <c r="Q31" s="3" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:19" customHeight="1" ht="24.75">
       <c r="A32" s="163" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B32" s="97" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C32" s="98"/>
-      <c r="D32" s="351" t="s">
-        <v>101</v>
+      <c r="D32" s="351">
+        <v>131</v>
       </c>
       <c r="E32" s="352"/>
       <c r="F32" s="353"/>
       <c r="G32" s="373" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="H32" s="335"/>
-      <c r="I32" s="356" t="s">
-        <v>103</v>
+      <c r="I32" s="356">
+        <v>99999999</v>
       </c>
       <c r="J32" s="357"/>
       <c r="K32" s="357"/>
@@ -7668,26 +7707,26 @@
       <c r="M32" s="357"/>
       <c r="N32" s="358"/>
       <c r="Q32" s="3" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:19" customHeight="1" ht="24.75">
       <c r="A33" s="402" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="B33" s="335"/>
       <c r="C33" s="403"/>
-      <c r="D33" s="351" t="s">
-        <v>106</v>
+      <c r="D33" s="351">
+        <v>31331</v>
       </c>
       <c r="E33" s="352"/>
       <c r="F33" s="353"/>
       <c r="G33" s="196" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="H33" s="150"/>
-      <c r="I33" s="356" t="s">
-        <v>108</v>
+      <c r="I33" s="356">
+        <v>9999999</v>
       </c>
       <c r="J33" s="357"/>
       <c r="K33" s="357"/>
@@ -7695,26 +7734,26 @@
       <c r="M33" s="357"/>
       <c r="N33" s="358"/>
       <c r="Q33" s="3" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:19" customHeight="1" ht="24.75">
       <c r="A34" s="168" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="B34" s="254"/>
       <c r="C34" s="152"/>
-      <c r="D34" s="390" t="s">
-        <v>111</v>
+      <c r="D34" s="390">
+        <v>31232</v>
       </c>
       <c r="E34" s="391"/>
       <c r="F34" s="392"/>
       <c r="G34" s="109" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="H34" s="99"/>
       <c r="I34" s="356" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="J34" s="357"/>
       <c r="K34" s="357"/>
@@ -7722,12 +7761,12 @@
       <c r="M34" s="357"/>
       <c r="N34" s="358"/>
       <c r="Q34" s="3" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:19" customHeight="1" ht="16.5">
       <c r="A35" s="205" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="B35" s="206"/>
       <c r="C35" s="206"/>
@@ -7743,54 +7782,54 @@
       <c r="M35" s="206"/>
       <c r="N35" s="207"/>
       <c r="Q35" s="3" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:19" customHeight="1" ht="21">
       <c r="A36" s="102" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="B36" s="215" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="C36" s="216"/>
       <c r="D36" s="309" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="E36" s="309"/>
       <c r="F36" s="309"/>
       <c r="G36" s="309"/>
       <c r="H36" s="309"/>
       <c r="I36" s="291" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="J36" s="291"/>
       <c r="K36" s="291"/>
       <c r="L36" s="292"/>
       <c r="M36" s="328" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="N36" s="329"/>
       <c r="Q36" s="3" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:19" customHeight="1" ht="21">
       <c r="A37" s="149"/>
       <c r="B37" s="255" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="C37" s="156"/>
       <c r="D37" s="404" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="E37" s="405"/>
       <c r="F37" s="406"/>
       <c r="G37" s="247" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="H37" s="248" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="I37" s="293"/>
       <c r="J37" s="266"/>
@@ -7799,17 +7838,17 @@
       <c r="M37" s="289"/>
       <c r="N37" s="290"/>
       <c r="Q37" s="3" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:19" customHeight="1" ht="21">
       <c r="A38" s="169"/>
       <c r="B38" s="210" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="C38" s="209"/>
       <c r="D38" s="404" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="E38" s="405"/>
       <c r="F38" s="405"/>
@@ -7822,17 +7861,17 @@
       <c r="M38" s="289"/>
       <c r="N38" s="290"/>
       <c r="Q38" s="3" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:19" customHeight="1" ht="21">
       <c r="A39" s="170"/>
       <c r="B39" s="97" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="C39" s="98"/>
       <c r="D39" s="310" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="E39" s="310"/>
       <c r="F39" s="310"/>
@@ -7845,17 +7884,17 @@
       <c r="M39" s="289"/>
       <c r="N39" s="290"/>
       <c r="Q39" s="3" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:19" customHeight="1" ht="21">
       <c r="A40" s="170"/>
       <c r="B40" s="97" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="C40" s="98"/>
       <c r="D40" s="310" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="E40" s="310"/>
       <c r="F40" s="310"/>
@@ -7868,17 +7907,17 @@
       <c r="M40" s="289"/>
       <c r="N40" s="290"/>
       <c r="Q40" s="3" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:19" customHeight="1" ht="21">
       <c r="A41" s="170"/>
       <c r="B41" s="97" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="C41" s="98"/>
       <c r="D41" s="310" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="E41" s="310"/>
       <c r="F41" s="310"/>
@@ -7891,17 +7930,17 @@
       <c r="M41" s="289"/>
       <c r="N41" s="290"/>
       <c r="Q41" s="3" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:19" customHeight="1" ht="21">
       <c r="A42" s="103"/>
       <c r="B42" s="104" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="C42" s="137"/>
       <c r="D42" s="310" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="E42" s="310"/>
       <c r="F42" s="310"/>
@@ -7914,19 +7953,19 @@
       <c r="M42" s="289"/>
       <c r="N42" s="290"/>
       <c r="Q42" s="3" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:19" customHeight="1" ht="21">
       <c r="A43" s="208" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="B43" s="213" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="C43" s="104"/>
       <c r="D43" s="310" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="E43" s="310"/>
       <c r="F43" s="310"/>
@@ -7939,7 +7978,7 @@
       <c r="M43" s="289"/>
       <c r="N43" s="290"/>
       <c r="Q43" s="3" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
     </row>
     <row r="44" spans="1:19" customHeight="1" ht="21">
@@ -7949,15 +7988,15 @@
       </c>
       <c r="C44" s="251"/>
       <c r="D44" s="404" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="E44" s="405"/>
       <c r="F44" s="406"/>
       <c r="G44" s="247" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="H44" s="248" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="I44" s="266"/>
       <c r="J44" s="266"/>
@@ -7966,17 +8005,17 @@
       <c r="M44" s="289"/>
       <c r="N44" s="290"/>
       <c r="Q44" s="3" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:19" customHeight="1" ht="21">
       <c r="A45" s="169"/>
       <c r="B45" s="203" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C45" s="203"/>
       <c r="D45" s="404" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="E45" s="405"/>
       <c r="F45" s="405"/>
@@ -7989,15 +8028,15 @@
       <c r="M45" s="289"/>
       <c r="N45" s="290"/>
       <c r="Q45" s="3" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46" spans="1:19" customHeight="1" ht="21">
       <c r="A46" s="149" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="B46" s="104" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="C46" s="104"/>
       <c r="D46" s="308"/>
@@ -8012,7 +8051,7 @@
       <c r="M46" s="289"/>
       <c r="N46" s="290"/>
       <c r="Q46" s="3" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:19" customHeight="1" ht="21">
@@ -8022,7 +8061,7 @@
       </c>
       <c r="C47" s="251"/>
       <c r="D47" s="461" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="E47" s="461"/>
       <c r="F47" s="461"/>
@@ -8035,7 +8074,7 @@
       <c r="M47" s="289"/>
       <c r="N47" s="290"/>
       <c r="Q47" s="3" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="1:19" customHeight="1" ht="21">
@@ -8045,7 +8084,7 @@
       </c>
       <c r="C48" s="251"/>
       <c r="D48" s="461" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="E48" s="461"/>
       <c r="F48" s="461"/>
@@ -8058,24 +8097,24 @@
       <c r="M48" s="289"/>
       <c r="N48" s="290"/>
       <c r="Q48" s="3" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:19" customHeight="1" ht="21">
       <c r="A49" s="171"/>
       <c r="B49" s="204" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C49" s="204"/>
       <c r="D49" s="301" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="E49" s="301"/>
       <c r="F49" s="301"/>
       <c r="G49" s="301"/>
       <c r="H49" s="301"/>
       <c r="I49" s="299" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="J49" s="299"/>
       <c r="K49" s="299"/>
@@ -8083,12 +8122,12 @@
       <c r="M49" s="299"/>
       <c r="N49" s="300"/>
       <c r="Q49" s="3" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
     </row>
     <row r="50" spans="1:19" customHeight="1" ht="15.75">
       <c r="A50" s="172" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="B50" s="172"/>
       <c r="C50" s="100"/>
@@ -8098,7 +8137,7 @@
       <c r="G50" s="101"/>
       <c r="H50" s="101"/>
       <c r="I50" s="388" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="J50" s="388"/>
       <c r="K50" s="388"/>
@@ -8106,42 +8145,42 @@
       <c r="M50" s="388"/>
       <c r="N50" s="389"/>
       <c r="Q50" s="3" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
     </row>
     <row r="51" spans="1:19" customHeight="1" ht="14.25">
       <c r="A51" s="381" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="B51" s="413" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="C51" s="413"/>
       <c r="D51" s="416" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="E51" s="417"/>
       <c r="F51" s="418"/>
       <c r="G51" s="416" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="H51" s="417"/>
       <c r="I51" s="462"/>
       <c r="J51" s="302" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="K51" s="303"/>
       <c r="L51" s="459" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="M51" s="383" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="N51" s="306" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="Q51" s="3" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
     </row>
     <row r="52" spans="1:19" customHeight="1" ht="19.5">
@@ -8160,7 +8199,7 @@
       <c r="M52" s="383"/>
       <c r="N52" s="306"/>
       <c r="Q52" s="3" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:19" customHeight="1" ht="14.25">
@@ -8174,10 +8213,10 @@
       <c r="H53" s="423"/>
       <c r="I53" s="464"/>
       <c r="J53" s="105" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="K53" s="106" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="L53" s="460"/>
       <c r="M53" s="384"/>
@@ -8185,76 +8224,106 @@
       <c r="O53" s="107"/>
       <c r="P53" s="107"/>
       <c r="Q53" s="3" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
     </row>
     <row r="54" spans="1:19" customHeight="1" ht="28.5">
       <c r="A54" s="217"/>
       <c r="B54" s="218" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="C54" s="218"/>
-      <c r="D54" s="424"/>
+      <c r="D54" s="424" t="s">
+        <v>162</v>
+      </c>
       <c r="E54" s="425"/>
       <c r="F54" s="426"/>
-      <c r="G54" s="294"/>
+      <c r="G54" s="294" t="s">
+        <v>161</v>
+      </c>
       <c r="H54" s="295"/>
       <c r="I54" s="296"/>
-      <c r="J54" s="157"/>
-      <c r="K54" s="260"/>
+      <c r="J54" s="157">
+        <v>2000</v>
+      </c>
+      <c r="K54" s="260">
+        <v>2006</v>
+      </c>
       <c r="L54" s="157"/>
-      <c r="M54" s="18"/>
+      <c r="M54" s="18">
+        <v>2006</v>
+      </c>
       <c r="N54" s="153"/>
       <c r="Q54" s="3" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
     </row>
     <row r="55" spans="1:19" customHeight="1" ht="28.5">
       <c r="A55" s="217"/>
       <c r="B55" s="218" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="C55" s="218"/>
-      <c r="D55" s="424"/>
+      <c r="D55" s="424" t="s">
+        <v>165</v>
+      </c>
       <c r="E55" s="425"/>
       <c r="F55" s="426"/>
-      <c r="G55" s="294"/>
+      <c r="G55" s="294" t="s">
+        <v>166</v>
+      </c>
       <c r="H55" s="295"/>
       <c r="I55" s="296"/>
-      <c r="J55" s="157"/>
-      <c r="K55" s="260"/>
+      <c r="J55" s="157">
+        <v>2007</v>
+      </c>
+      <c r="K55" s="260">
+        <v>2011</v>
+      </c>
       <c r="L55" s="157"/>
-      <c r="M55" s="19"/>
+      <c r="M55" s="19">
+        <v>2011</v>
+      </c>
       <c r="N55" s="153"/>
       <c r="Q55" s="3" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
     </row>
     <row r="56" spans="1:19" customHeight="1" ht="28.5">
       <c r="A56" s="217"/>
       <c r="B56" s="218" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="C56" s="218"/>
-      <c r="D56" s="424"/>
+      <c r="D56" s="424" t="s">
+        <v>169</v>
+      </c>
       <c r="E56" s="425"/>
       <c r="F56" s="426"/>
-      <c r="G56" s="294"/>
+      <c r="G56" s="294" t="s">
+        <v>170</v>
+      </c>
       <c r="H56" s="295"/>
       <c r="I56" s="296"/>
-      <c r="J56" s="157"/>
-      <c r="K56" s="260"/>
+      <c r="J56" s="157">
+        <v>2012</v>
+      </c>
+      <c r="K56" s="260">
+        <v>2016</v>
+      </c>
       <c r="L56" s="157"/>
-      <c r="M56" s="18"/>
+      <c r="M56" s="18">
+        <v>2016</v>
+      </c>
       <c r="N56" s="153"/>
       <c r="Q56" s="3" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
     <row r="57" spans="1:19" customHeight="1" ht="28.5">
       <c r="A57" s="217"/>
       <c r="B57" s="218" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C57" s="218"/>
       <c r="D57" s="424"/>
@@ -8269,13 +8338,13 @@
       <c r="M57" s="19"/>
       <c r="N57" s="153"/>
       <c r="Q57" s="3" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="58" spans="1:19" customHeight="1" ht="28.5">
       <c r="A58" s="219"/>
       <c r="B58" s="220" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="C58" s="220"/>
       <c r="D58" s="427"/>
@@ -8290,12 +8359,12 @@
       <c r="M58" s="21"/>
       <c r="N58" s="153"/>
       <c r="Q58" s="3" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59" spans="1:19" customHeight="1" ht="12">
       <c r="A59" s="448" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="B59" s="449"/>
       <c r="C59" s="449"/>
@@ -8311,12 +8380,12 @@
       <c r="M59" s="449"/>
       <c r="N59" s="450"/>
       <c r="Q59" s="3" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
     </row>
     <row r="60" spans="1:19" customHeight="1" ht="27.75">
       <c r="A60" s="445" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="B60" s="446"/>
       <c r="C60" s="447"/>
@@ -8327,19 +8396,19 @@
       <c r="H60" s="455"/>
       <c r="I60" s="456"/>
       <c r="J60" s="457" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="K60" s="458"/>
       <c r="L60" s="451"/>
       <c r="M60" s="452"/>
       <c r="N60" s="453"/>
       <c r="Q60" s="3" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
     </row>
     <row r="61" spans="1:19" customHeight="1" ht="12" s="143" customFormat="1">
       <c r="A61" s="442" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="B61" s="443"/>
       <c r="C61" s="443"/>
@@ -8355,7 +8424,7 @@
       <c r="M61" s="443"/>
       <c r="N61" s="444"/>
       <c r="Q61" s="233" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
     </row>
     <row r="62" spans="1:19" customHeight="1" ht="14.25">
@@ -8374,7 +8443,7 @@
       <c r="M62" s="108"/>
       <c r="N62" s="108"/>
       <c r="Q62" s="3" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
     </row>
     <row r="63" spans="1:19" customHeight="1" ht="14.25">
@@ -8393,7 +8462,7 @@
       <c r="M63" s="108"/>
       <c r="N63" s="108"/>
       <c r="Q63" s="3" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
     </row>
     <row r="64" spans="1:19" customHeight="1" ht="28.5">
@@ -8412,7 +8481,7 @@
       <c r="M64" s="108"/>
       <c r="N64" s="108"/>
       <c r="Q64" s="3" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
     </row>
     <row r="65" spans="1:19" customHeight="1" ht="14.25">
@@ -8431,7 +8500,7 @@
       <c r="M65" s="108"/>
       <c r="N65" s="108"/>
       <c r="Q65" s="3" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
     </row>
     <row r="66" spans="1:19" customHeight="1" ht="14.25">
@@ -8450,7 +8519,7 @@
       <c r="M66" s="108"/>
       <c r="N66" s="108"/>
       <c r="Q66" s="3" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
     </row>
     <row r="67" spans="1:19" customHeight="1" ht="14.25">
@@ -8469,7 +8538,7 @@
       <c r="M67" s="108"/>
       <c r="N67" s="108"/>
       <c r="Q67" s="3" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
     </row>
     <row r="68" spans="1:19" customHeight="1" ht="14.25">
@@ -8488,7 +8557,7 @@
       <c r="M68" s="108"/>
       <c r="N68" s="108"/>
       <c r="Q68" s="3" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
     </row>
     <row r="69" spans="1:19" customHeight="1" ht="28.5">
@@ -8507,7 +8576,7 @@
       <c r="M69" s="108"/>
       <c r="N69" s="108"/>
       <c r="Q69" s="3" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
     </row>
     <row r="70" spans="1:19" customHeight="1" ht="14.25">
@@ -8526,7 +8595,7 @@
       <c r="M70" s="108"/>
       <c r="N70" s="108"/>
       <c r="Q70" s="3" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
     </row>
     <row r="71" spans="1:19" customHeight="1" ht="14.25">
@@ -8545,7 +8614,7 @@
       <c r="M71" s="108"/>
       <c r="N71" s="108"/>
       <c r="Q71" s="3" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
     </row>
     <row r="72" spans="1:19" customHeight="1" ht="14.25">
@@ -8564,7 +8633,7 @@
       <c r="M72" s="108"/>
       <c r="N72" s="108"/>
       <c r="Q72" s="3" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
     </row>
     <row r="73" spans="1:19" customHeight="1" ht="14.25">
@@ -8583,7 +8652,7 @@
       <c r="M73" s="108"/>
       <c r="N73" s="108"/>
       <c r="Q73" s="3" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
     </row>
     <row r="74" spans="1:19" customHeight="1" ht="14.25">
@@ -8602,7 +8671,7 @@
       <c r="M74" s="108"/>
       <c r="N74" s="108"/>
       <c r="Q74" s="3" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="75" spans="1:19" customHeight="1" ht="14.25">
@@ -8621,7 +8690,7 @@
       <c r="M75" s="108"/>
       <c r="N75" s="108"/>
       <c r="Q75" s="3" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="76" spans="1:19" customHeight="1" ht="14.25">
@@ -8640,7 +8709,7 @@
       <c r="M76" s="108"/>
       <c r="N76" s="108"/>
       <c r="Q76" s="3" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="77" spans="1:19" customHeight="1" ht="14.25">
@@ -8659,7 +8728,7 @@
       <c r="M77" s="108"/>
       <c r="N77" s="108"/>
       <c r="Q77" s="3" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
     </row>
     <row r="78" spans="1:19" customHeight="1" ht="14.25">
@@ -8678,7 +8747,7 @@
       <c r="M78" s="108"/>
       <c r="N78" s="108"/>
       <c r="Q78" s="3" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
     </row>
     <row r="79" spans="1:19" customHeight="1" ht="14.25">
@@ -8697,7 +8766,7 @@
       <c r="M79" s="108"/>
       <c r="N79" s="108"/>
       <c r="Q79" s="3" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
     </row>
     <row r="80" spans="1:19" customHeight="1" ht="14.25">
@@ -8716,7 +8785,7 @@
       <c r="M80" s="108"/>
       <c r="N80" s="108"/>
       <c r="Q80" s="3" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
     </row>
     <row r="81" spans="1:19" customHeight="1" ht="14.25">
@@ -8735,7 +8804,7 @@
       <c r="M81" s="108"/>
       <c r="N81" s="108"/>
       <c r="Q81" s="3" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
     </row>
     <row r="82" spans="1:19" customHeight="1" ht="14.25">
@@ -8754,7 +8823,7 @@
       <c r="M82" s="108"/>
       <c r="N82" s="108"/>
       <c r="Q82" s="3" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
     </row>
     <row r="83" spans="1:19" customHeight="1" ht="14.25">
@@ -8773,7 +8842,7 @@
       <c r="M83" s="108"/>
       <c r="N83" s="108"/>
       <c r="Q83" s="3" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
     </row>
     <row r="84" spans="1:19" customHeight="1" ht="14.25">
@@ -8792,7 +8861,7 @@
       <c r="M84" s="108"/>
       <c r="N84" s="108"/>
       <c r="Q84" s="3" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
     </row>
     <row r="85" spans="1:19" customHeight="1" ht="28.5">
@@ -8811,7 +8880,7 @@
       <c r="M85" s="108"/>
       <c r="N85" s="108"/>
       <c r="Q85" s="3" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
     </row>
     <row r="86" spans="1:19" customHeight="1" ht="14.25">
@@ -8830,7 +8899,7 @@
       <c r="M86" s="108"/>
       <c r="N86" s="108"/>
       <c r="Q86" s="3" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
     </row>
     <row r="87" spans="1:19" customHeight="1" ht="14.25">
@@ -8849,7 +8918,7 @@
       <c r="M87" s="108"/>
       <c r="N87" s="108"/>
       <c r="Q87" s="3" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
     </row>
     <row r="88" spans="1:19" customHeight="1" ht="14.25">
@@ -8868,7 +8937,7 @@
       <c r="M88" s="108"/>
       <c r="N88" s="108"/>
       <c r="Q88" s="3" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
     </row>
     <row r="89" spans="1:19" customHeight="1" ht="14.25">
@@ -8887,7 +8956,7 @@
       <c r="M89" s="108"/>
       <c r="N89" s="108"/>
       <c r="Q89" s="3" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
     </row>
     <row r="90" spans="1:19" customHeight="1" ht="14.25">
@@ -8906,7 +8975,7 @@
       <c r="M90" s="108"/>
       <c r="N90" s="108"/>
       <c r="Q90" s="3" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
     </row>
     <row r="91" spans="1:19" customHeight="1" ht="14.25">
@@ -8925,7 +8994,7 @@
       <c r="M91" s="108"/>
       <c r="N91" s="108"/>
       <c r="Q91" s="3" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
     </row>
     <row r="92" spans="1:19" customHeight="1" ht="14.25">
@@ -8944,7 +9013,7 @@
       <c r="M92" s="108"/>
       <c r="N92" s="108"/>
       <c r="Q92" s="3" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
     </row>
     <row r="93" spans="1:19" customHeight="1" ht="14.25">
@@ -8963,7 +9032,7 @@
       <c r="M93" s="108"/>
       <c r="N93" s="108"/>
       <c r="Q93" s="3" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
     </row>
     <row r="94" spans="1:19" customHeight="1" ht="14.25">
@@ -8982,7 +9051,7 @@
       <c r="M94" s="108"/>
       <c r="N94" s="108"/>
       <c r="Q94" s="3" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
     </row>
     <row r="95" spans="1:19" customHeight="1" ht="14.25">
@@ -9001,7 +9070,7 @@
       <c r="M95" s="108"/>
       <c r="N95" s="108"/>
       <c r="Q95" s="3" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
     </row>
     <row r="96" spans="1:19" customHeight="1" ht="14.25">
@@ -9020,7 +9089,7 @@
       <c r="M96" s="108"/>
       <c r="N96" s="108"/>
       <c r="Q96" s="3" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
     </row>
     <row r="97" spans="1:19" customHeight="1" ht="14.25">
@@ -9039,7 +9108,7 @@
       <c r="M97" s="108"/>
       <c r="N97" s="108"/>
       <c r="Q97" s="3" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
     </row>
     <row r="98" spans="1:19" customHeight="1" ht="14.25">
@@ -9058,7 +9127,7 @@
       <c r="M98" s="108"/>
       <c r="N98" s="108"/>
       <c r="Q98" s="3" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
     </row>
     <row r="99" spans="1:19" customHeight="1" ht="14.25">
@@ -9077,7 +9146,7 @@
       <c r="M99" s="108"/>
       <c r="N99" s="108"/>
       <c r="Q99" s="3" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
     </row>
     <row r="100" spans="1:19" customHeight="1" ht="14.25">
@@ -9096,7 +9165,7 @@
       <c r="M100" s="108"/>
       <c r="N100" s="108"/>
       <c r="Q100" s="3" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
     </row>
     <row r="101" spans="1:19" customHeight="1" ht="14.25">
@@ -9115,7 +9184,7 @@
       <c r="M101" s="108"/>
       <c r="N101" s="108"/>
       <c r="Q101" s="3" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
     </row>
     <row r="102" spans="1:19" customHeight="1" ht="14.25">
@@ -9134,7 +9203,7 @@
       <c r="M102" s="108"/>
       <c r="N102" s="108"/>
       <c r="Q102" s="3" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
     </row>
     <row r="103" spans="1:19" customHeight="1" ht="14.25">
@@ -9153,7 +9222,7 @@
       <c r="M103" s="108"/>
       <c r="N103" s="108"/>
       <c r="Q103" s="3" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
     </row>
     <row r="104" spans="1:19" customHeight="1" ht="14.25">
@@ -9172,7 +9241,7 @@
       <c r="M104" s="108"/>
       <c r="N104" s="108"/>
       <c r="Q104" s="3" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
     </row>
     <row r="105" spans="1:19" customHeight="1" ht="14.25">
@@ -9191,7 +9260,7 @@
       <c r="M105" s="108"/>
       <c r="N105" s="108"/>
       <c r="Q105" s="3" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
     </row>
     <row r="106" spans="1:19" customHeight="1" ht="14.25">
@@ -9210,7 +9279,7 @@
       <c r="M106" s="108"/>
       <c r="N106" s="108"/>
       <c r="Q106" s="3" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
     </row>
     <row r="107" spans="1:19" customHeight="1" ht="14.25">
@@ -9229,7 +9298,7 @@
       <c r="M107" s="108"/>
       <c r="N107" s="108"/>
       <c r="Q107" s="3" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
     </row>
     <row r="108" spans="1:19" customHeight="1" ht="14.25">
@@ -9248,7 +9317,7 @@
       <c r="M108" s="108"/>
       <c r="N108" s="108"/>
       <c r="Q108" s="3" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
     </row>
     <row r="109" spans="1:19" customHeight="1" ht="14.25">
@@ -9267,7 +9336,7 @@
       <c r="M109" s="108"/>
       <c r="N109" s="108"/>
       <c r="Q109" s="3" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
     </row>
     <row r="110" spans="1:19" customHeight="1" ht="14.25">
@@ -9286,7 +9355,7 @@
       <c r="M110" s="108"/>
       <c r="N110" s="108"/>
       <c r="Q110" s="3" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
     </row>
     <row r="111" spans="1:19" customHeight="1" ht="14.25">
@@ -9305,7 +9374,7 @@
       <c r="M111" s="108"/>
       <c r="N111" s="108"/>
       <c r="Q111" s="3" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
     </row>
     <row r="112" spans="1:19" customHeight="1" ht="14.25">
@@ -9324,7 +9393,7 @@
       <c r="M112" s="108"/>
       <c r="N112" s="108"/>
       <c r="Q112" s="3" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
     </row>
     <row r="113" spans="1:19" customHeight="1" ht="14.25">
@@ -9343,7 +9412,7 @@
       <c r="M113" s="108"/>
       <c r="N113" s="108"/>
       <c r="Q113" s="3" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
     </row>
     <row r="114" spans="1:19" customHeight="1" ht="14.25">
@@ -9362,7 +9431,7 @@
       <c r="M114" s="108"/>
       <c r="N114" s="108"/>
       <c r="Q114" s="3" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
     </row>
     <row r="115" spans="1:19" customHeight="1" ht="14.25">
@@ -9381,7 +9450,7 @@
       <c r="M115" s="108"/>
       <c r="N115" s="108"/>
       <c r="Q115" s="3" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
     </row>
     <row r="116" spans="1:19" customHeight="1" ht="14.25">
@@ -9400,7 +9469,7 @@
       <c r="M116" s="108"/>
       <c r="N116" s="108"/>
       <c r="Q116" s="3" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
     </row>
     <row r="117" spans="1:19" customHeight="1" ht="14.25">
@@ -9419,7 +9488,7 @@
       <c r="M117" s="108"/>
       <c r="N117" s="108"/>
       <c r="Q117" s="3" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
     </row>
     <row r="118" spans="1:19" customHeight="1" ht="14.25">
@@ -9438,7 +9507,7 @@
       <c r="M118" s="108"/>
       <c r="N118" s="108"/>
       <c r="Q118" s="3" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
     </row>
     <row r="119" spans="1:19" customHeight="1" ht="14.25">
@@ -9457,7 +9526,7 @@
       <c r="M119" s="108"/>
       <c r="N119" s="108"/>
       <c r="Q119" s="3" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
     </row>
     <row r="120" spans="1:19" customHeight="1" ht="14.25">
@@ -9476,7 +9545,7 @@
       <c r="M120" s="108"/>
       <c r="N120" s="108"/>
       <c r="Q120" s="3" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
     </row>
     <row r="121" spans="1:19" customHeight="1" ht="14.25">
@@ -9495,7 +9564,7 @@
       <c r="M121" s="108"/>
       <c r="N121" s="108"/>
       <c r="Q121" s="3" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
     </row>
     <row r="122" spans="1:19" customHeight="1" ht="14.25">
@@ -9514,7 +9583,7 @@
       <c r="M122" s="108"/>
       <c r="N122" s="108"/>
       <c r="Q122" s="3" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
     </row>
     <row r="123" spans="1:19" customHeight="1" ht="14.25">
@@ -9533,7 +9602,7 @@
       <c r="M123" s="108"/>
       <c r="N123" s="108"/>
       <c r="Q123" s="3" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
     </row>
     <row r="124" spans="1:19" customHeight="1" ht="14.25">
@@ -9552,7 +9621,7 @@
       <c r="M124" s="108"/>
       <c r="N124" s="108"/>
       <c r="Q124" s="3" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
     </row>
     <row r="125" spans="1:19" customHeight="1" ht="14.25">
@@ -9571,7 +9640,7 @@
       <c r="M125" s="108"/>
       <c r="N125" s="108"/>
       <c r="Q125" s="3" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
     </row>
     <row r="126" spans="1:19" customHeight="1" ht="14.25">
@@ -9590,7 +9659,7 @@
       <c r="M126" s="108"/>
       <c r="N126" s="108"/>
       <c r="Q126" s="3" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
     </row>
     <row r="127" spans="1:19" customHeight="1" ht="14.25">
@@ -9609,7 +9678,7 @@
       <c r="M127" s="108"/>
       <c r="N127" s="108"/>
       <c r="Q127" s="3" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
     </row>
     <row r="128" spans="1:19" customHeight="1" ht="28.5">
@@ -9628,7 +9697,7 @@
       <c r="M128" s="108"/>
       <c r="N128" s="108"/>
       <c r="Q128" s="3" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
     </row>
     <row r="129" spans="1:19" customHeight="1" ht="14.25">
@@ -9647,7 +9716,7 @@
       <c r="M129" s="108"/>
       <c r="N129" s="108"/>
       <c r="Q129" s="3" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
     </row>
     <row r="130" spans="1:19" customHeight="1" ht="14.25">
@@ -9666,7 +9735,7 @@
       <c r="M130" s="108"/>
       <c r="N130" s="108"/>
       <c r="Q130" s="3" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
     </row>
     <row r="131" spans="1:19" customHeight="1" ht="14.25">
@@ -9685,7 +9754,7 @@
       <c r="M131" s="108"/>
       <c r="N131" s="108"/>
       <c r="Q131" s="3" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
     </row>
     <row r="132" spans="1:19" customHeight="1" ht="14.25">
@@ -9704,7 +9773,7 @@
       <c r="M132" s="108"/>
       <c r="N132" s="108"/>
       <c r="Q132" s="3" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
     </row>
     <row r="133" spans="1:19" customHeight="1" ht="14.25">
@@ -9723,7 +9792,7 @@
       <c r="M133" s="108"/>
       <c r="N133" s="108"/>
       <c r="Q133" s="3" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
     </row>
     <row r="134" spans="1:19" customHeight="1" ht="14.25">
@@ -9742,7 +9811,7 @@
       <c r="M134" s="108"/>
       <c r="N134" s="108"/>
       <c r="Q134" s="3" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
     </row>
     <row r="135" spans="1:19" customHeight="1" ht="14.25">
@@ -9761,7 +9830,7 @@
       <c r="M135" s="108"/>
       <c r="N135" s="108"/>
       <c r="Q135" s="3" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
     </row>
     <row r="136" spans="1:19" customHeight="1" ht="14.25">
@@ -9780,7 +9849,7 @@
       <c r="M136" s="108"/>
       <c r="N136" s="108"/>
       <c r="Q136" s="3" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
     </row>
     <row r="137" spans="1:19" customHeight="1" ht="14.25">
@@ -9799,7 +9868,7 @@
       <c r="M137" s="108"/>
       <c r="N137" s="108"/>
       <c r="Q137" s="3" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
     </row>
     <row r="138" spans="1:19" customHeight="1" ht="14.25">
@@ -9818,7 +9887,7 @@
       <c r="M138" s="108"/>
       <c r="N138" s="108"/>
       <c r="Q138" s="3" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
     </row>
     <row r="139" spans="1:19" customHeight="1" ht="14.25">
@@ -9837,7 +9906,7 @@
       <c r="M139" s="108"/>
       <c r="N139" s="108"/>
       <c r="Q139" s="3" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
     </row>
     <row r="140" spans="1:19" customHeight="1" ht="14.25">
@@ -9856,7 +9925,7 @@
       <c r="M140" s="108"/>
       <c r="N140" s="108"/>
       <c r="Q140" s="3" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
     </row>
     <row r="141" spans="1:19" customHeight="1" ht="14.25">
@@ -9875,7 +9944,7 @@
       <c r="M141" s="108"/>
       <c r="N141" s="108"/>
       <c r="Q141" s="3" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
     </row>
     <row r="142" spans="1:19" customHeight="1" ht="14.25">
@@ -9894,7 +9963,7 @@
       <c r="M142" s="108"/>
       <c r="N142" s="108"/>
       <c r="Q142" s="3" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
     </row>
     <row r="143" spans="1:19" customHeight="1" ht="28.5">
@@ -9913,7 +9982,7 @@
       <c r="M143" s="108"/>
       <c r="N143" s="108"/>
       <c r="Q143" s="3" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
     </row>
     <row r="144" spans="1:19" customHeight="1" ht="14.25">
@@ -9932,7 +10001,7 @@
       <c r="M144" s="108"/>
       <c r="N144" s="108"/>
       <c r="Q144" s="3" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
     </row>
     <row r="145" spans="1:19" customHeight="1" ht="14.25">
@@ -9951,7 +10020,7 @@
       <c r="M145" s="108"/>
       <c r="N145" s="108"/>
       <c r="Q145" s="3" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
     </row>
     <row r="146" spans="1:19" customHeight="1" ht="14.25">
@@ -9970,7 +10039,7 @@
       <c r="M146" s="108"/>
       <c r="N146" s="108"/>
       <c r="Q146" s="3" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
     </row>
     <row r="147" spans="1:19" customHeight="1" ht="14.25">
@@ -9989,7 +10058,7 @@
       <c r="M147" s="108"/>
       <c r="N147" s="108"/>
       <c r="Q147" s="3" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
     </row>
     <row r="148" spans="1:19" customHeight="1" ht="14.25">
@@ -10008,7 +10077,7 @@
       <c r="M148" s="108"/>
       <c r="N148" s="108"/>
       <c r="Q148" s="3" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
     </row>
     <row r="149" spans="1:19" customHeight="1" ht="14.25">
@@ -10027,7 +10096,7 @@
       <c r="M149" s="108"/>
       <c r="N149" s="108"/>
       <c r="Q149" s="3" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
     </row>
     <row r="150" spans="1:19" customHeight="1" ht="14.25">
@@ -10046,7 +10115,7 @@
       <c r="M150" s="108"/>
       <c r="N150" s="108"/>
       <c r="Q150" s="3" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
     </row>
     <row r="151" spans="1:19" customHeight="1" ht="14.25">
@@ -10065,7 +10134,7 @@
       <c r="M151" s="108"/>
       <c r="N151" s="108"/>
       <c r="Q151" s="3" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
     </row>
     <row r="152" spans="1:19" customHeight="1" ht="14.25">
@@ -10084,7 +10153,7 @@
       <c r="M152" s="108"/>
       <c r="N152" s="108"/>
       <c r="Q152" s="3" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="153" spans="1:19" customHeight="1" ht="28.5">
@@ -10103,7 +10172,7 @@
       <c r="M153" s="108"/>
       <c r="N153" s="108"/>
       <c r="Q153" s="3" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
     </row>
     <row r="154" spans="1:19" customHeight="1" ht="14.25">
@@ -10122,7 +10191,7 @@
       <c r="M154" s="108"/>
       <c r="N154" s="108"/>
       <c r="Q154" s="3" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
     </row>
     <row r="155" spans="1:19" customHeight="1" ht="28.5">
@@ -10141,7 +10210,7 @@
       <c r="M155" s="108"/>
       <c r="N155" s="108"/>
       <c r="Q155" s="3" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
     </row>
     <row r="156" spans="1:19" customHeight="1" ht="14.25">
@@ -10160,7 +10229,7 @@
       <c r="M156" s="108"/>
       <c r="N156" s="108"/>
       <c r="Q156" s="3" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
     </row>
     <row r="157" spans="1:19" customHeight="1" ht="14.25">
@@ -10179,7 +10248,7 @@
       <c r="M157" s="108"/>
       <c r="N157" s="108"/>
       <c r="Q157" s="3" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
     </row>
     <row r="158" spans="1:19" customHeight="1" ht="14.25">
@@ -10198,7 +10267,7 @@
       <c r="M158" s="108"/>
       <c r="N158" s="108"/>
       <c r="Q158" s="3" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
     </row>
     <row r="159" spans="1:19" customHeight="1" ht="14.25">
@@ -10217,7 +10286,7 @@
       <c r="M159" s="108"/>
       <c r="N159" s="108"/>
       <c r="Q159" s="3" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
     </row>
     <row r="160" spans="1:19" customHeight="1" ht="14.25">
@@ -10236,7 +10305,7 @@
       <c r="M160" s="108"/>
       <c r="N160" s="108"/>
       <c r="Q160" s="3" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
     </row>
     <row r="161" spans="1:19" customHeight="1" ht="14.25">
@@ -10255,7 +10324,7 @@
       <c r="M161" s="108"/>
       <c r="N161" s="108"/>
       <c r="Q161" s="3" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
     </row>
     <row r="162" spans="1:19" customHeight="1" ht="14.25">
@@ -10274,7 +10343,7 @@
       <c r="M162" s="108"/>
       <c r="N162" s="108"/>
       <c r="Q162" s="3" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
     </row>
     <row r="163" spans="1:19" customHeight="1" ht="14.25">
@@ -10293,7 +10362,7 @@
       <c r="M163" s="108"/>
       <c r="N163" s="108"/>
       <c r="Q163" s="3" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
     </row>
     <row r="164" spans="1:19" customHeight="1" ht="14.25">
@@ -10312,7 +10381,7 @@
       <c r="M164" s="108"/>
       <c r="N164" s="108"/>
       <c r="Q164" s="3" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
     </row>
     <row r="165" spans="1:19" customHeight="1" ht="28.5">
@@ -10331,7 +10400,7 @@
       <c r="M165" s="108"/>
       <c r="N165" s="108"/>
       <c r="Q165" s="3" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
     </row>
     <row r="166" spans="1:19" customHeight="1" ht="14.25">
@@ -10350,7 +10419,7 @@
       <c r="M166" s="108"/>
       <c r="N166" s="108"/>
       <c r="Q166" s="3" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
     </row>
     <row r="167" spans="1:19" customHeight="1" ht="42.75">
@@ -10369,7 +10438,7 @@
       <c r="M167" s="108"/>
       <c r="N167" s="108"/>
       <c r="Q167" s="3" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
     </row>
     <row r="168" spans="1:19" customHeight="1" ht="14.25">
@@ -10388,7 +10457,7 @@
       <c r="M168" s="108"/>
       <c r="N168" s="108"/>
       <c r="Q168" s="3" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
     </row>
     <row r="169" spans="1:19" customHeight="1" ht="14.25">
@@ -10407,7 +10476,7 @@
       <c r="M169" s="108"/>
       <c r="N169" s="108"/>
       <c r="Q169" s="3" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
     </row>
     <row r="170" spans="1:19" customHeight="1" ht="28.5">
@@ -10426,7 +10495,7 @@
       <c r="M170" s="108"/>
       <c r="N170" s="108"/>
       <c r="Q170" s="3" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
     </row>
     <row r="171" spans="1:19" customHeight="1" ht="14.25">
@@ -10445,7 +10514,7 @@
       <c r="M171" s="108"/>
       <c r="N171" s="108"/>
       <c r="Q171" s="3" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
     </row>
     <row r="172" spans="1:19" customHeight="1" ht="14.25">
@@ -10464,7 +10533,7 @@
       <c r="M172" s="108"/>
       <c r="N172" s="108"/>
       <c r="Q172" s="3" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
     </row>
     <row r="173" spans="1:19" customHeight="1" ht="14.25">
@@ -10483,7 +10552,7 @@
       <c r="M173" s="108"/>
       <c r="N173" s="108"/>
       <c r="Q173" s="3" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
     </row>
     <row r="174" spans="1:19" customHeight="1" ht="14.25">
@@ -10502,7 +10571,7 @@
       <c r="M174" s="108"/>
       <c r="N174" s="108"/>
       <c r="Q174" s="3" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
     </row>
     <row r="175" spans="1:19" customHeight="1" ht="14.25">
@@ -10521,7 +10590,7 @@
       <c r="M175" s="108"/>
       <c r="N175" s="108"/>
       <c r="Q175" s="3" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
     </row>
     <row r="176" spans="1:19" customHeight="1" ht="14.25">
@@ -10540,7 +10609,7 @@
       <c r="M176" s="108"/>
       <c r="N176" s="108"/>
       <c r="Q176" s="3" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
     </row>
     <row r="177" spans="1:19" customHeight="1" ht="14.25">
@@ -10559,7 +10628,7 @@
       <c r="M177" s="108"/>
       <c r="N177" s="108"/>
       <c r="Q177" s="3" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
     </row>
     <row r="178" spans="1:19" customHeight="1" ht="14.25">
@@ -10578,7 +10647,7 @@
       <c r="M178" s="108"/>
       <c r="N178" s="108"/>
       <c r="Q178" s="3" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
     </row>
     <row r="179" spans="1:19" customHeight="1" ht="14.25">
@@ -10597,7 +10666,7 @@
       <c r="M179" s="108"/>
       <c r="N179" s="108"/>
       <c r="Q179" s="3" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
     </row>
     <row r="180" spans="1:19" customHeight="1" ht="28.5">
@@ -10616,7 +10685,7 @@
       <c r="M180" s="108"/>
       <c r="N180" s="108"/>
       <c r="Q180" s="3" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
     </row>
     <row r="181" spans="1:19" customHeight="1" ht="14.25">
@@ -10635,7 +10704,7 @@
       <c r="M181" s="108"/>
       <c r="N181" s="108"/>
       <c r="Q181" s="3" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
     </row>
     <row r="182" spans="1:19" customHeight="1" ht="14.25">
@@ -10654,7 +10723,7 @@
       <c r="M182" s="108"/>
       <c r="N182" s="108"/>
       <c r="Q182" s="3" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
     </row>
     <row r="183" spans="1:19" customHeight="1" ht="14.25">
@@ -10673,7 +10742,7 @@
       <c r="M183" s="108"/>
       <c r="N183" s="108"/>
       <c r="Q183" s="3" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
     </row>
     <row r="184" spans="1:19" customHeight="1" ht="14.25">
@@ -10692,7 +10761,7 @@
       <c r="M184" s="108"/>
       <c r="N184" s="108"/>
       <c r="Q184" s="3" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
     </row>
     <row r="185" spans="1:19" customHeight="1" ht="14.25">
@@ -10711,7 +10780,7 @@
       <c r="M185" s="108"/>
       <c r="N185" s="108"/>
       <c r="Q185" s="3" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
     </row>
     <row r="186" spans="1:19" customHeight="1" ht="14.25">
@@ -10730,7 +10799,7 @@
       <c r="M186" s="108"/>
       <c r="N186" s="108"/>
       <c r="Q186" s="3" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
     </row>
     <row r="187" spans="1:19" customHeight="1" ht="14.25">
@@ -10749,7 +10818,7 @@
       <c r="M187" s="108"/>
       <c r="N187" s="108"/>
       <c r="Q187" s="3" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
     </row>
     <row r="188" spans="1:19" customHeight="1" ht="14.25">
@@ -10768,7 +10837,7 @@
       <c r="M188" s="108"/>
       <c r="N188" s="108"/>
       <c r="Q188" s="3" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
     </row>
     <row r="189" spans="1:19" customHeight="1" ht="14.25">
@@ -10787,7 +10856,7 @@
       <c r="M189" s="108"/>
       <c r="N189" s="108"/>
       <c r="Q189" s="3" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
     </row>
     <row r="190" spans="1:19" customHeight="1" ht="14.25">
@@ -10806,7 +10875,7 @@
       <c r="M190" s="108"/>
       <c r="N190" s="108"/>
       <c r="Q190" s="3" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
     </row>
     <row r="191" spans="1:19" customHeight="1" ht="14.25">
@@ -10825,7 +10894,7 @@
       <c r="M191" s="108"/>
       <c r="N191" s="108"/>
       <c r="Q191" s="3" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
     </row>
     <row r="192" spans="1:19" customHeight="1" ht="14.25">
@@ -10844,7 +10913,7 @@
       <c r="M192" s="108"/>
       <c r="N192" s="108"/>
       <c r="Q192" s="3" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
     </row>
     <row r="193" spans="1:19" customHeight="1" ht="14.25">
@@ -10863,7 +10932,7 @@
       <c r="M193" s="108"/>
       <c r="N193" s="108"/>
       <c r="Q193" s="3" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
     </row>
     <row r="194" spans="1:19" customHeight="1" ht="14.25">
@@ -10882,7 +10951,7 @@
       <c r="M194" s="108"/>
       <c r="N194" s="108"/>
       <c r="Q194" s="3" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
     </row>
     <row r="195" spans="1:19" customHeight="1" ht="14.25">
@@ -10901,7 +10970,7 @@
       <c r="M195" s="108"/>
       <c r="N195" s="108"/>
       <c r="Q195" s="3" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
     </row>
     <row r="196" spans="1:19" customHeight="1" ht="14.25">
@@ -10920,7 +10989,7 @@
       <c r="M196" s="108"/>
       <c r="N196" s="108"/>
       <c r="Q196" s="3" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
     </row>
     <row r="197" spans="1:19" customHeight="1" ht="14.25">
@@ -10939,7 +11008,7 @@
       <c r="M197" s="108"/>
       <c r="N197" s="108"/>
       <c r="Q197" s="3" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
     </row>
     <row r="198" spans="1:19" customHeight="1" ht="14.25">
@@ -10958,7 +11027,7 @@
       <c r="M198" s="108"/>
       <c r="N198" s="108"/>
       <c r="Q198" s="3" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
     </row>
     <row r="199" spans="1:19" customHeight="1" ht="14.25">
@@ -10977,7 +11046,7 @@
       <c r="M199" s="108"/>
       <c r="N199" s="108"/>
       <c r="Q199" s="3" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
     </row>
     <row r="200" spans="1:19" customHeight="1" ht="28.5">
@@ -10996,7 +11065,7 @@
       <c r="M200" s="108"/>
       <c r="N200" s="108"/>
       <c r="Q200" s="3" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
     </row>
     <row r="201" spans="1:19" customHeight="1" ht="14.25">
@@ -11015,7 +11084,7 @@
       <c r="M201" s="108"/>
       <c r="N201" s="108"/>
       <c r="Q201" s="3" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
     </row>
     <row r="202" spans="1:19" customHeight="1" ht="14.25">
@@ -11034,7 +11103,7 @@
       <c r="M202" s="108"/>
       <c r="N202" s="108"/>
       <c r="Q202" s="3" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
     </row>
     <row r="203" spans="1:19" customHeight="1" ht="14.25">
@@ -11053,7 +11122,7 @@
       <c r="M203" s="108"/>
       <c r="N203" s="108"/>
       <c r="Q203" s="3" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
     </row>
     <row r="204" spans="1:19" customHeight="1" ht="14.25">
@@ -11072,7 +11141,7 @@
       <c r="M204" s="108"/>
       <c r="N204" s="108"/>
       <c r="Q204" s="3" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
     </row>
     <row r="205" spans="1:19" customHeight="1" ht="14.25">
@@ -11091,7 +11160,7 @@
       <c r="M205" s="108"/>
       <c r="N205" s="108"/>
       <c r="Q205" s="3" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
     </row>
     <row r="206" spans="1:19" customHeight="1" ht="14.25">
@@ -11110,7 +11179,7 @@
       <c r="M206" s="108"/>
       <c r="N206" s="108"/>
       <c r="Q206" s="3" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
     </row>
     <row r="207" spans="1:19" customHeight="1" ht="28.5">
@@ -11129,7 +11198,7 @@
       <c r="M207" s="108"/>
       <c r="N207" s="108"/>
       <c r="Q207" s="3" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
     </row>
     <row r="208" spans="1:19" customHeight="1" ht="28.5">
@@ -11148,7 +11217,7 @@
       <c r="M208" s="108"/>
       <c r="N208" s="108"/>
       <c r="Q208" s="3" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
     </row>
     <row r="209" spans="1:19" customHeight="1" ht="14.25">
@@ -11167,7 +11236,7 @@
       <c r="M209" s="108"/>
       <c r="N209" s="108"/>
       <c r="Q209" s="3" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
     </row>
     <row r="210" spans="1:19" customHeight="1" ht="14.25">
@@ -11186,7 +11255,7 @@
       <c r="M210" s="108"/>
       <c r="N210" s="108"/>
       <c r="Q210" s="3" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
     </row>
     <row r="211" spans="1:19" customHeight="1" ht="14.25">
@@ -11205,7 +11274,7 @@
       <c r="M211" s="108"/>
       <c r="N211" s="108"/>
       <c r="Q211" s="3" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
     </row>
     <row r="212" spans="1:19" customHeight="1" ht="14.25">
@@ -11224,7 +11293,7 @@
       <c r="M212" s="108"/>
       <c r="N212" s="108"/>
       <c r="Q212" s="3" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
     </row>
     <row r="213" spans="1:19" customHeight="1" ht="14.25">
@@ -11243,7 +11312,7 @@
       <c r="M213" s="108"/>
       <c r="N213" s="108"/>
       <c r="Q213" s="3" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
     </row>
     <row r="214" spans="1:19" customHeight="1" ht="14.25">
@@ -11262,7 +11331,7 @@
       <c r="M214" s="108"/>
       <c r="N214" s="108"/>
       <c r="Q214" s="3" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
     </row>
     <row r="215" spans="1:19" customHeight="1" ht="14.25">
@@ -11281,7 +11350,7 @@
       <c r="M215" s="108"/>
       <c r="N215" s="108"/>
       <c r="Q215" s="3" t="s">
-        <v>348</v>
+        <v>335</v>
       </c>
     </row>
     <row r="216" spans="1:19" customHeight="1" ht="14.25">
@@ -11300,7 +11369,7 @@
       <c r="M216" s="108"/>
       <c r="N216" s="108"/>
       <c r="Q216" s="3" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
     </row>
     <row r="217" spans="1:19">
@@ -12482,7 +12551,7 @@
     </row>
     <row r="2" spans="1:14" customHeight="1" ht="18">
       <c r="A2" s="514" t="s">
-        <v>350</v>
+        <v>337</v>
       </c>
       <c r="B2" s="515"/>
       <c r="C2" s="515"/>
@@ -12499,28 +12568,28 @@
     </row>
     <row r="3" spans="1:14" customHeight="1" ht="15">
       <c r="A3" s="140" t="s">
-        <v>351</v>
+        <v>338</v>
       </c>
       <c r="B3" s="507" t="s">
-        <v>352</v>
+        <v>339</v>
       </c>
       <c r="C3" s="507"/>
       <c r="D3" s="507"/>
       <c r="E3" s="508"/>
       <c r="F3" s="512" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="G3" s="509" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
       <c r="H3" s="508"/>
       <c r="I3" s="509" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="J3" s="507"/>
       <c r="K3" s="508"/>
       <c r="L3" s="510" t="s">
-        <v>356</v>
+        <v>343</v>
       </c>
       <c r="M3" s="511"/>
     </row>
@@ -12537,26 +12606,36 @@
       <c r="J4" s="483"/>
       <c r="K4" s="484"/>
       <c r="L4" s="5" t="s">
-        <v>357</v>
+        <v>344</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>358</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:14" customHeight="1" ht="27">
-      <c r="A5" s="493"/>
+      <c r="A5" s="493" t="s">
+        <v>346</v>
+      </c>
       <c r="B5" s="468"/>
       <c r="C5" s="468"/>
       <c r="D5" s="468"/>
       <c r="E5" s="468"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="492"/>
+      <c r="F5" s="16">
+        <v>80</v>
+      </c>
+      <c r="G5" s="492" t="s">
+        <v>347</v>
+      </c>
       <c r="H5" s="492"/>
       <c r="I5" s="496"/>
       <c r="J5" s="496"/>
       <c r="K5" s="496"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="22"/>
+      <c r="L5" s="9">
+        <v>123456</v>
+      </c>
+      <c r="M5" s="22" t="s">
+        <v>348</v>
+      </c>
     </row>
     <row r="6" spans="1:14" customHeight="1" ht="27">
       <c r="A6" s="493"/>
@@ -12650,24 +12729,38 @@
     </row>
     <row r="12" spans="1:14" customHeight="1" ht="12">
       <c r="A12" s="485" t="s">
-        <v>161</v>
+        <v>349</v>
       </c>
       <c r="B12" s="486"/>
-      <c r="C12" s="486"/>
-      <c r="D12" s="486"/>
+      <c r="C12" s="486" t="s">
+        <v>350</v>
+      </c>
+      <c r="D12" s="486" t="s">
+        <v>351</v>
+      </c>
       <c r="E12" s="486"/>
       <c r="F12" s="486"/>
-      <c r="G12" s="486"/>
+      <c r="G12" s="486" t="s">
+        <v>352</v>
+      </c>
       <c r="H12" s="486"/>
       <c r="I12" s="486"/>
-      <c r="J12" s="486"/>
-      <c r="K12" s="486"/>
-      <c r="L12" s="486"/>
-      <c r="M12" s="487"/>
+      <c r="J12" s="486">
+        <v>200000.0</v>
+      </c>
+      <c r="K12" s="486">
+        <v>30</v>
+      </c>
+      <c r="L12" s="486" t="s">
+        <v>353</v>
+      </c>
+      <c r="M12" s="487" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="13" spans="1:14" customHeight="1" ht="18">
       <c r="A13" s="488" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B13" s="489"/>
       <c r="C13" s="489"/>
@@ -12684,7 +12777,7 @@
     </row>
     <row r="14" spans="1:14" customHeight="1" ht="12">
       <c r="A14" s="202" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B14" s="101"/>
       <c r="C14" s="101"/>
@@ -12701,33 +12794,33 @@
     </row>
     <row r="15" spans="1:14" customHeight="1" ht="18">
       <c r="A15" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B15" s="481" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C15" s="482"/>
       <c r="D15" s="494" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="E15" s="481"/>
       <c r="F15" s="482"/>
       <c r="G15" s="494" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="H15" s="481"/>
       <c r="I15" s="482"/>
       <c r="J15" s="498" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="K15" s="519" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="L15" s="473" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="M15" s="517" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="16" spans="1:14" customHeight="1" ht="15">
@@ -12747,11 +12840,11 @@
     </row>
     <row r="17" spans="1:14" customHeight="1" ht="18.75">
       <c r="A17" s="521" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="B17" s="522"/>
       <c r="C17" s="8" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="D17" s="495"/>
       <c r="E17" s="483"/>
@@ -13186,7 +13279,7 @@
     </row>
     <row r="46" spans="1:14" customHeight="1" ht="9.75">
       <c r="A46" s="476" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="B46" s="477"/>
       <c r="C46" s="477"/>
@@ -13203,7 +13296,7 @@
     </row>
     <row r="47" spans="1:14" customHeight="1" ht="27.75">
       <c r="A47" s="445" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="B47" s="446"/>
       <c r="C47" s="447"/>
@@ -13213,7 +13306,7 @@
       <c r="G47" s="502"/>
       <c r="H47" s="503"/>
       <c r="I47" s="228" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="J47" s="229"/>
       <c r="K47" s="230"/>
@@ -13223,7 +13316,7 @@
     </row>
     <row r="48" spans="1:14" customHeight="1" ht="9">
       <c r="A48" s="500" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B48" s="500"/>
       <c r="C48" s="500"/>
@@ -13427,7 +13520,7 @@
     </row>
     <row r="2" spans="1:13" customHeight="1" ht="22.5">
       <c r="A2" s="571" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B2" s="572"/>
       <c r="C2" s="572"/>
@@ -13442,22 +13535,22 @@
     </row>
     <row r="3" spans="1:13" customHeight="1" ht="15">
       <c r="A3" s="555" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B3" s="556" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C3" s="556"/>
       <c r="D3" s="557"/>
       <c r="E3" s="507" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F3" s="508"/>
       <c r="G3" s="576" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="H3" s="509" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="I3" s="566"/>
       <c r="J3" s="566"/>
@@ -13482,10 +13575,10 @@
       <c r="C5" s="574"/>
       <c r="D5" s="575"/>
       <c r="E5" s="27" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="G5" s="520"/>
       <c r="H5" s="570"/>
@@ -13494,14 +13587,24 @@
       <c r="K5" s="432"/>
     </row>
     <row r="6" spans="1:13" customHeight="1" ht="27.75">
-      <c r="A6" s="563"/>
+      <c r="A6" s="563" t="s">
+        <v>372</v>
+      </c>
       <c r="B6" s="564"/>
       <c r="C6" s="564"/>
       <c r="D6" s="565"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="552"/>
+      <c r="E6" s="33" t="s">
+        <v>373</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>374</v>
+      </c>
+      <c r="G6" s="34">
+        <v>50</v>
+      </c>
+      <c r="H6" s="552" t="s">
+        <v>375</v>
+      </c>
       <c r="I6" s="553"/>
       <c r="J6" s="553"/>
       <c r="K6" s="554"/>
@@ -13572,21 +13675,33 @@
       <c r="K11" s="554"/>
     </row>
     <row r="12" spans="1:13" customHeight="1" ht="27.75">
-      <c r="A12" s="560"/>
+      <c r="A12" s="560" t="s">
+        <v>376</v>
+      </c>
       <c r="B12" s="561"/>
       <c r="C12" s="561"/>
       <c r="D12" s="562"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="525"/>
-      <c r="I12" s="526"/>
+      <c r="E12" s="33" t="s">
+        <v>348</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>377</v>
+      </c>
+      <c r="G12" s="35">
+        <v>50</v>
+      </c>
+      <c r="H12" s="525" t="s">
+        <v>378</v>
+      </c>
+      <c r="I12" s="526" t="s">
+        <v>379</v>
+      </c>
       <c r="J12" s="526"/>
       <c r="K12" s="527"/>
     </row>
     <row r="13" spans="1:13" customHeight="1" ht="11.25">
       <c r="A13" s="485" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="B13" s="486"/>
       <c r="C13" s="486"/>
@@ -13601,7 +13716,7 @@
     </row>
     <row r="14" spans="1:13" customHeight="1" ht="18">
       <c r="A14" s="528" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="B14" s="529"/>
       <c r="C14" s="529"/>
@@ -13616,25 +13731,25 @@
     </row>
     <row r="15" spans="1:13" customHeight="1" ht="18">
       <c r="A15" s="543" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="B15" s="481" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="C15" s="549"/>
       <c r="D15" s="550"/>
       <c r="E15" s="481" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="F15" s="482"/>
       <c r="G15" s="519" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="H15" s="498" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="I15" s="494" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="J15" s="549"/>
       <c r="K15" s="569"/>
@@ -13658,10 +13773,10 @@
       <c r="C17" s="431"/>
       <c r="D17" s="551"/>
       <c r="E17" s="27" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="G17" s="520"/>
       <c r="H17" s="499"/>
@@ -13944,7 +14059,7 @@
     </row>
     <row r="39" spans="1:13" customHeight="1" ht="13.5">
       <c r="A39" s="448" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="B39" s="449"/>
       <c r="C39" s="449"/>
@@ -13959,7 +14074,7 @@
     </row>
     <row r="40" spans="1:13" customHeight="1" ht="22.5">
       <c r="A40" s="585" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="B40" s="586"/>
       <c r="C40" s="586"/>
@@ -13974,33 +14089,35 @@
     </row>
     <row r="41" spans="1:13" customHeight="1" ht="33.75">
       <c r="A41" s="141" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="B41" s="146" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="C41" s="142" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="D41" s="577" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="E41" s="577"/>
       <c r="F41" s="577"/>
       <c r="G41" s="577"/>
       <c r="H41" s="578"/>
       <c r="I41" s="142" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="J41" s="577" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="K41" s="584"/>
     </row>
     <row r="42" spans="1:13" customHeight="1" ht="24.75">
       <c r="A42" s="582"/>
       <c r="B42" s="583"/>
-      <c r="C42" s="579"/>
+      <c r="C42" s="579" t="s">
+        <v>393</v>
+      </c>
       <c r="D42" s="580"/>
       <c r="E42" s="580"/>
       <c r="F42" s="580"/>
@@ -14090,7 +14207,7 @@
     </row>
     <row r="49" spans="1:13" customHeight="1" ht="11.25">
       <c r="A49" s="448" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="B49" s="449"/>
       <c r="C49" s="449"/>
@@ -14105,7 +14222,7 @@
     </row>
     <row r="50" spans="1:13" customHeight="1" ht="28.5">
       <c r="A50" s="445" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="B50" s="447"/>
       <c r="C50" s="501"/>
@@ -14113,7 +14230,7 @@
       <c r="E50" s="502"/>
       <c r="F50" s="503"/>
       <c r="G50" s="588" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="H50" s="589"/>
       <c r="I50" s="501"/>
@@ -14124,7 +14241,7 @@
     </row>
     <row r="51" spans="1:13" customHeight="1" ht="9.75">
       <c r="K51" s="236" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
     </row>
     <row r="52" spans="1:13" customHeight="1" ht="3"/>
@@ -14294,11 +14411,11 @@
     </row>
     <row r="2" spans="1:14" customHeight="1" ht="13.5">
       <c r="A2" s="624" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="B2" s="625"/>
       <c r="C2" s="603" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="D2" s="603"/>
       <c r="E2" s="603"/>
@@ -14315,7 +14432,7 @@
       <c r="A3" s="39"/>
       <c r="B3" s="40"/>
       <c r="C3" s="607" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="D3" s="607"/>
       <c r="E3" s="607"/>
@@ -14332,7 +14449,7 @@
       <c r="A4" s="39"/>
       <c r="B4" s="40"/>
       <c r="C4" s="607" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="D4" s="607"/>
       <c r="E4" s="607"/>
@@ -14358,12 +14475,14 @@
       <c r="A6" s="39"/>
       <c r="B6" s="40"/>
       <c r="C6" s="607" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="D6" s="607"/>
       <c r="E6" s="607"/>
       <c r="F6" s="608"/>
-      <c r="G6" s="629"/>
+      <c r="G6" s="629" t="s">
+        <v>400</v>
+      </c>
       <c r="H6" s="630"/>
       <c r="I6" s="630"/>
       <c r="J6" s="630"/>
@@ -14390,12 +14509,14 @@
       <c r="A8" s="39"/>
       <c r="B8" s="40"/>
       <c r="C8" s="607" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="D8" s="607"/>
       <c r="E8" s="607"/>
       <c r="F8" s="608"/>
-      <c r="G8" s="632"/>
+      <c r="G8" s="632" t="s">
+        <v>400</v>
+      </c>
       <c r="H8" s="633"/>
       <c r="I8" s="633"/>
       <c r="J8" s="633"/>
@@ -14420,7 +14541,7 @@
       <c r="E10" s="607"/>
       <c r="F10" s="608"/>
       <c r="G10" s="592" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="H10" s="592"/>
       <c r="I10" s="592"/>
@@ -14461,16 +14582,18 @@
     </row>
     <row r="13" spans="1:14" customHeight="1" ht="18">
       <c r="A13" s="622" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="B13" s="623"/>
       <c r="C13" s="590" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="D13" s="590"/>
       <c r="E13" s="549"/>
       <c r="F13" s="550"/>
-      <c r="G13" s="594"/>
+      <c r="G13" s="594" t="s">
+        <v>400</v>
+      </c>
       <c r="H13" s="595"/>
       <c r="I13" s="595"/>
       <c r="J13" s="595"/>
@@ -14486,7 +14609,7 @@
       <c r="E14" s="549"/>
       <c r="F14" s="550"/>
       <c r="G14" s="591" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="H14" s="592"/>
       <c r="I14" s="592"/>
@@ -14544,12 +14667,14 @@
       <c r="A18" s="51"/>
       <c r="B18" s="52"/>
       <c r="C18" s="737" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="D18" s="737"/>
       <c r="E18" s="738"/>
       <c r="F18" s="739"/>
-      <c r="G18" s="728"/>
+      <c r="G18" s="728" t="s">
+        <v>400</v>
+      </c>
       <c r="H18" s="729"/>
       <c r="I18" s="729"/>
       <c r="J18" s="729"/>
@@ -14565,7 +14690,7 @@
       <c r="E19" s="738"/>
       <c r="F19" s="739"/>
       <c r="G19" s="591" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="H19" s="592"/>
       <c r="I19" s="592"/>
@@ -14583,7 +14708,7 @@
       <c r="F20" s="739"/>
       <c r="G20" s="56"/>
       <c r="H20" s="733" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="I20" s="733"/>
       <c r="J20" s="246"/>
@@ -14599,7 +14724,7 @@
       <c r="E21" s="738"/>
       <c r="F21" s="739"/>
       <c r="G21" s="734" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="H21" s="735"/>
       <c r="I21" s="735"/>
@@ -14616,7 +14741,7 @@
       <c r="E22" s="740"/>
       <c r="F22" s="741"/>
       <c r="G22" s="125" t="s">
-        <v>402</v>
+        <v>408</v>
       </c>
       <c r="H22" s="237"/>
       <c r="I22" s="685"/>
@@ -14627,16 +14752,18 @@
     </row>
     <row r="23" spans="1:14" customHeight="1" ht="18">
       <c r="A23" s="636" t="s">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="B23" s="637"/>
       <c r="C23" s="618" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
       <c r="D23" s="618"/>
       <c r="E23" s="618"/>
       <c r="F23" s="619"/>
-      <c r="G23" s="594"/>
+      <c r="G23" s="594" t="s">
+        <v>400</v>
+      </c>
       <c r="H23" s="595"/>
       <c r="I23" s="595"/>
       <c r="J23" s="595"/>
@@ -14652,7 +14779,7 @@
       <c r="E24" s="610"/>
       <c r="F24" s="609"/>
       <c r="G24" s="591" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="H24" s="592"/>
       <c r="I24" s="592"/>
@@ -14693,16 +14820,18 @@
     </row>
     <row r="27" spans="1:14" customHeight="1" ht="14.25">
       <c r="A27" s="636" t="s">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="B27" s="637"/>
       <c r="C27" s="618" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="D27" s="618"/>
       <c r="E27" s="618"/>
       <c r="F27" s="619"/>
-      <c r="G27" s="594"/>
+      <c r="G27" s="594" t="s">
+        <v>400</v>
+      </c>
       <c r="H27" s="595"/>
       <c r="I27" s="595"/>
       <c r="J27" s="595"/>
@@ -14718,7 +14847,7 @@
       <c r="E28" s="610"/>
       <c r="F28" s="609"/>
       <c r="G28" s="591" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="H28" s="592"/>
       <c r="I28" s="592"/>
@@ -14758,16 +14887,18 @@
     </row>
     <row r="31" spans="1:14" customHeight="1" ht="18">
       <c r="A31" s="636" t="s">
-        <v>407</v>
+        <v>413</v>
       </c>
       <c r="B31" s="637"/>
       <c r="C31" s="618" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="D31" s="618"/>
       <c r="E31" s="618"/>
       <c r="F31" s="619"/>
-      <c r="G31" s="594"/>
+      <c r="G31" s="594" t="s">
+        <v>400</v>
+      </c>
       <c r="H31" s="595"/>
       <c r="I31" s="595"/>
       <c r="J31" s="595"/>
@@ -14783,7 +14914,7 @@
       <c r="E32" s="610"/>
       <c r="F32" s="609"/>
       <c r="G32" s="672" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="H32" s="673"/>
       <c r="I32" s="673"/>
@@ -14811,12 +14942,14 @@
       <c r="A34" s="49"/>
       <c r="B34" s="50"/>
       <c r="C34" s="610" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="D34" s="610"/>
       <c r="E34" s="610"/>
       <c r="F34" s="609"/>
-      <c r="G34" s="674"/>
+      <c r="G34" s="674" t="s">
+        <v>400</v>
+      </c>
       <c r="H34" s="675"/>
       <c r="I34" s="675"/>
       <c r="J34" s="675"/>
@@ -14832,7 +14965,7 @@
       <c r="E35" s="610"/>
       <c r="F35" s="609"/>
       <c r="G35" s="672" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="H35" s="673"/>
       <c r="I35" s="673"/>
@@ -14857,16 +14990,18 @@
     </row>
     <row r="37" spans="1:14" customHeight="1" ht="18">
       <c r="A37" s="636" t="s">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c r="B37" s="637"/>
       <c r="C37" s="613" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="D37" s="613"/>
       <c r="E37" s="613"/>
       <c r="F37" s="614"/>
-      <c r="G37" s="594"/>
+      <c r="G37" s="594" t="s">
+        <v>400</v>
+      </c>
       <c r="H37" s="595"/>
       <c r="I37" s="595"/>
       <c r="J37" s="595"/>
@@ -14882,7 +15017,7 @@
       <c r="E38" s="590"/>
       <c r="F38" s="615"/>
       <c r="G38" s="591" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="H38" s="592"/>
       <c r="I38" s="592"/>
@@ -14923,11 +15058,11 @@
     </row>
     <row r="41" spans="1:14" customHeight="1" ht="28.5">
       <c r="A41" s="611" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="B41" s="612"/>
       <c r="C41" s="610" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="D41" s="610"/>
       <c r="E41" s="610"/>
@@ -14957,16 +15092,18 @@
     </row>
     <row r="43" spans="1:14" customHeight="1" ht="13.5">
       <c r="A43" s="64" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="B43" s="65"/>
       <c r="C43" s="610" t="s">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="D43" s="610"/>
       <c r="E43" s="610"/>
       <c r="F43" s="609"/>
-      <c r="G43" s="632"/>
+      <c r="G43" s="632" t="s">
+        <v>400</v>
+      </c>
       <c r="H43" s="633"/>
       <c r="I43" s="633"/>
       <c r="J43" s="633"/>
@@ -14982,7 +15119,7 @@
       <c r="E44" s="610"/>
       <c r="F44" s="609"/>
       <c r="G44" s="187" t="s">
-        <v>418</v>
+        <v>424</v>
       </c>
       <c r="H44" s="239"/>
       <c r="I44" s="118"/>
@@ -14993,16 +15130,18 @@
     </row>
     <row r="45" spans="1:14" customHeight="1" ht="13.5">
       <c r="A45" s="64" t="s">
-        <v>419</v>
+        <v>425</v>
       </c>
       <c r="B45" s="65"/>
       <c r="C45" s="609" t="s">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="D45" s="609"/>
       <c r="E45" s="609"/>
       <c r="F45" s="609"/>
-      <c r="G45" s="632"/>
+      <c r="G45" s="632" t="s">
+        <v>400</v>
+      </c>
       <c r="H45" s="633"/>
       <c r="I45" s="633"/>
       <c r="J45" s="633"/>
@@ -15018,7 +15157,7 @@
       <c r="E46" s="609"/>
       <c r="F46" s="609"/>
       <c r="G46" s="188" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="H46" s="240"/>
       <c r="I46" s="118"/>
@@ -15030,16 +15169,18 @@
     </row>
     <row r="47" spans="1:14" customHeight="1" ht="13.5">
       <c r="A47" s="64" t="s">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="B47" s="65"/>
       <c r="C47" s="610" t="s">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="D47" s="610"/>
       <c r="E47" s="115"/>
       <c r="F47" s="116"/>
-      <c r="G47" s="632"/>
+      <c r="G47" s="632" t="s">
+        <v>400</v>
+      </c>
       <c r="H47" s="633"/>
       <c r="I47" s="633"/>
       <c r="J47" s="633"/>
@@ -15055,7 +15196,7 @@
       <c r="E48" s="652"/>
       <c r="F48" s="653"/>
       <c r="G48" s="189" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="H48" s="241"/>
       <c r="I48" s="120"/>
@@ -15083,11 +15224,11 @@
     </row>
     <row r="50" spans="1:14" customHeight="1" ht="23.25">
       <c r="A50" s="725" t="s">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="B50" s="726"/>
       <c r="C50" s="185" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="D50" s="185"/>
       <c r="E50" s="185"/>
@@ -15102,17 +15243,17 @@
     </row>
     <row r="51" spans="1:14" customHeight="1" ht="18">
       <c r="A51" s="648" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="B51" s="649"/>
       <c r="C51" s="649"/>
       <c r="D51" s="649"/>
       <c r="E51" s="650"/>
       <c r="F51" s="177" t="s">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="G51" s="657" t="s">
-        <v>428</v>
+        <v>434</v>
       </c>
       <c r="H51" s="577"/>
       <c r="I51" s="584"/>
@@ -15122,13 +15263,19 @@
       <c r="M51" s="644"/>
     </row>
     <row r="52" spans="1:14" customHeight="1" ht="24">
-      <c r="A52" s="665"/>
+      <c r="A52" s="665" t="s">
+        <v>435</v>
+      </c>
       <c r="B52" s="666"/>
       <c r="C52" s="668"/>
       <c r="D52" s="668"/>
       <c r="E52" s="669"/>
-      <c r="F52" s="72"/>
-      <c r="G52" s="658"/>
+      <c r="F52" s="72" t="s">
+        <v>436</v>
+      </c>
+      <c r="G52" s="658" t="s">
+        <v>437</v>
+      </c>
       <c r="H52" s="659"/>
       <c r="I52" s="660"/>
       <c r="J52" s="642"/>
@@ -15137,13 +15284,19 @@
       <c r="M52" s="644"/>
     </row>
     <row r="53" spans="1:14" customHeight="1" ht="24">
-      <c r="A53" s="665"/>
+      <c r="A53" s="665" t="s">
+        <v>438</v>
+      </c>
       <c r="B53" s="666"/>
       <c r="C53" s="666"/>
       <c r="D53" s="666"/>
       <c r="E53" s="667"/>
-      <c r="F53" s="72"/>
-      <c r="G53" s="658"/>
+      <c r="F53" s="72" t="s">
+        <v>439</v>
+      </c>
+      <c r="G53" s="658" t="s">
+        <v>440</v>
+      </c>
       <c r="H53" s="659"/>
       <c r="I53" s="660"/>
       <c r="J53" s="642"/>
@@ -15152,13 +15305,19 @@
       <c r="M53" s="644"/>
     </row>
     <row r="54" spans="1:14" customHeight="1" ht="24">
-      <c r="A54" s="661"/>
+      <c r="A54" s="661" t="s">
+        <v>441</v>
+      </c>
       <c r="B54" s="662"/>
       <c r="C54" s="663"/>
       <c r="D54" s="663"/>
       <c r="E54" s="664"/>
-      <c r="F54" s="193"/>
-      <c r="G54" s="645"/>
+      <c r="F54" s="193" t="s">
+        <v>442</v>
+      </c>
+      <c r="G54" s="645" t="s">
+        <v>443</v>
+      </c>
       <c r="H54" s="646"/>
       <c r="I54" s="647"/>
       <c r="J54" s="642"/>
@@ -15168,11 +15327,11 @@
     </row>
     <row r="55" spans="1:14" customHeight="1" ht="39.75">
       <c r="A55" s="624" t="s">
-        <v>429</v>
+        <v>444</v>
       </c>
       <c r="B55" s="625"/>
       <c r="C55" s="670" t="s">
-        <v>430</v>
+        <v>445</v>
       </c>
       <c r="D55" s="670"/>
       <c r="E55" s="670"/>
@@ -15197,7 +15356,7 @@
       <c r="I56" s="243"/>
       <c r="J56" s="192"/>
       <c r="K56" s="605" t="s">
-        <v>431</v>
+        <v>446</v>
       </c>
       <c r="L56" s="605"/>
       <c r="M56" s="176"/>
@@ -15247,7 +15406,7 @@
     <row r="60" spans="1:14" customHeight="1" ht="25.5">
       <c r="A60" s="75"/>
       <c r="B60" s="677" t="s">
-        <v>432</v>
+        <v>447</v>
       </c>
       <c r="C60" s="678"/>
       <c r="D60" s="679"/>
@@ -15262,10 +15421,12 @@
     <row r="61" spans="1:14" customHeight="1" ht="20.25">
       <c r="A61" s="75"/>
       <c r="B61" s="712" t="s">
-        <v>433</v>
+        <v>448</v>
       </c>
       <c r="C61" s="713"/>
-      <c r="D61" s="131"/>
+      <c r="D61" s="131" t="s">
+        <v>449</v>
+      </c>
       <c r="F61" s="719"/>
       <c r="G61" s="720"/>
       <c r="H61" s="720"/>
@@ -15277,10 +15438,12 @@
     <row r="62" spans="1:14" customHeight="1" ht="9">
       <c r="A62" s="75"/>
       <c r="B62" s="701" t="s">
-        <v>434</v>
+        <v>450</v>
       </c>
       <c r="C62" s="702"/>
-      <c r="D62" s="680"/>
+      <c r="D62" s="680">
+        <v>123123</v>
+      </c>
       <c r="F62" s="722"/>
       <c r="G62" s="723"/>
       <c r="H62" s="723"/>
@@ -15295,7 +15458,7 @@
       <c r="C63" s="715"/>
       <c r="D63" s="681"/>
       <c r="F63" s="682" t="s">
-        <v>435</v>
+        <v>451</v>
       </c>
       <c r="G63" s="683"/>
       <c r="H63" s="683"/>
@@ -15307,10 +15470,12 @@
     <row r="64" spans="1:14" customHeight="1" ht="10.5">
       <c r="A64" s="75"/>
       <c r="B64" s="701" t="s">
-        <v>436</v>
+        <v>452</v>
       </c>
       <c r="C64" s="702"/>
-      <c r="D64" s="680"/>
+      <c r="D64" s="680" t="s">
+        <v>453</v>
+      </c>
       <c r="F64" s="77"/>
       <c r="G64" s="178"/>
       <c r="H64" s="178"/>
@@ -15326,14 +15491,14 @@
       <c r="C65" s="704"/>
       <c r="D65" s="705"/>
       <c r="F65" s="698" t="s">
-        <v>437</v>
+        <v>454</v>
       </c>
       <c r="G65" s="699"/>
       <c r="H65" s="699"/>
       <c r="I65" s="700"/>
       <c r="J65" s="78"/>
       <c r="K65" s="696" t="s">
-        <v>438</v>
+        <v>455</v>
       </c>
       <c r="L65" s="697"/>
       <c r="M65" s="76"/>
@@ -15355,7 +15520,7 @@
     </row>
     <row r="67" spans="1:14" customHeight="1" ht="28.5">
       <c r="A67" s="693" t="s">
-        <v>439</v>
+        <v>456</v>
       </c>
       <c r="B67" s="694"/>
       <c r="C67" s="694"/>
@@ -15390,7 +15555,7 @@
       <c r="C69" s="227"/>
       <c r="D69" s="227"/>
       <c r="E69" s="687" t="s">
-        <v>440</v>
+        <v>457</v>
       </c>
       <c r="F69" s="688"/>
       <c r="G69" s="688"/>
@@ -15418,7 +15583,7 @@
     </row>
     <row r="71" spans="1:14" customHeight="1" ht="10.5">
       <c r="A71" s="686" t="s">
-        <v>441</v>
+        <v>458</v>
       </c>
       <c r="B71" s="686"/>
       <c r="C71" s="686"/>
@@ -15597,35 +15762,35 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>442</v>
+        <v>459</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>443</v>
+        <v>460</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>444</v>
+        <v>461</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>445</v>
+        <v>462</v>
       </c>
       <c r="B2" t="s">
-        <v>446</v>
+        <v>463</v>
       </c>
       <c r="C2" t="s">
-        <v>447</v>
+        <v>464</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>448</v>
+        <v>465</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>449</v>
+        <v>466</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -15635,7 +15800,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="B5" t="s">
-        <v>450</v>
+        <v>467</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added feature in RNR for date awarded, fix bugs on idp, roles and permission
</commit_message>
<xml_diff>
--- a/storage/PDS.xlsx
+++ b/storage/PDS.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="404">
   <si>
     <t xml:space="preserve">        </t>
   </si>
@@ -102,15 +102,9 @@
     <t>SURNAME</t>
   </si>
   <si>
-    <t>JOHNS</t>
-  </si>
-  <si>
     <t>FIRST NAME</t>
   </si>
   <si>
-    <t>ELDORA</t>
-  </si>
-  <si>
     <t xml:space="preserve">NAME EXTENSION (JR., SR)                                           </t>
   </si>
   <si>
@@ -121,9 +115,6 @@
   </si>
   <si>
     <t>MIDDLE NAME</t>
-  </si>
-  <si>
-    <t>CRONIN</t>
   </si>
   <si>
     <t>Widow/er</t>
@@ -139,15 +130,9 @@
 (mm/dd/yyyy)  </t>
   </si>
   <si>
-    <t>02-02-2000</t>
-  </si>
-  <si>
     <t>16. CITIZENSHIP</t>
   </si>
   <si>
-    <t>Filipino</t>
-  </si>
-  <si>
     <t>Separated</t>
   </si>
   <si>
@@ -160,9 +145,6 @@
     <t>PLACE OF BIRTH</t>
   </si>
   <si>
-    <t>TUGUEGARAO CITY</t>
-  </si>
-  <si>
     <t xml:space="preserve">If holder of  dual citizenship, </t>
   </si>
   <si>
@@ -178,9 +160,6 @@
     <t>SEX</t>
   </si>
   <si>
-    <t>MALE</t>
-  </si>
-  <si>
     <t>please indicate the details.</t>
   </si>
   <si>
@@ -193,15 +172,9 @@
     <t>CIVIL STATUS</t>
   </si>
   <si>
-    <t xml:space="preserve">Others: </t>
-  </si>
-  <si>
     <t>17. RESIDENTIAL ADDRESS</t>
   </si>
   <si>
-    <t>ASDF</t>
-  </si>
-  <si>
     <t>Angola</t>
   </si>
   <si>
@@ -214,12 +187,6 @@
     <t>Antigua and Barbuda</t>
   </si>
   <si>
-    <t>SUBDIVISION</t>
-  </si>
-  <si>
-    <t>ATULAYAN</t>
-  </si>
-  <si>
     <t>Argentina</t>
   </si>
   <si>
@@ -241,12 +208,6 @@
     <t>HEIGHT (m)</t>
   </si>
   <si>
-    <t>TUGUEGARAO</t>
-  </si>
-  <si>
-    <t>CAGAYAN</t>
-  </si>
-  <si>
     <t>Australia</t>
   </si>
   <si>
@@ -277,9 +238,6 @@
     <t>BLOOD TYPE</t>
   </si>
   <si>
-    <t>O</t>
-  </si>
-  <si>
     <t>18. PERMANENT ADDRESS</t>
   </si>
   <si>
@@ -349,9 +307,6 @@
     <t>21. E-MAIL ADDRESS (if any)</t>
   </si>
   <si>
-    <t>JESTERADDURU@GMAIL.COM</t>
-  </si>
-  <si>
     <t>Bolivia</t>
   </si>
   <si>
@@ -367,9 +322,6 @@
     <t>SPOUSE'S SURNAME</t>
   </si>
   <si>
-    <t>DUCIMUS FUGA POSSI</t>
-  </si>
-  <si>
     <t>23. NAME of CHILDREN  (Write full name and list all)</t>
   </si>
   <si>
@@ -382,60 +334,39 @@
     <t xml:space="preserve">  FIRST NAME</t>
   </si>
   <si>
-    <t>EXPEDITA REICIENDIS</t>
-  </si>
-  <si>
     <t xml:space="preserve">NAME EXTENSION (JR., SR)                                     </t>
   </si>
   <si>
-    <t>QUASI REICIENDIS SIM</t>
-  </si>
-  <si>
     <t>Brazil</t>
   </si>
   <si>
     <t xml:space="preserve">  MIDDLE NAME</t>
   </si>
   <si>
-    <t>MOLESTIAE QUI QUI AU</t>
-  </si>
-  <si>
     <t>Brunei </t>
   </si>
   <si>
     <t>OCCUPATION</t>
   </si>
   <si>
-    <t>DOLOR EXPEDITA ET FA</t>
-  </si>
-  <si>
     <t>Bulgaria</t>
   </si>
   <si>
     <t>EMPLOYER/BUSINESS NAME</t>
   </si>
   <si>
-    <t>SINT QUAE SUNT QUIS</t>
-  </si>
-  <si>
     <t>Burkina Faso</t>
   </si>
   <si>
     <t>BUSINESS ADDRESS</t>
   </si>
   <si>
-    <t>RATIONE HARUM SUNT</t>
-  </si>
-  <si>
     <t>Burma</t>
   </si>
   <si>
     <t>TELEPHONE NO.</t>
   </si>
   <si>
-    <t>MODI EIUS UT LABORIO</t>
-  </si>
-  <si>
     <t>Burundi</t>
   </si>
   <si>
@@ -445,27 +376,15 @@
     <t>FATHER'S SURNAME</t>
   </si>
   <si>
-    <t>OFFICIA CORPORIS AUT</t>
-  </si>
-  <si>
     <t>Cambodia</t>
   </si>
   <si>
-    <t>ET ODIT CONSEQUUNTUR</t>
-  </si>
-  <si>
     <t xml:space="preserve">NAME EXTENSION (JR., SR)                                                  </t>
   </si>
   <si>
-    <t>OFFICIA VENIAM ULLA</t>
-  </si>
-  <si>
     <t>Cameroon</t>
   </si>
   <si>
-    <t>IURE PLACEAT LABORE</t>
-  </si>
-  <si>
     <t>Canada</t>
   </si>
   <si>
@@ -478,19 +397,10 @@
     <t>Cape Verde</t>
   </si>
   <si>
-    <t>PROIDENT SIT EIUS N</t>
-  </si>
-  <si>
     <t>Central African Republic</t>
   </si>
   <si>
-    <t>EARUM ET CORPORIS EA</t>
-  </si>
-  <si>
     <t>Chad</t>
-  </si>
-  <si>
-    <t>CONSEQUUNTUR OFFICIA</t>
   </si>
   <si>
     <t>(Continue on separate sheet if necessary)</t>
@@ -551,31 +461,16 @@
     <t>ELEMENTARY</t>
   </si>
   <si>
-    <t>TEST SCHOOL</t>
-  </si>
-  <si>
     <t>Congo, Republic of the</t>
   </si>
   <si>
     <t>SECONDARY</t>
   </si>
   <si>
-    <t>TEST HIGH SCHOOL</t>
-  </si>
-  <si>
-    <t>HIGH SCHOOL</t>
-  </si>
-  <si>
     <t>Costa Rica</t>
   </si>
   <si>
     <t>VOCATIONAL /                                                                                                                                                                                                        TRADE COURSE</t>
-  </si>
-  <si>
-    <t>TEST UNIVERSITY</t>
-  </si>
-  <si>
-    <t>BSIT</t>
   </si>
   <si>
     <t>Cote d'Ivoire</t>
@@ -1105,33 +1000,6 @@
 Validity</t>
   </si>
   <si>
-    <t>CS PROF</t>
-  </si>
-  <si>
-    <t>12/12/2012</t>
-  </si>
-  <si>
-    <t>12/31/2024</t>
-  </si>
-  <si>
-    <t>03/01/2020</t>
-  </si>
-  <si>
-    <t>TO PRESENT</t>
-  </si>
-  <si>
-    <t>ECONOMIC DEVELOPMENT SPECIALIST I</t>
-  </si>
-  <si>
-    <t>NEDA</t>
-  </si>
-  <si>
-    <t>PERMANENT</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t xml:space="preserve">V.  WORK EXPERIENCE </t>
   </si>
   <si>
@@ -1181,30 +1049,6 @@
   </si>
   <si>
     <t>POSITION / NATURE OF WORK</t>
-  </si>
-  <si>
-    <t>TEST ORG</t>
-  </si>
-  <si>
-    <t>12/31/2018</t>
-  </si>
-  <si>
-    <t>12/31/2021</t>
-  </si>
-  <si>
-    <t>POSITION</t>
-  </si>
-  <si>
-    <t>TEST TRAINING</t>
-  </si>
-  <si>
-    <t>07/29/2024</t>
-  </si>
-  <si>
-    <t>TECHNICAL</t>
-  </si>
-  <si>
-    <t>DICT</t>
   </si>
   <si>
     <t>VII.  LEARNING AND DEVELOPMENT (L&amp;D) INTERVENTIONS/TRAINING PROGRAMS ATTENDED</t>
@@ -1248,7 +1092,7 @@
     <t>MEMBERSHIP IN ASSOCIATION/ORGANIZATION                                                                                         (Write in full)</t>
   </si>
   <si>
-    <t>GAWAD NG DIREKTOR</t>
+    <t>GAWAD NG DIREKTOR (TECHNICAL)</t>
   </si>
   <si>
     <t xml:space="preserve"> CS FORM 212 (Revised 2017), Page 3 of 4</t>
@@ -1267,9 +1111,6 @@
   </si>
   <si>
     <t>a. within the third degree?</t>
-  </si>
-  <si>
-    <t>NO</t>
   </si>
   <si>
     <t>b. within the fourth degree (for Local Government Unit - Career Employees)?</t>
@@ -1404,33 +1245,6 @@
     <t>TEL. NO.</t>
   </si>
   <si>
-    <t>RIA COOK</t>
-  </si>
-  <si>
-    <t>CHESTER ADKINS</t>
-  </si>
-  <si>
-    <t>DEXTER POPE</t>
-  </si>
-  <si>
-    <t>WARREN SINGLETON</t>
-  </si>
-  <si>
-    <t>HEDWIG GENTRY</t>
-  </si>
-  <si>
-    <t>QUINTESSA HOWARD</t>
-  </si>
-  <si>
-    <t>RAYA GILMORE</t>
-  </si>
-  <si>
-    <t>CAILIN HARRIS</t>
-  </si>
-  <si>
-    <t>ECHO KIRKLAND</t>
-  </si>
-  <si>
     <t>42.</t>
   </si>
   <si>
@@ -1505,9 +1319,6 @@
     <t xml:space="preserve">Government Issued ID: </t>
   </si>
   <si>
-    <t>MATTHEW SHARPE</t>
-  </si>
-  <si>
     <t xml:space="preserve">ID/License/Passport No.: </t>
   </si>
   <si>
@@ -1515,9 +1326,6 @@
   </si>
   <si>
     <t>Date/Place of Issuance:</t>
-  </si>
-  <si>
-    <t>DECEMBER 25, 2023</t>
   </si>
   <si>
     <t>Date Accomplished</t>
@@ -7129,9 +6937,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="380"/>
-      <c r="D10" s="385" t="s">
-        <v>13</v>
-      </c>
+      <c r="D10" s="385"/>
       <c r="E10" s="385"/>
       <c r="F10" s="385"/>
       <c r="G10" s="385"/>
@@ -7147,12 +6953,10 @@
     <row r="11" spans="1:19" customHeight="1" ht="22.5">
       <c r="A11" s="163"/>
       <c r="B11" s="396" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="397"/>
-      <c r="D11" s="197" t="s">
-        <v>15</v>
-      </c>
+      <c r="D11" s="197"/>
       <c r="E11" s="198"/>
       <c r="F11" s="198"/>
       <c r="G11" s="198"/>
@@ -7161,26 +6965,24 @@
       <c r="J11" s="198"/>
       <c r="K11" s="198"/>
       <c r="L11" s="365" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M11" s="366"/>
       <c r="N11" s="252"/>
       <c r="P11" s="96" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="Q11" s="143" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:19" customHeight="1" ht="21.75">
       <c r="A12" s="164"/>
       <c r="B12" s="398" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C12" s="399"/>
-      <c r="D12" s="194" t="s">
-        <v>20</v>
-      </c>
+      <c r="D12" s="194"/>
       <c r="E12" s="195"/>
       <c r="F12" s="195"/>
       <c r="G12" s="195"/>
@@ -7192,42 +6994,38 @@
       <c r="M12" s="199"/>
       <c r="N12" s="200"/>
       <c r="P12" s="96" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:19" customHeight="1" ht="24">
       <c r="A13" s="226" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B13" s="379" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C13" s="380"/>
-      <c r="D13" s="268" t="s">
-        <v>25</v>
-      </c>
+      <c r="D13" s="268"/>
       <c r="E13" s="268"/>
       <c r="F13" s="269"/>
       <c r="G13" s="102" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H13" s="145"/>
       <c r="I13" s="145"/>
-      <c r="J13" s="359" t="s">
-        <v>27</v>
-      </c>
+      <c r="J13" s="359"/>
       <c r="K13" s="360"/>
       <c r="L13" s="360"/>
       <c r="M13" s="360"/>
       <c r="N13" s="361"/>
       <c r="P13" s="96" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:19" customHeight="1" ht="12">
@@ -7250,19 +7048,17 @@
     </row>
     <row r="15" spans="1:19" customHeight="1" ht="24.75">
       <c r="A15" s="165" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B15" s="97" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C15" s="97"/>
-      <c r="D15" s="371" t="s">
-        <v>32</v>
-      </c>
+      <c r="D15" s="371"/>
       <c r="E15" s="371"/>
       <c r="F15" s="372"/>
       <c r="G15" s="273" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="H15" s="274"/>
       <c r="I15" s="274"/>
@@ -7272,27 +7068,25 @@
       <c r="M15" s="284"/>
       <c r="N15" s="285"/>
       <c r="P15" s="96" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:19" customHeight="1" ht="24.75">
       <c r="A16" s="166" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B16" s="97" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C16" s="98"/>
-      <c r="D16" s="387" t="s">
-        <v>38</v>
-      </c>
+      <c r="D16" s="387"/>
       <c r="E16" s="387"/>
       <c r="F16" s="320"/>
       <c r="G16" s="270" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H16" s="271"/>
       <c r="I16" s="272"/>
@@ -7302,10 +7096,10 @@
       <c r="M16" s="287"/>
       <c r="N16" s="288"/>
       <c r="P16" s="96" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:19" customHeight="1" ht="15.75">
@@ -7313,30 +7107,24 @@
         <v>6</v>
       </c>
       <c r="B17" s="279" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C17" s="280"/>
-      <c r="D17" s="277" t="s">
-        <v>43</v>
-      </c>
+      <c r="D17" s="277"/>
       <c r="E17" s="277"/>
       <c r="F17" s="277"/>
       <c r="G17" s="103" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H17" s="104"/>
-      <c r="I17" s="354">
-        <v>321231</v>
-      </c>
+      <c r="I17" s="354"/>
       <c r="J17" s="355"/>
       <c r="K17" s="355"/>
-      <c r="L17" s="355" t="s">
-        <v>45</v>
-      </c>
+      <c r="L17" s="355"/>
       <c r="M17" s="355"/>
       <c r="N17" s="362"/>
       <c r="Q17" s="3" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:19" customHeight="1" ht="9">
@@ -7349,17 +7137,17 @@
       <c r="G18" s="151"/>
       <c r="H18" s="255"/>
       <c r="I18" s="363" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J18" s="364"/>
       <c r="K18" s="364"/>
       <c r="L18" s="364" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="M18" s="364"/>
       <c r="N18" s="367"/>
       <c r="Q18" s="3" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:19" customHeight="1" ht="5.25">
@@ -7371,18 +7159,14 @@
       <c r="F19" s="257"/>
       <c r="G19" s="151"/>
       <c r="H19" s="255"/>
-      <c r="I19" s="377" t="s">
-        <v>50</v>
-      </c>
+      <c r="I19" s="377"/>
       <c r="J19" s="312"/>
       <c r="K19" s="312"/>
-      <c r="L19" s="311" t="s">
-        <v>51</v>
-      </c>
+      <c r="L19" s="311"/>
       <c r="M19" s="312"/>
       <c r="N19" s="313"/>
       <c r="Q19" s="3" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:19" customHeight="1" ht="9.75">
@@ -7401,7 +7185,7 @@
       <c r="M20" s="314"/>
       <c r="N20" s="315"/>
       <c r="Q20" s="3" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:19" customHeight="1" ht="9">
@@ -7414,46 +7198,40 @@
       <c r="G21" s="149"/>
       <c r="H21" s="251"/>
       <c r="I21" s="316" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="J21" s="317"/>
       <c r="K21" s="317"/>
       <c r="L21" s="430" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="M21" s="431"/>
       <c r="N21" s="432"/>
       <c r="Q21" s="3" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:19" customHeight="1" ht="15.75">
       <c r="A22" s="326" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B22" s="330" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C22" s="331"/>
-      <c r="D22" s="320">
-        <v>100</v>
-      </c>
+      <c r="D22" s="320"/>
       <c r="E22" s="277"/>
       <c r="F22" s="321"/>
       <c r="G22" s="149"/>
       <c r="H22" s="251"/>
-      <c r="I22" s="354" t="s">
-        <v>59</v>
-      </c>
+      <c r="I22" s="354"/>
       <c r="J22" s="355"/>
       <c r="K22" s="355"/>
-      <c r="L22" s="355" t="s">
-        <v>60</v>
-      </c>
+      <c r="L22" s="355"/>
       <c r="M22" s="355"/>
       <c r="N22" s="362"/>
       <c r="Q22" s="3" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:19" customHeight="1" ht="8.25">
@@ -7466,63 +7244,57 @@
       <c r="G23" s="149"/>
       <c r="H23" s="251"/>
       <c r="I23" s="435" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="J23" s="436"/>
       <c r="K23" s="436"/>
       <c r="L23" s="433" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="M23" s="433"/>
       <c r="N23" s="434"/>
       <c r="Q23" s="3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:19" customHeight="1" ht="22.5">
       <c r="A24" s="163" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B24" s="334" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C24" s="335"/>
-      <c r="D24" s="351">
-        <v>100</v>
-      </c>
+      <c r="D24" s="351"/>
       <c r="E24" s="352"/>
       <c r="F24" s="353"/>
       <c r="G24" s="400" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="H24" s="401"/>
-      <c r="I24" s="368">
-        <v>3500</v>
-      </c>
+      <c r="I24" s="368"/>
       <c r="J24" s="369"/>
       <c r="K24" s="369"/>
       <c r="L24" s="369"/>
       <c r="M24" s="369"/>
       <c r="N24" s="370"/>
       <c r="Q24" s="3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:19" customHeight="1" ht="15.75">
       <c r="A25" s="318" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B25" s="330" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C25" s="331"/>
-      <c r="D25" s="320" t="s">
-        <v>71</v>
-      </c>
+      <c r="D25" s="320"/>
       <c r="E25" s="277"/>
       <c r="F25" s="321"/>
       <c r="G25" s="109" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="H25" s="99"/>
       <c r="I25" s="354"/>
@@ -7532,7 +7304,7 @@
       <c r="M25" s="355"/>
       <c r="N25" s="362"/>
       <c r="Q25" s="3" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:19" customHeight="1" ht="9">
@@ -7545,30 +7317,28 @@
       <c r="G26" s="149"/>
       <c r="H26" s="251"/>
       <c r="I26" s="363" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="J26" s="364"/>
       <c r="K26" s="364"/>
       <c r="L26" s="364" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="M26" s="364"/>
       <c r="N26" s="367"/>
       <c r="Q26" s="3" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:19" customHeight="1" ht="15.75">
       <c r="A27" s="318" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B27" s="330" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="C27" s="331"/>
-      <c r="D27" s="320">
-        <v>1324</v>
-      </c>
+      <c r="D27" s="320"/>
       <c r="E27" s="277"/>
       <c r="F27" s="321"/>
       <c r="G27" s="151"/>
@@ -7580,7 +7350,7 @@
       <c r="M27" s="355"/>
       <c r="N27" s="362"/>
       <c r="Q27" s="3" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:19" customHeight="1" ht="9">
@@ -7593,30 +7363,28 @@
       <c r="G28" s="151"/>
       <c r="H28" s="255"/>
       <c r="I28" s="412" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="J28" s="410"/>
       <c r="K28" s="410"/>
       <c r="L28" s="409" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="M28" s="410"/>
       <c r="N28" s="411"/>
       <c r="Q28" s="3" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:19" customHeight="1" ht="15.75">
       <c r="A29" s="318" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B29" s="330" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C29" s="331"/>
-      <c r="D29" s="320">
-        <v>1234</v>
-      </c>
+      <c r="D29" s="320"/>
       <c r="E29" s="277"/>
       <c r="F29" s="321"/>
       <c r="G29" s="151"/>
@@ -7628,7 +7396,7 @@
       <c r="M29" s="408"/>
       <c r="N29" s="441"/>
       <c r="Q29" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:19" customHeight="1" ht="9.75">
@@ -7641,34 +7409,32 @@
       <c r="G30" s="151"/>
       <c r="H30" s="156"/>
       <c r="I30" s="437" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="J30" s="437"/>
       <c r="K30" s="437"/>
       <c r="L30" s="437" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="M30" s="437"/>
       <c r="N30" s="438"/>
       <c r="Q30" s="3" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:19" customHeight="1" ht="24.75">
       <c r="A31" s="165" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B31" s="97" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C31" s="98"/>
-      <c r="D31" s="351">
-        <v>12345313</v>
-      </c>
+      <c r="D31" s="351"/>
       <c r="E31" s="352"/>
       <c r="F31" s="353"/>
       <c r="G31" s="439" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="H31" s="440"/>
       <c r="I31" s="356"/>
@@ -7678,95 +7444,83 @@
       <c r="M31" s="357"/>
       <c r="N31" s="358"/>
       <c r="Q31" s="3" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:19" customHeight="1" ht="24.75">
       <c r="A32" s="163" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B32" s="97" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C32" s="98"/>
-      <c r="D32" s="351">
-        <v>131</v>
-      </c>
+      <c r="D32" s="351"/>
       <c r="E32" s="352"/>
       <c r="F32" s="353"/>
       <c r="G32" s="373" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="H32" s="335"/>
-      <c r="I32" s="356">
-        <v>99999999</v>
-      </c>
+      <c r="I32" s="356"/>
       <c r="J32" s="357"/>
       <c r="K32" s="357"/>
       <c r="L32" s="357"/>
       <c r="M32" s="357"/>
       <c r="N32" s="358"/>
       <c r="Q32" s="3" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:19" customHeight="1" ht="24.75">
       <c r="A33" s="402" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B33" s="335"/>
       <c r="C33" s="403"/>
-      <c r="D33" s="351">
-        <v>31331</v>
-      </c>
+      <c r="D33" s="351"/>
       <c r="E33" s="352"/>
       <c r="F33" s="353"/>
       <c r="G33" s="196" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="H33" s="150"/>
-      <c r="I33" s="356">
-        <v>9999999</v>
-      </c>
+      <c r="I33" s="356"/>
       <c r="J33" s="357"/>
       <c r="K33" s="357"/>
       <c r="L33" s="357"/>
       <c r="M33" s="357"/>
       <c r="N33" s="358"/>
       <c r="Q33" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:19" customHeight="1" ht="24.75">
       <c r="A34" s="168" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B34" s="254"/>
       <c r="C34" s="152"/>
-      <c r="D34" s="390">
-        <v>31232</v>
-      </c>
+      <c r="D34" s="390"/>
       <c r="E34" s="391"/>
       <c r="F34" s="392"/>
       <c r="G34" s="109" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="H34" s="99"/>
-      <c r="I34" s="356" t="s">
-        <v>95</v>
-      </c>
+      <c r="I34" s="356"/>
       <c r="J34" s="357"/>
       <c r="K34" s="357"/>
       <c r="L34" s="357"/>
       <c r="M34" s="357"/>
       <c r="N34" s="358"/>
       <c r="Q34" s="3" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:19" customHeight="1" ht="16.5">
       <c r="A35" s="205" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B35" s="206"/>
       <c r="C35" s="206"/>
@@ -7782,55 +7536,49 @@
       <c r="M35" s="206"/>
       <c r="N35" s="207"/>
       <c r="Q35" s="3" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:19" customHeight="1" ht="21">
       <c r="A36" s="102" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B36" s="215" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="C36" s="216"/>
-      <c r="D36" s="309" t="s">
-        <v>101</v>
-      </c>
+      <c r="D36" s="309"/>
       <c r="E36" s="309"/>
       <c r="F36" s="309"/>
       <c r="G36" s="309"/>
       <c r="H36" s="309"/>
       <c r="I36" s="291" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="J36" s="291"/>
       <c r="K36" s="291"/>
       <c r="L36" s="292"/>
       <c r="M36" s="328" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="N36" s="329"/>
       <c r="Q36" s="3" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:19" customHeight="1" ht="21">
       <c r="A37" s="149"/>
       <c r="B37" s="255" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C37" s="156"/>
-      <c r="D37" s="404" t="s">
-        <v>106</v>
-      </c>
+      <c r="D37" s="404"/>
       <c r="E37" s="405"/>
       <c r="F37" s="406"/>
       <c r="G37" s="247" t="s">
-        <v>107</v>
-      </c>
-      <c r="H37" s="248" t="s">
-        <v>108</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H37" s="248"/>
       <c r="I37" s="293"/>
       <c r="J37" s="266"/>
       <c r="K37" s="266"/>
@@ -7838,18 +7586,16 @@
       <c r="M37" s="289"/>
       <c r="N37" s="290"/>
       <c r="Q37" s="3" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:19" customHeight="1" ht="21">
       <c r="A38" s="169"/>
       <c r="B38" s="210" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C38" s="209"/>
-      <c r="D38" s="404" t="s">
-        <v>111</v>
-      </c>
+      <c r="D38" s="404"/>
       <c r="E38" s="405"/>
       <c r="F38" s="405"/>
       <c r="G38" s="405"/>
@@ -7861,18 +7607,16 @@
       <c r="M38" s="289"/>
       <c r="N38" s="290"/>
       <c r="Q38" s="3" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:19" customHeight="1" ht="21">
       <c r="A39" s="170"/>
       <c r="B39" s="97" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="C39" s="98"/>
-      <c r="D39" s="310" t="s">
-        <v>114</v>
-      </c>
+      <c r="D39" s="310"/>
       <c r="E39" s="310"/>
       <c r="F39" s="310"/>
       <c r="G39" s="310"/>
@@ -7884,18 +7628,16 @@
       <c r="M39" s="289"/>
       <c r="N39" s="290"/>
       <c r="Q39" s="3" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:19" customHeight="1" ht="21">
       <c r="A40" s="170"/>
       <c r="B40" s="97" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="C40" s="98"/>
-      <c r="D40" s="310" t="s">
-        <v>117</v>
-      </c>
+      <c r="D40" s="310"/>
       <c r="E40" s="310"/>
       <c r="F40" s="310"/>
       <c r="G40" s="310"/>
@@ -7907,18 +7649,16 @@
       <c r="M40" s="289"/>
       <c r="N40" s="290"/>
       <c r="Q40" s="3" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:19" customHeight="1" ht="21">
       <c r="A41" s="170"/>
       <c r="B41" s="97" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="C41" s="98"/>
-      <c r="D41" s="310" t="s">
-        <v>120</v>
-      </c>
+      <c r="D41" s="310"/>
       <c r="E41" s="310"/>
       <c r="F41" s="310"/>
       <c r="G41" s="310"/>
@@ -7930,18 +7670,16 @@
       <c r="M41" s="289"/>
       <c r="N41" s="290"/>
       <c r="Q41" s="3" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:19" customHeight="1" ht="21">
       <c r="A42" s="103"/>
       <c r="B42" s="104" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="C42" s="137"/>
-      <c r="D42" s="310" t="s">
-        <v>123</v>
-      </c>
+      <c r="D42" s="310"/>
       <c r="E42" s="310"/>
       <c r="F42" s="310"/>
       <c r="G42" s="310"/>
@@ -7953,20 +7691,18 @@
       <c r="M42" s="289"/>
       <c r="N42" s="290"/>
       <c r="Q42" s="3" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:19" customHeight="1" ht="21">
       <c r="A43" s="208" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="B43" s="213" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="C43" s="104"/>
-      <c r="D43" s="310" t="s">
-        <v>127</v>
-      </c>
+      <c r="D43" s="310"/>
       <c r="E43" s="310"/>
       <c r="F43" s="310"/>
       <c r="G43" s="310"/>
@@ -7978,26 +7714,22 @@
       <c r="M43" s="289"/>
       <c r="N43" s="290"/>
       <c r="Q43" s="3" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:19" customHeight="1" ht="21">
       <c r="A44" s="149"/>
       <c r="B44" s="251" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C44" s="251"/>
-      <c r="D44" s="404" t="s">
-        <v>129</v>
-      </c>
+      <c r="D44" s="404"/>
       <c r="E44" s="405"/>
       <c r="F44" s="406"/>
       <c r="G44" s="247" t="s">
-        <v>130</v>
-      </c>
-      <c r="H44" s="248" t="s">
-        <v>131</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="H44" s="248"/>
       <c r="I44" s="266"/>
       <c r="J44" s="266"/>
       <c r="K44" s="266"/>
@@ -8005,18 +7737,16 @@
       <c r="M44" s="289"/>
       <c r="N44" s="290"/>
       <c r="Q44" s="3" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:19" customHeight="1" ht="21">
       <c r="A45" s="169"/>
       <c r="B45" s="203" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C45" s="203"/>
-      <c r="D45" s="404" t="s">
-        <v>133</v>
-      </c>
+      <c r="D45" s="404"/>
       <c r="E45" s="405"/>
       <c r="F45" s="405"/>
       <c r="G45" s="405"/>
@@ -8028,15 +7758,15 @@
       <c r="M45" s="289"/>
       <c r="N45" s="290"/>
       <c r="Q45" s="3" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:19" customHeight="1" ht="21">
       <c r="A46" s="149" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="B46" s="104" t="s">
-        <v>136</v>
+        <v>109</v>
       </c>
       <c r="C46" s="104"/>
       <c r="D46" s="308"/>
@@ -8051,7 +7781,7 @@
       <c r="M46" s="289"/>
       <c r="N46" s="290"/>
       <c r="Q46" s="3" t="s">
-        <v>137</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:19" customHeight="1" ht="21">
@@ -8060,9 +7790,7 @@
         <v>12</v>
       </c>
       <c r="C47" s="251"/>
-      <c r="D47" s="461" t="s">
-        <v>138</v>
-      </c>
+      <c r="D47" s="461"/>
       <c r="E47" s="461"/>
       <c r="F47" s="461"/>
       <c r="G47" s="461"/>
@@ -8074,18 +7802,16 @@
       <c r="M47" s="289"/>
       <c r="N47" s="290"/>
       <c r="Q47" s="3" t="s">
-        <v>139</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:19" customHeight="1" ht="21">
       <c r="A48" s="149"/>
       <c r="B48" s="251" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C48" s="251"/>
-      <c r="D48" s="461" t="s">
-        <v>140</v>
-      </c>
+      <c r="D48" s="461"/>
       <c r="E48" s="461"/>
       <c r="F48" s="461"/>
       <c r="G48" s="461"/>
@@ -8097,24 +7823,22 @@
       <c r="M48" s="289"/>
       <c r="N48" s="290"/>
       <c r="Q48" s="3" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:19" customHeight="1" ht="21">
       <c r="A49" s="171"/>
       <c r="B49" s="204" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C49" s="204"/>
-      <c r="D49" s="301" t="s">
-        <v>142</v>
-      </c>
+      <c r="D49" s="301"/>
       <c r="E49" s="301"/>
       <c r="F49" s="301"/>
       <c r="G49" s="301"/>
       <c r="H49" s="301"/>
       <c r="I49" s="299" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
       <c r="J49" s="299"/>
       <c r="K49" s="299"/>
@@ -8122,12 +7846,12 @@
       <c r="M49" s="299"/>
       <c r="N49" s="300"/>
       <c r="Q49" s="3" t="s">
-        <v>144</v>
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:19" customHeight="1" ht="15.75">
       <c r="A50" s="172" t="s">
-        <v>145</v>
+        <v>115</v>
       </c>
       <c r="B50" s="172"/>
       <c r="C50" s="100"/>
@@ -8137,7 +7861,7 @@
       <c r="G50" s="101"/>
       <c r="H50" s="101"/>
       <c r="I50" s="388" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
       <c r="J50" s="388"/>
       <c r="K50" s="388"/>
@@ -8145,42 +7869,42 @@
       <c r="M50" s="388"/>
       <c r="N50" s="389"/>
       <c r="Q50" s="3" t="s">
-        <v>147</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:19" customHeight="1" ht="14.25">
       <c r="A51" s="381" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
       <c r="B51" s="413" t="s">
-        <v>149</v>
+        <v>119</v>
       </c>
       <c r="C51" s="413"/>
       <c r="D51" s="416" t="s">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="E51" s="417"/>
       <c r="F51" s="418"/>
       <c r="G51" s="416" t="s">
-        <v>151</v>
+        <v>121</v>
       </c>
       <c r="H51" s="417"/>
       <c r="I51" s="462"/>
       <c r="J51" s="302" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="K51" s="303"/>
       <c r="L51" s="459" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
       <c r="M51" s="383" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
       <c r="N51" s="306" t="s">
-        <v>155</v>
+        <v>125</v>
       </c>
       <c r="Q51" s="3" t="s">
-        <v>156</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:19" customHeight="1" ht="19.5">
@@ -8199,7 +7923,7 @@
       <c r="M52" s="383"/>
       <c r="N52" s="306"/>
       <c r="Q52" s="3" t="s">
-        <v>157</v>
+        <v>127</v>
       </c>
     </row>
     <row r="53" spans="1:19" customHeight="1" ht="14.25">
@@ -8213,10 +7937,10 @@
       <c r="H53" s="423"/>
       <c r="I53" s="464"/>
       <c r="J53" s="105" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
       <c r="K53" s="106" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="L53" s="460"/>
       <c r="M53" s="384"/>
@@ -8224,106 +7948,76 @@
       <c r="O53" s="107"/>
       <c r="P53" s="107"/>
       <c r="Q53" s="3" t="s">
-        <v>160</v>
+        <v>130</v>
       </c>
     </row>
     <row r="54" spans="1:19" customHeight="1" ht="28.5">
       <c r="A54" s="217"/>
       <c r="B54" s="218" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
       <c r="C54" s="218"/>
-      <c r="D54" s="424" t="s">
-        <v>162</v>
-      </c>
+      <c r="D54" s="424"/>
       <c r="E54" s="425"/>
       <c r="F54" s="426"/>
-      <c r="G54" s="294" t="s">
-        <v>161</v>
-      </c>
+      <c r="G54" s="294"/>
       <c r="H54" s="295"/>
       <c r="I54" s="296"/>
-      <c r="J54" s="157">
-        <v>2000</v>
-      </c>
-      <c r="K54" s="260">
-        <v>2006</v>
-      </c>
+      <c r="J54" s="157"/>
+      <c r="K54" s="260"/>
       <c r="L54" s="157"/>
-      <c r="M54" s="18">
-        <v>2006</v>
-      </c>
+      <c r="M54" s="18"/>
       <c r="N54" s="153"/>
       <c r="Q54" s="3" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
     </row>
     <row r="55" spans="1:19" customHeight="1" ht="28.5">
       <c r="A55" s="217"/>
       <c r="B55" s="218" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
       <c r="C55" s="218"/>
-      <c r="D55" s="424" t="s">
-        <v>165</v>
-      </c>
+      <c r="D55" s="424"/>
       <c r="E55" s="425"/>
       <c r="F55" s="426"/>
-      <c r="G55" s="294" t="s">
-        <v>166</v>
-      </c>
+      <c r="G55" s="294"/>
       <c r="H55" s="295"/>
       <c r="I55" s="296"/>
-      <c r="J55" s="157">
-        <v>2007</v>
-      </c>
-      <c r="K55" s="260">
-        <v>2011</v>
-      </c>
+      <c r="J55" s="157"/>
+      <c r="K55" s="260"/>
       <c r="L55" s="157"/>
-      <c r="M55" s="19">
-        <v>2011</v>
-      </c>
+      <c r="M55" s="19"/>
       <c r="N55" s="153"/>
       <c r="Q55" s="3" t="s">
-        <v>167</v>
+        <v>134</v>
       </c>
     </row>
     <row r="56" spans="1:19" customHeight="1" ht="28.5">
       <c r="A56" s="217"/>
       <c r="B56" s="218" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="C56" s="218"/>
-      <c r="D56" s="424" t="s">
-        <v>169</v>
-      </c>
+      <c r="D56" s="424"/>
       <c r="E56" s="425"/>
       <c r="F56" s="426"/>
-      <c r="G56" s="294" t="s">
-        <v>170</v>
-      </c>
+      <c r="G56" s="294"/>
       <c r="H56" s="295"/>
       <c r="I56" s="296"/>
-      <c r="J56" s="157">
-        <v>2012</v>
-      </c>
-      <c r="K56" s="260">
-        <v>2016</v>
-      </c>
+      <c r="J56" s="157"/>
+      <c r="K56" s="260"/>
       <c r="L56" s="157"/>
-      <c r="M56" s="18">
-        <v>2016</v>
-      </c>
+      <c r="M56" s="18"/>
       <c r="N56" s="153"/>
       <c r="Q56" s="3" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:19" customHeight="1" ht="28.5">
       <c r="A57" s="217"/>
       <c r="B57" s="218" t="s">
-        <v>172</v>
+        <v>137</v>
       </c>
       <c r="C57" s="218"/>
       <c r="D57" s="424"/>
@@ -8338,13 +8032,13 @@
       <c r="M57" s="19"/>
       <c r="N57" s="153"/>
       <c r="Q57" s="3" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:19" customHeight="1" ht="28.5">
       <c r="A58" s="219"/>
       <c r="B58" s="220" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="C58" s="220"/>
       <c r="D58" s="427"/>
@@ -8359,12 +8053,12 @@
       <c r="M58" s="21"/>
       <c r="N58" s="153"/>
       <c r="Q58" s="3" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
     </row>
     <row r="59" spans="1:19" customHeight="1" ht="12">
       <c r="A59" s="448" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
       <c r="B59" s="449"/>
       <c r="C59" s="449"/>
@@ -8380,12 +8074,12 @@
       <c r="M59" s="449"/>
       <c r="N59" s="450"/>
       <c r="Q59" s="3" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
     </row>
     <row r="60" spans="1:19" customHeight="1" ht="27.75">
       <c r="A60" s="445" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="B60" s="446"/>
       <c r="C60" s="447"/>
@@ -8396,19 +8090,19 @@
       <c r="H60" s="455"/>
       <c r="I60" s="456"/>
       <c r="J60" s="457" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="K60" s="458"/>
       <c r="L60" s="451"/>
       <c r="M60" s="452"/>
       <c r="N60" s="453"/>
       <c r="Q60" s="3" t="s">
-        <v>179</v>
+        <v>144</v>
       </c>
     </row>
     <row r="61" spans="1:19" customHeight="1" ht="12" s="143" customFormat="1">
       <c r="A61" s="442" t="s">
-        <v>180</v>
+        <v>145</v>
       </c>
       <c r="B61" s="443"/>
       <c r="C61" s="443"/>
@@ -8424,7 +8118,7 @@
       <c r="M61" s="443"/>
       <c r="N61" s="444"/>
       <c r="Q61" s="233" t="s">
-        <v>181</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62" spans="1:19" customHeight="1" ht="14.25">
@@ -8443,7 +8137,7 @@
       <c r="M62" s="108"/>
       <c r="N62" s="108"/>
       <c r="Q62" s="3" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
     </row>
     <row r="63" spans="1:19" customHeight="1" ht="14.25">
@@ -8462,7 +8156,7 @@
       <c r="M63" s="108"/>
       <c r="N63" s="108"/>
       <c r="Q63" s="3" t="s">
-        <v>183</v>
+        <v>148</v>
       </c>
     </row>
     <row r="64" spans="1:19" customHeight="1" ht="28.5">
@@ -8481,7 +8175,7 @@
       <c r="M64" s="108"/>
       <c r="N64" s="108"/>
       <c r="Q64" s="3" t="s">
-        <v>184</v>
+        <v>149</v>
       </c>
     </row>
     <row r="65" spans="1:19" customHeight="1" ht="14.25">
@@ -8500,7 +8194,7 @@
       <c r="M65" s="108"/>
       <c r="N65" s="108"/>
       <c r="Q65" s="3" t="s">
-        <v>185</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:19" customHeight="1" ht="14.25">
@@ -8519,7 +8213,7 @@
       <c r="M66" s="108"/>
       <c r="N66" s="108"/>
       <c r="Q66" s="3" t="s">
-        <v>186</v>
+        <v>151</v>
       </c>
     </row>
     <row r="67" spans="1:19" customHeight="1" ht="14.25">
@@ -8538,7 +8232,7 @@
       <c r="M67" s="108"/>
       <c r="N67" s="108"/>
       <c r="Q67" s="3" t="s">
-        <v>187</v>
+        <v>152</v>
       </c>
     </row>
     <row r="68" spans="1:19" customHeight="1" ht="14.25">
@@ -8557,7 +8251,7 @@
       <c r="M68" s="108"/>
       <c r="N68" s="108"/>
       <c r="Q68" s="3" t="s">
-        <v>188</v>
+        <v>153</v>
       </c>
     </row>
     <row r="69" spans="1:19" customHeight="1" ht="28.5">
@@ -8576,7 +8270,7 @@
       <c r="M69" s="108"/>
       <c r="N69" s="108"/>
       <c r="Q69" s="3" t="s">
-        <v>189</v>
+        <v>154</v>
       </c>
     </row>
     <row r="70" spans="1:19" customHeight="1" ht="14.25">
@@ -8595,7 +8289,7 @@
       <c r="M70" s="108"/>
       <c r="N70" s="108"/>
       <c r="Q70" s="3" t="s">
-        <v>190</v>
+        <v>155</v>
       </c>
     </row>
     <row r="71" spans="1:19" customHeight="1" ht="14.25">
@@ -8614,7 +8308,7 @@
       <c r="M71" s="108"/>
       <c r="N71" s="108"/>
       <c r="Q71" s="3" t="s">
-        <v>191</v>
+        <v>156</v>
       </c>
     </row>
     <row r="72" spans="1:19" customHeight="1" ht="14.25">
@@ -8633,7 +8327,7 @@
       <c r="M72" s="108"/>
       <c r="N72" s="108"/>
       <c r="Q72" s="3" t="s">
-        <v>192</v>
+        <v>157</v>
       </c>
     </row>
     <row r="73" spans="1:19" customHeight="1" ht="14.25">
@@ -8652,7 +8346,7 @@
       <c r="M73" s="108"/>
       <c r="N73" s="108"/>
       <c r="Q73" s="3" t="s">
-        <v>193</v>
+        <v>158</v>
       </c>
     </row>
     <row r="74" spans="1:19" customHeight="1" ht="14.25">
@@ -8671,7 +8365,7 @@
       <c r="M74" s="108"/>
       <c r="N74" s="108"/>
       <c r="Q74" s="3" t="s">
-        <v>194</v>
+        <v>159</v>
       </c>
     </row>
     <row r="75" spans="1:19" customHeight="1" ht="14.25">
@@ -8690,7 +8384,7 @@
       <c r="M75" s="108"/>
       <c r="N75" s="108"/>
       <c r="Q75" s="3" t="s">
-        <v>195</v>
+        <v>160</v>
       </c>
     </row>
     <row r="76" spans="1:19" customHeight="1" ht="14.25">
@@ -8709,7 +8403,7 @@
       <c r="M76" s="108"/>
       <c r="N76" s="108"/>
       <c r="Q76" s="3" t="s">
-        <v>196</v>
+        <v>161</v>
       </c>
     </row>
     <row r="77" spans="1:19" customHeight="1" ht="14.25">
@@ -8728,7 +8422,7 @@
       <c r="M77" s="108"/>
       <c r="N77" s="108"/>
       <c r="Q77" s="3" t="s">
-        <v>197</v>
+        <v>162</v>
       </c>
     </row>
     <row r="78" spans="1:19" customHeight="1" ht="14.25">
@@ -8747,7 +8441,7 @@
       <c r="M78" s="108"/>
       <c r="N78" s="108"/>
       <c r="Q78" s="3" t="s">
-        <v>198</v>
+        <v>163</v>
       </c>
     </row>
     <row r="79" spans="1:19" customHeight="1" ht="14.25">
@@ -8766,7 +8460,7 @@
       <c r="M79" s="108"/>
       <c r="N79" s="108"/>
       <c r="Q79" s="3" t="s">
-        <v>199</v>
+        <v>164</v>
       </c>
     </row>
     <row r="80" spans="1:19" customHeight="1" ht="14.25">
@@ -8785,7 +8479,7 @@
       <c r="M80" s="108"/>
       <c r="N80" s="108"/>
       <c r="Q80" s="3" t="s">
-        <v>200</v>
+        <v>165</v>
       </c>
     </row>
     <row r="81" spans="1:19" customHeight="1" ht="14.25">
@@ -8804,7 +8498,7 @@
       <c r="M81" s="108"/>
       <c r="N81" s="108"/>
       <c r="Q81" s="3" t="s">
-        <v>201</v>
+        <v>166</v>
       </c>
     </row>
     <row r="82" spans="1:19" customHeight="1" ht="14.25">
@@ -8823,7 +8517,7 @@
       <c r="M82" s="108"/>
       <c r="N82" s="108"/>
       <c r="Q82" s="3" t="s">
-        <v>202</v>
+        <v>167</v>
       </c>
     </row>
     <row r="83" spans="1:19" customHeight="1" ht="14.25">
@@ -8842,7 +8536,7 @@
       <c r="M83" s="108"/>
       <c r="N83" s="108"/>
       <c r="Q83" s="3" t="s">
-        <v>203</v>
+        <v>168</v>
       </c>
     </row>
     <row r="84" spans="1:19" customHeight="1" ht="14.25">
@@ -8861,7 +8555,7 @@
       <c r="M84" s="108"/>
       <c r="N84" s="108"/>
       <c r="Q84" s="3" t="s">
-        <v>204</v>
+        <v>169</v>
       </c>
     </row>
     <row r="85" spans="1:19" customHeight="1" ht="28.5">
@@ -8880,7 +8574,7 @@
       <c r="M85" s="108"/>
       <c r="N85" s="108"/>
       <c r="Q85" s="3" t="s">
-        <v>205</v>
+        <v>170</v>
       </c>
     </row>
     <row r="86" spans="1:19" customHeight="1" ht="14.25">
@@ -8899,7 +8593,7 @@
       <c r="M86" s="108"/>
       <c r="N86" s="108"/>
       <c r="Q86" s="3" t="s">
-        <v>206</v>
+        <v>171</v>
       </c>
     </row>
     <row r="87" spans="1:19" customHeight="1" ht="14.25">
@@ -8918,7 +8612,7 @@
       <c r="M87" s="108"/>
       <c r="N87" s="108"/>
       <c r="Q87" s="3" t="s">
-        <v>207</v>
+        <v>172</v>
       </c>
     </row>
     <row r="88" spans="1:19" customHeight="1" ht="14.25">
@@ -8937,7 +8631,7 @@
       <c r="M88" s="108"/>
       <c r="N88" s="108"/>
       <c r="Q88" s="3" t="s">
-        <v>208</v>
+        <v>173</v>
       </c>
     </row>
     <row r="89" spans="1:19" customHeight="1" ht="14.25">
@@ -8956,7 +8650,7 @@
       <c r="M89" s="108"/>
       <c r="N89" s="108"/>
       <c r="Q89" s="3" t="s">
-        <v>209</v>
+        <v>174</v>
       </c>
     </row>
     <row r="90" spans="1:19" customHeight="1" ht="14.25">
@@ -8975,7 +8669,7 @@
       <c r="M90" s="108"/>
       <c r="N90" s="108"/>
       <c r="Q90" s="3" t="s">
-        <v>210</v>
+        <v>175</v>
       </c>
     </row>
     <row r="91" spans="1:19" customHeight="1" ht="14.25">
@@ -8994,7 +8688,7 @@
       <c r="M91" s="108"/>
       <c r="N91" s="108"/>
       <c r="Q91" s="3" t="s">
-        <v>211</v>
+        <v>176</v>
       </c>
     </row>
     <row r="92" spans="1:19" customHeight="1" ht="14.25">
@@ -9013,7 +8707,7 @@
       <c r="M92" s="108"/>
       <c r="N92" s="108"/>
       <c r="Q92" s="3" t="s">
-        <v>212</v>
+        <v>177</v>
       </c>
     </row>
     <row r="93" spans="1:19" customHeight="1" ht="14.25">
@@ -9032,7 +8726,7 @@
       <c r="M93" s="108"/>
       <c r="N93" s="108"/>
       <c r="Q93" s="3" t="s">
-        <v>213</v>
+        <v>178</v>
       </c>
     </row>
     <row r="94" spans="1:19" customHeight="1" ht="14.25">
@@ -9051,7 +8745,7 @@
       <c r="M94" s="108"/>
       <c r="N94" s="108"/>
       <c r="Q94" s="3" t="s">
-        <v>214</v>
+        <v>179</v>
       </c>
     </row>
     <row r="95" spans="1:19" customHeight="1" ht="14.25">
@@ -9070,7 +8764,7 @@
       <c r="M95" s="108"/>
       <c r="N95" s="108"/>
       <c r="Q95" s="3" t="s">
-        <v>215</v>
+        <v>180</v>
       </c>
     </row>
     <row r="96" spans="1:19" customHeight="1" ht="14.25">
@@ -9089,7 +8783,7 @@
       <c r="M96" s="108"/>
       <c r="N96" s="108"/>
       <c r="Q96" s="3" t="s">
-        <v>216</v>
+        <v>181</v>
       </c>
     </row>
     <row r="97" spans="1:19" customHeight="1" ht="14.25">
@@ -9108,7 +8802,7 @@
       <c r="M97" s="108"/>
       <c r="N97" s="108"/>
       <c r="Q97" s="3" t="s">
-        <v>217</v>
+        <v>182</v>
       </c>
     </row>
     <row r="98" spans="1:19" customHeight="1" ht="14.25">
@@ -9127,7 +8821,7 @@
       <c r="M98" s="108"/>
       <c r="N98" s="108"/>
       <c r="Q98" s="3" t="s">
-        <v>218</v>
+        <v>183</v>
       </c>
     </row>
     <row r="99" spans="1:19" customHeight="1" ht="14.25">
@@ -9146,7 +8840,7 @@
       <c r="M99" s="108"/>
       <c r="N99" s="108"/>
       <c r="Q99" s="3" t="s">
-        <v>219</v>
+        <v>184</v>
       </c>
     </row>
     <row r="100" spans="1:19" customHeight="1" ht="14.25">
@@ -9165,7 +8859,7 @@
       <c r="M100" s="108"/>
       <c r="N100" s="108"/>
       <c r="Q100" s="3" t="s">
-        <v>220</v>
+        <v>185</v>
       </c>
     </row>
     <row r="101" spans="1:19" customHeight="1" ht="14.25">
@@ -9184,7 +8878,7 @@
       <c r="M101" s="108"/>
       <c r="N101" s="108"/>
       <c r="Q101" s="3" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
     </row>
     <row r="102" spans="1:19" customHeight="1" ht="14.25">
@@ -9203,7 +8897,7 @@
       <c r="M102" s="108"/>
       <c r="N102" s="108"/>
       <c r="Q102" s="3" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
     </row>
     <row r="103" spans="1:19" customHeight="1" ht="14.25">
@@ -9222,7 +8916,7 @@
       <c r="M103" s="108"/>
       <c r="N103" s="108"/>
       <c r="Q103" s="3" t="s">
-        <v>223</v>
+        <v>188</v>
       </c>
     </row>
     <row r="104" spans="1:19" customHeight="1" ht="14.25">
@@ -9241,7 +8935,7 @@
       <c r="M104" s="108"/>
       <c r="N104" s="108"/>
       <c r="Q104" s="3" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
     </row>
     <row r="105" spans="1:19" customHeight="1" ht="14.25">
@@ -9260,7 +8954,7 @@
       <c r="M105" s="108"/>
       <c r="N105" s="108"/>
       <c r="Q105" s="3" t="s">
-        <v>225</v>
+        <v>190</v>
       </c>
     </row>
     <row r="106" spans="1:19" customHeight="1" ht="14.25">
@@ -9279,7 +8973,7 @@
       <c r="M106" s="108"/>
       <c r="N106" s="108"/>
       <c r="Q106" s="3" t="s">
-        <v>226</v>
+        <v>191</v>
       </c>
     </row>
     <row r="107" spans="1:19" customHeight="1" ht="14.25">
@@ -9298,7 +8992,7 @@
       <c r="M107" s="108"/>
       <c r="N107" s="108"/>
       <c r="Q107" s="3" t="s">
-        <v>227</v>
+        <v>192</v>
       </c>
     </row>
     <row r="108" spans="1:19" customHeight="1" ht="14.25">
@@ -9317,7 +9011,7 @@
       <c r="M108" s="108"/>
       <c r="N108" s="108"/>
       <c r="Q108" s="3" t="s">
-        <v>228</v>
+        <v>193</v>
       </c>
     </row>
     <row r="109" spans="1:19" customHeight="1" ht="14.25">
@@ -9336,7 +9030,7 @@
       <c r="M109" s="108"/>
       <c r="N109" s="108"/>
       <c r="Q109" s="3" t="s">
-        <v>229</v>
+        <v>194</v>
       </c>
     </row>
     <row r="110" spans="1:19" customHeight="1" ht="14.25">
@@ -9355,7 +9049,7 @@
       <c r="M110" s="108"/>
       <c r="N110" s="108"/>
       <c r="Q110" s="3" t="s">
-        <v>230</v>
+        <v>195</v>
       </c>
     </row>
     <row r="111" spans="1:19" customHeight="1" ht="14.25">
@@ -9374,7 +9068,7 @@
       <c r="M111" s="108"/>
       <c r="N111" s="108"/>
       <c r="Q111" s="3" t="s">
-        <v>231</v>
+        <v>196</v>
       </c>
     </row>
     <row r="112" spans="1:19" customHeight="1" ht="14.25">
@@ -9393,7 +9087,7 @@
       <c r="M112" s="108"/>
       <c r="N112" s="108"/>
       <c r="Q112" s="3" t="s">
-        <v>232</v>
+        <v>197</v>
       </c>
     </row>
     <row r="113" spans="1:19" customHeight="1" ht="14.25">
@@ -9412,7 +9106,7 @@
       <c r="M113" s="108"/>
       <c r="N113" s="108"/>
       <c r="Q113" s="3" t="s">
-        <v>233</v>
+        <v>198</v>
       </c>
     </row>
     <row r="114" spans="1:19" customHeight="1" ht="14.25">
@@ -9431,7 +9125,7 @@
       <c r="M114" s="108"/>
       <c r="N114" s="108"/>
       <c r="Q114" s="3" t="s">
-        <v>234</v>
+        <v>199</v>
       </c>
     </row>
     <row r="115" spans="1:19" customHeight="1" ht="14.25">
@@ -9450,7 +9144,7 @@
       <c r="M115" s="108"/>
       <c r="N115" s="108"/>
       <c r="Q115" s="3" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
     </row>
     <row r="116" spans="1:19" customHeight="1" ht="14.25">
@@ -9469,7 +9163,7 @@
       <c r="M116" s="108"/>
       <c r="N116" s="108"/>
       <c r="Q116" s="3" t="s">
-        <v>236</v>
+        <v>201</v>
       </c>
     </row>
     <row r="117" spans="1:19" customHeight="1" ht="14.25">
@@ -9488,7 +9182,7 @@
       <c r="M117" s="108"/>
       <c r="N117" s="108"/>
       <c r="Q117" s="3" t="s">
-        <v>237</v>
+        <v>202</v>
       </c>
     </row>
     <row r="118" spans="1:19" customHeight="1" ht="14.25">
@@ -9507,7 +9201,7 @@
       <c r="M118" s="108"/>
       <c r="N118" s="108"/>
       <c r="Q118" s="3" t="s">
-        <v>238</v>
+        <v>203</v>
       </c>
     </row>
     <row r="119" spans="1:19" customHeight="1" ht="14.25">
@@ -9526,7 +9220,7 @@
       <c r="M119" s="108"/>
       <c r="N119" s="108"/>
       <c r="Q119" s="3" t="s">
-        <v>239</v>
+        <v>204</v>
       </c>
     </row>
     <row r="120" spans="1:19" customHeight="1" ht="14.25">
@@ -9545,7 +9239,7 @@
       <c r="M120" s="108"/>
       <c r="N120" s="108"/>
       <c r="Q120" s="3" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
     </row>
     <row r="121" spans="1:19" customHeight="1" ht="14.25">
@@ -9564,7 +9258,7 @@
       <c r="M121" s="108"/>
       <c r="N121" s="108"/>
       <c r="Q121" s="3" t="s">
-        <v>241</v>
+        <v>206</v>
       </c>
     </row>
     <row r="122" spans="1:19" customHeight="1" ht="14.25">
@@ -9583,7 +9277,7 @@
       <c r="M122" s="108"/>
       <c r="N122" s="108"/>
       <c r="Q122" s="3" t="s">
-        <v>242</v>
+        <v>207</v>
       </c>
     </row>
     <row r="123" spans="1:19" customHeight="1" ht="14.25">
@@ -9602,7 +9296,7 @@
       <c r="M123" s="108"/>
       <c r="N123" s="108"/>
       <c r="Q123" s="3" t="s">
-        <v>243</v>
+        <v>208</v>
       </c>
     </row>
     <row r="124" spans="1:19" customHeight="1" ht="14.25">
@@ -9621,7 +9315,7 @@
       <c r="M124" s="108"/>
       <c r="N124" s="108"/>
       <c r="Q124" s="3" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
     </row>
     <row r="125" spans="1:19" customHeight="1" ht="14.25">
@@ -9640,7 +9334,7 @@
       <c r="M125" s="108"/>
       <c r="N125" s="108"/>
       <c r="Q125" s="3" t="s">
-        <v>245</v>
+        <v>210</v>
       </c>
     </row>
     <row r="126" spans="1:19" customHeight="1" ht="14.25">
@@ -9659,7 +9353,7 @@
       <c r="M126" s="108"/>
       <c r="N126" s="108"/>
       <c r="Q126" s="3" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
     </row>
     <row r="127" spans="1:19" customHeight="1" ht="14.25">
@@ -9678,7 +9372,7 @@
       <c r="M127" s="108"/>
       <c r="N127" s="108"/>
       <c r="Q127" s="3" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
     </row>
     <row r="128" spans="1:19" customHeight="1" ht="28.5">
@@ -9697,7 +9391,7 @@
       <c r="M128" s="108"/>
       <c r="N128" s="108"/>
       <c r="Q128" s="3" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
     </row>
     <row r="129" spans="1:19" customHeight="1" ht="14.25">
@@ -9716,7 +9410,7 @@
       <c r="M129" s="108"/>
       <c r="N129" s="108"/>
       <c r="Q129" s="3" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
     </row>
     <row r="130" spans="1:19" customHeight="1" ht="14.25">
@@ -9735,7 +9429,7 @@
       <c r="M130" s="108"/>
       <c r="N130" s="108"/>
       <c r="Q130" s="3" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
     </row>
     <row r="131" spans="1:19" customHeight="1" ht="14.25">
@@ -9754,7 +9448,7 @@
       <c r="M131" s="108"/>
       <c r="N131" s="108"/>
       <c r="Q131" s="3" t="s">
-        <v>251</v>
+        <v>216</v>
       </c>
     </row>
     <row r="132" spans="1:19" customHeight="1" ht="14.25">
@@ -9773,7 +9467,7 @@
       <c r="M132" s="108"/>
       <c r="N132" s="108"/>
       <c r="Q132" s="3" t="s">
-        <v>252</v>
+        <v>217</v>
       </c>
     </row>
     <row r="133" spans="1:19" customHeight="1" ht="14.25">
@@ -9792,7 +9486,7 @@
       <c r="M133" s="108"/>
       <c r="N133" s="108"/>
       <c r="Q133" s="3" t="s">
-        <v>253</v>
+        <v>218</v>
       </c>
     </row>
     <row r="134" spans="1:19" customHeight="1" ht="14.25">
@@ -9811,7 +9505,7 @@
       <c r="M134" s="108"/>
       <c r="N134" s="108"/>
       <c r="Q134" s="3" t="s">
-        <v>254</v>
+        <v>219</v>
       </c>
     </row>
     <row r="135" spans="1:19" customHeight="1" ht="14.25">
@@ -9830,7 +9524,7 @@
       <c r="M135" s="108"/>
       <c r="N135" s="108"/>
       <c r="Q135" s="3" t="s">
-        <v>255</v>
+        <v>220</v>
       </c>
     </row>
     <row r="136" spans="1:19" customHeight="1" ht="14.25">
@@ -9849,7 +9543,7 @@
       <c r="M136" s="108"/>
       <c r="N136" s="108"/>
       <c r="Q136" s="3" t="s">
-        <v>256</v>
+        <v>221</v>
       </c>
     </row>
     <row r="137" spans="1:19" customHeight="1" ht="14.25">
@@ -9868,7 +9562,7 @@
       <c r="M137" s="108"/>
       <c r="N137" s="108"/>
       <c r="Q137" s="3" t="s">
-        <v>257</v>
+        <v>222</v>
       </c>
     </row>
     <row r="138" spans="1:19" customHeight="1" ht="14.25">
@@ -9887,7 +9581,7 @@
       <c r="M138" s="108"/>
       <c r="N138" s="108"/>
       <c r="Q138" s="3" t="s">
-        <v>258</v>
+        <v>223</v>
       </c>
     </row>
     <row r="139" spans="1:19" customHeight="1" ht="14.25">
@@ -9906,7 +9600,7 @@
       <c r="M139" s="108"/>
       <c r="N139" s="108"/>
       <c r="Q139" s="3" t="s">
-        <v>259</v>
+        <v>224</v>
       </c>
     </row>
     <row r="140" spans="1:19" customHeight="1" ht="14.25">
@@ -9925,7 +9619,7 @@
       <c r="M140" s="108"/>
       <c r="N140" s="108"/>
       <c r="Q140" s="3" t="s">
-        <v>260</v>
+        <v>225</v>
       </c>
     </row>
     <row r="141" spans="1:19" customHeight="1" ht="14.25">
@@ -9944,7 +9638,7 @@
       <c r="M141" s="108"/>
       <c r="N141" s="108"/>
       <c r="Q141" s="3" t="s">
-        <v>261</v>
+        <v>226</v>
       </c>
     </row>
     <row r="142" spans="1:19" customHeight="1" ht="14.25">
@@ -9963,7 +9657,7 @@
       <c r="M142" s="108"/>
       <c r="N142" s="108"/>
       <c r="Q142" s="3" t="s">
-        <v>262</v>
+        <v>227</v>
       </c>
     </row>
     <row r="143" spans="1:19" customHeight="1" ht="28.5">
@@ -9982,7 +9676,7 @@
       <c r="M143" s="108"/>
       <c r="N143" s="108"/>
       <c r="Q143" s="3" t="s">
-        <v>263</v>
+        <v>228</v>
       </c>
     </row>
     <row r="144" spans="1:19" customHeight="1" ht="14.25">
@@ -10001,7 +9695,7 @@
       <c r="M144" s="108"/>
       <c r="N144" s="108"/>
       <c r="Q144" s="3" t="s">
-        <v>264</v>
+        <v>229</v>
       </c>
     </row>
     <row r="145" spans="1:19" customHeight="1" ht="14.25">
@@ -10020,7 +9714,7 @@
       <c r="M145" s="108"/>
       <c r="N145" s="108"/>
       <c r="Q145" s="3" t="s">
-        <v>265</v>
+        <v>230</v>
       </c>
     </row>
     <row r="146" spans="1:19" customHeight="1" ht="14.25">
@@ -10039,7 +9733,7 @@
       <c r="M146" s="108"/>
       <c r="N146" s="108"/>
       <c r="Q146" s="3" t="s">
-        <v>266</v>
+        <v>231</v>
       </c>
     </row>
     <row r="147" spans="1:19" customHeight="1" ht="14.25">
@@ -10058,7 +9752,7 @@
       <c r="M147" s="108"/>
       <c r="N147" s="108"/>
       <c r="Q147" s="3" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
     </row>
     <row r="148" spans="1:19" customHeight="1" ht="14.25">
@@ -10077,7 +9771,7 @@
       <c r="M148" s="108"/>
       <c r="N148" s="108"/>
       <c r="Q148" s="3" t="s">
-        <v>268</v>
+        <v>233</v>
       </c>
     </row>
     <row r="149" spans="1:19" customHeight="1" ht="14.25">
@@ -10096,7 +9790,7 @@
       <c r="M149" s="108"/>
       <c r="N149" s="108"/>
       <c r="Q149" s="3" t="s">
-        <v>269</v>
+        <v>234</v>
       </c>
     </row>
     <row r="150" spans="1:19" customHeight="1" ht="14.25">
@@ -10115,7 +9809,7 @@
       <c r="M150" s="108"/>
       <c r="N150" s="108"/>
       <c r="Q150" s="3" t="s">
-        <v>270</v>
+        <v>235</v>
       </c>
     </row>
     <row r="151" spans="1:19" customHeight="1" ht="14.25">
@@ -10134,7 +9828,7 @@
       <c r="M151" s="108"/>
       <c r="N151" s="108"/>
       <c r="Q151" s="3" t="s">
-        <v>271</v>
+        <v>236</v>
       </c>
     </row>
     <row r="152" spans="1:19" customHeight="1" ht="14.25">
@@ -10153,7 +9847,7 @@
       <c r="M152" s="108"/>
       <c r="N152" s="108"/>
       <c r="Q152" s="3" t="s">
-        <v>272</v>
+        <v>237</v>
       </c>
     </row>
     <row r="153" spans="1:19" customHeight="1" ht="28.5">
@@ -10172,7 +9866,7 @@
       <c r="M153" s="108"/>
       <c r="N153" s="108"/>
       <c r="Q153" s="3" t="s">
-        <v>273</v>
+        <v>238</v>
       </c>
     </row>
     <row r="154" spans="1:19" customHeight="1" ht="14.25">
@@ -10191,7 +9885,7 @@
       <c r="M154" s="108"/>
       <c r="N154" s="108"/>
       <c r="Q154" s="3" t="s">
-        <v>274</v>
+        <v>239</v>
       </c>
     </row>
     <row r="155" spans="1:19" customHeight="1" ht="28.5">
@@ -10210,7 +9904,7 @@
       <c r="M155" s="108"/>
       <c r="N155" s="108"/>
       <c r="Q155" s="3" t="s">
-        <v>275</v>
+        <v>240</v>
       </c>
     </row>
     <row r="156" spans="1:19" customHeight="1" ht="14.25">
@@ -10229,7 +9923,7 @@
       <c r="M156" s="108"/>
       <c r="N156" s="108"/>
       <c r="Q156" s="3" t="s">
-        <v>276</v>
+        <v>241</v>
       </c>
     </row>
     <row r="157" spans="1:19" customHeight="1" ht="14.25">
@@ -10248,7 +9942,7 @@
       <c r="M157" s="108"/>
       <c r="N157" s="108"/>
       <c r="Q157" s="3" t="s">
-        <v>277</v>
+        <v>242</v>
       </c>
     </row>
     <row r="158" spans="1:19" customHeight="1" ht="14.25">
@@ -10267,7 +9961,7 @@
       <c r="M158" s="108"/>
       <c r="N158" s="108"/>
       <c r="Q158" s="3" t="s">
-        <v>278</v>
+        <v>243</v>
       </c>
     </row>
     <row r="159" spans="1:19" customHeight="1" ht="14.25">
@@ -10286,7 +9980,7 @@
       <c r="M159" s="108"/>
       <c r="N159" s="108"/>
       <c r="Q159" s="3" t="s">
-        <v>279</v>
+        <v>244</v>
       </c>
     </row>
     <row r="160" spans="1:19" customHeight="1" ht="14.25">
@@ -10305,7 +9999,7 @@
       <c r="M160" s="108"/>
       <c r="N160" s="108"/>
       <c r="Q160" s="3" t="s">
-        <v>280</v>
+        <v>245</v>
       </c>
     </row>
     <row r="161" spans="1:19" customHeight="1" ht="14.25">
@@ -10324,7 +10018,7 @@
       <c r="M161" s="108"/>
       <c r="N161" s="108"/>
       <c r="Q161" s="3" t="s">
-        <v>281</v>
+        <v>246</v>
       </c>
     </row>
     <row r="162" spans="1:19" customHeight="1" ht="14.25">
@@ -10343,7 +10037,7 @@
       <c r="M162" s="108"/>
       <c r="N162" s="108"/>
       <c r="Q162" s="3" t="s">
-        <v>282</v>
+        <v>247</v>
       </c>
     </row>
     <row r="163" spans="1:19" customHeight="1" ht="14.25">
@@ -10362,7 +10056,7 @@
       <c r="M163" s="108"/>
       <c r="N163" s="108"/>
       <c r="Q163" s="3" t="s">
-        <v>283</v>
+        <v>248</v>
       </c>
     </row>
     <row r="164" spans="1:19" customHeight="1" ht="14.25">
@@ -10381,7 +10075,7 @@
       <c r="M164" s="108"/>
       <c r="N164" s="108"/>
       <c r="Q164" s="3" t="s">
-        <v>284</v>
+        <v>249</v>
       </c>
     </row>
     <row r="165" spans="1:19" customHeight="1" ht="28.5">
@@ -10400,7 +10094,7 @@
       <c r="M165" s="108"/>
       <c r="N165" s="108"/>
       <c r="Q165" s="3" t="s">
-        <v>285</v>
+        <v>250</v>
       </c>
     </row>
     <row r="166" spans="1:19" customHeight="1" ht="14.25">
@@ -10419,7 +10113,7 @@
       <c r="M166" s="108"/>
       <c r="N166" s="108"/>
       <c r="Q166" s="3" t="s">
-        <v>286</v>
+        <v>251</v>
       </c>
     </row>
     <row r="167" spans="1:19" customHeight="1" ht="42.75">
@@ -10438,7 +10132,7 @@
       <c r="M167" s="108"/>
       <c r="N167" s="108"/>
       <c r="Q167" s="3" t="s">
-        <v>287</v>
+        <v>252</v>
       </c>
     </row>
     <row r="168" spans="1:19" customHeight="1" ht="14.25">
@@ -10457,7 +10151,7 @@
       <c r="M168" s="108"/>
       <c r="N168" s="108"/>
       <c r="Q168" s="3" t="s">
-        <v>288</v>
+        <v>253</v>
       </c>
     </row>
     <row r="169" spans="1:19" customHeight="1" ht="14.25">
@@ -10476,7 +10170,7 @@
       <c r="M169" s="108"/>
       <c r="N169" s="108"/>
       <c r="Q169" s="3" t="s">
-        <v>289</v>
+        <v>254</v>
       </c>
     </row>
     <row r="170" spans="1:19" customHeight="1" ht="28.5">
@@ -10495,7 +10189,7 @@
       <c r="M170" s="108"/>
       <c r="N170" s="108"/>
       <c r="Q170" s="3" t="s">
-        <v>290</v>
+        <v>255</v>
       </c>
     </row>
     <row r="171" spans="1:19" customHeight="1" ht="14.25">
@@ -10514,7 +10208,7 @@
       <c r="M171" s="108"/>
       <c r="N171" s="108"/>
       <c r="Q171" s="3" t="s">
-        <v>291</v>
+        <v>256</v>
       </c>
     </row>
     <row r="172" spans="1:19" customHeight="1" ht="14.25">
@@ -10533,7 +10227,7 @@
       <c r="M172" s="108"/>
       <c r="N172" s="108"/>
       <c r="Q172" s="3" t="s">
-        <v>292</v>
+        <v>257</v>
       </c>
     </row>
     <row r="173" spans="1:19" customHeight="1" ht="14.25">
@@ -10552,7 +10246,7 @@
       <c r="M173" s="108"/>
       <c r="N173" s="108"/>
       <c r="Q173" s="3" t="s">
-        <v>293</v>
+        <v>258</v>
       </c>
     </row>
     <row r="174" spans="1:19" customHeight="1" ht="14.25">
@@ -10571,7 +10265,7 @@
       <c r="M174" s="108"/>
       <c r="N174" s="108"/>
       <c r="Q174" s="3" t="s">
-        <v>294</v>
+        <v>259</v>
       </c>
     </row>
     <row r="175" spans="1:19" customHeight="1" ht="14.25">
@@ -10590,7 +10284,7 @@
       <c r="M175" s="108"/>
       <c r="N175" s="108"/>
       <c r="Q175" s="3" t="s">
-        <v>295</v>
+        <v>260</v>
       </c>
     </row>
     <row r="176" spans="1:19" customHeight="1" ht="14.25">
@@ -10609,7 +10303,7 @@
       <c r="M176" s="108"/>
       <c r="N176" s="108"/>
       <c r="Q176" s="3" t="s">
-        <v>296</v>
+        <v>261</v>
       </c>
     </row>
     <row r="177" spans="1:19" customHeight="1" ht="14.25">
@@ -10628,7 +10322,7 @@
       <c r="M177" s="108"/>
       <c r="N177" s="108"/>
       <c r="Q177" s="3" t="s">
-        <v>297</v>
+        <v>262</v>
       </c>
     </row>
     <row r="178" spans="1:19" customHeight="1" ht="14.25">
@@ -10647,7 +10341,7 @@
       <c r="M178" s="108"/>
       <c r="N178" s="108"/>
       <c r="Q178" s="3" t="s">
-        <v>298</v>
+        <v>263</v>
       </c>
     </row>
     <row r="179" spans="1:19" customHeight="1" ht="14.25">
@@ -10666,7 +10360,7 @@
       <c r="M179" s="108"/>
       <c r="N179" s="108"/>
       <c r="Q179" s="3" t="s">
-        <v>299</v>
+        <v>264</v>
       </c>
     </row>
     <row r="180" spans="1:19" customHeight="1" ht="28.5">
@@ -10685,7 +10379,7 @@
       <c r="M180" s="108"/>
       <c r="N180" s="108"/>
       <c r="Q180" s="3" t="s">
-        <v>300</v>
+        <v>265</v>
       </c>
     </row>
     <row r="181" spans="1:19" customHeight="1" ht="14.25">
@@ -10704,7 +10398,7 @@
       <c r="M181" s="108"/>
       <c r="N181" s="108"/>
       <c r="Q181" s="3" t="s">
-        <v>301</v>
+        <v>266</v>
       </c>
     </row>
     <row r="182" spans="1:19" customHeight="1" ht="14.25">
@@ -10723,7 +10417,7 @@
       <c r="M182" s="108"/>
       <c r="N182" s="108"/>
       <c r="Q182" s="3" t="s">
-        <v>302</v>
+        <v>267</v>
       </c>
     </row>
     <row r="183" spans="1:19" customHeight="1" ht="14.25">
@@ -10742,7 +10436,7 @@
       <c r="M183" s="108"/>
       <c r="N183" s="108"/>
       <c r="Q183" s="3" t="s">
-        <v>303</v>
+        <v>268</v>
       </c>
     </row>
     <row r="184" spans="1:19" customHeight="1" ht="14.25">
@@ -10761,7 +10455,7 @@
       <c r="M184" s="108"/>
       <c r="N184" s="108"/>
       <c r="Q184" s="3" t="s">
-        <v>304</v>
+        <v>269</v>
       </c>
     </row>
     <row r="185" spans="1:19" customHeight="1" ht="14.25">
@@ -10780,7 +10474,7 @@
       <c r="M185" s="108"/>
       <c r="N185" s="108"/>
       <c r="Q185" s="3" t="s">
-        <v>305</v>
+        <v>270</v>
       </c>
     </row>
     <row r="186" spans="1:19" customHeight="1" ht="14.25">
@@ -10799,7 +10493,7 @@
       <c r="M186" s="108"/>
       <c r="N186" s="108"/>
       <c r="Q186" s="3" t="s">
-        <v>306</v>
+        <v>271</v>
       </c>
     </row>
     <row r="187" spans="1:19" customHeight="1" ht="14.25">
@@ -10818,7 +10512,7 @@
       <c r="M187" s="108"/>
       <c r="N187" s="108"/>
       <c r="Q187" s="3" t="s">
-        <v>307</v>
+        <v>272</v>
       </c>
     </row>
     <row r="188" spans="1:19" customHeight="1" ht="14.25">
@@ -10837,7 +10531,7 @@
       <c r="M188" s="108"/>
       <c r="N188" s="108"/>
       <c r="Q188" s="3" t="s">
-        <v>308</v>
+        <v>273</v>
       </c>
     </row>
     <row r="189" spans="1:19" customHeight="1" ht="14.25">
@@ -10856,7 +10550,7 @@
       <c r="M189" s="108"/>
       <c r="N189" s="108"/>
       <c r="Q189" s="3" t="s">
-        <v>309</v>
+        <v>274</v>
       </c>
     </row>
     <row r="190" spans="1:19" customHeight="1" ht="14.25">
@@ -10875,7 +10569,7 @@
       <c r="M190" s="108"/>
       <c r="N190" s="108"/>
       <c r="Q190" s="3" t="s">
-        <v>310</v>
+        <v>275</v>
       </c>
     </row>
     <row r="191" spans="1:19" customHeight="1" ht="14.25">
@@ -10894,7 +10588,7 @@
       <c r="M191" s="108"/>
       <c r="N191" s="108"/>
       <c r="Q191" s="3" t="s">
-        <v>311</v>
+        <v>276</v>
       </c>
     </row>
     <row r="192" spans="1:19" customHeight="1" ht="14.25">
@@ -10913,7 +10607,7 @@
       <c r="M192" s="108"/>
       <c r="N192" s="108"/>
       <c r="Q192" s="3" t="s">
-        <v>312</v>
+        <v>277</v>
       </c>
     </row>
     <row r="193" spans="1:19" customHeight="1" ht="14.25">
@@ -10932,7 +10626,7 @@
       <c r="M193" s="108"/>
       <c r="N193" s="108"/>
       <c r="Q193" s="3" t="s">
-        <v>313</v>
+        <v>278</v>
       </c>
     </row>
     <row r="194" spans="1:19" customHeight="1" ht="14.25">
@@ -10951,7 +10645,7 @@
       <c r="M194" s="108"/>
       <c r="N194" s="108"/>
       <c r="Q194" s="3" t="s">
-        <v>314</v>
+        <v>279</v>
       </c>
     </row>
     <row r="195" spans="1:19" customHeight="1" ht="14.25">
@@ -10970,7 +10664,7 @@
       <c r="M195" s="108"/>
       <c r="N195" s="108"/>
       <c r="Q195" s="3" t="s">
-        <v>315</v>
+        <v>280</v>
       </c>
     </row>
     <row r="196" spans="1:19" customHeight="1" ht="14.25">
@@ -10989,7 +10683,7 @@
       <c r="M196" s="108"/>
       <c r="N196" s="108"/>
       <c r="Q196" s="3" t="s">
-        <v>316</v>
+        <v>281</v>
       </c>
     </row>
     <row r="197" spans="1:19" customHeight="1" ht="14.25">
@@ -11008,7 +10702,7 @@
       <c r="M197" s="108"/>
       <c r="N197" s="108"/>
       <c r="Q197" s="3" t="s">
-        <v>317</v>
+        <v>282</v>
       </c>
     </row>
     <row r="198" spans="1:19" customHeight="1" ht="14.25">
@@ -11027,7 +10721,7 @@
       <c r="M198" s="108"/>
       <c r="N198" s="108"/>
       <c r="Q198" s="3" t="s">
-        <v>318</v>
+        <v>283</v>
       </c>
     </row>
     <row r="199" spans="1:19" customHeight="1" ht="14.25">
@@ -11046,7 +10740,7 @@
       <c r="M199" s="108"/>
       <c r="N199" s="108"/>
       <c r="Q199" s="3" t="s">
-        <v>319</v>
+        <v>284</v>
       </c>
     </row>
     <row r="200" spans="1:19" customHeight="1" ht="28.5">
@@ -11065,7 +10759,7 @@
       <c r="M200" s="108"/>
       <c r="N200" s="108"/>
       <c r="Q200" s="3" t="s">
-        <v>320</v>
+        <v>285</v>
       </c>
     </row>
     <row r="201" spans="1:19" customHeight="1" ht="14.25">
@@ -11084,7 +10778,7 @@
       <c r="M201" s="108"/>
       <c r="N201" s="108"/>
       <c r="Q201" s="3" t="s">
-        <v>321</v>
+        <v>286</v>
       </c>
     </row>
     <row r="202" spans="1:19" customHeight="1" ht="14.25">
@@ -11103,7 +10797,7 @@
       <c r="M202" s="108"/>
       <c r="N202" s="108"/>
       <c r="Q202" s="3" t="s">
-        <v>322</v>
+        <v>287</v>
       </c>
     </row>
     <row r="203" spans="1:19" customHeight="1" ht="14.25">
@@ -11122,7 +10816,7 @@
       <c r="M203" s="108"/>
       <c r="N203" s="108"/>
       <c r="Q203" s="3" t="s">
-        <v>323</v>
+        <v>288</v>
       </c>
     </row>
     <row r="204" spans="1:19" customHeight="1" ht="14.25">
@@ -11141,7 +10835,7 @@
       <c r="M204" s="108"/>
       <c r="N204" s="108"/>
       <c r="Q204" s="3" t="s">
-        <v>324</v>
+        <v>289</v>
       </c>
     </row>
     <row r="205" spans="1:19" customHeight="1" ht="14.25">
@@ -11160,7 +10854,7 @@
       <c r="M205" s="108"/>
       <c r="N205" s="108"/>
       <c r="Q205" s="3" t="s">
-        <v>325</v>
+        <v>290</v>
       </c>
     </row>
     <row r="206" spans="1:19" customHeight="1" ht="14.25">
@@ -11179,7 +10873,7 @@
       <c r="M206" s="108"/>
       <c r="N206" s="108"/>
       <c r="Q206" s="3" t="s">
-        <v>326</v>
+        <v>291</v>
       </c>
     </row>
     <row r="207" spans="1:19" customHeight="1" ht="28.5">
@@ -11198,7 +10892,7 @@
       <c r="M207" s="108"/>
       <c r="N207" s="108"/>
       <c r="Q207" s="3" t="s">
-        <v>327</v>
+        <v>292</v>
       </c>
     </row>
     <row r="208" spans="1:19" customHeight="1" ht="28.5">
@@ -11217,7 +10911,7 @@
       <c r="M208" s="108"/>
       <c r="N208" s="108"/>
       <c r="Q208" s="3" t="s">
-        <v>328</v>
+        <v>293</v>
       </c>
     </row>
     <row r="209" spans="1:19" customHeight="1" ht="14.25">
@@ -11236,7 +10930,7 @@
       <c r="M209" s="108"/>
       <c r="N209" s="108"/>
       <c r="Q209" s="3" t="s">
-        <v>329</v>
+        <v>294</v>
       </c>
     </row>
     <row r="210" spans="1:19" customHeight="1" ht="14.25">
@@ -11255,7 +10949,7 @@
       <c r="M210" s="108"/>
       <c r="N210" s="108"/>
       <c r="Q210" s="3" t="s">
-        <v>330</v>
+        <v>295</v>
       </c>
     </row>
     <row r="211" spans="1:19" customHeight="1" ht="14.25">
@@ -11274,7 +10968,7 @@
       <c r="M211" s="108"/>
       <c r="N211" s="108"/>
       <c r="Q211" s="3" t="s">
-        <v>331</v>
+        <v>296</v>
       </c>
     </row>
     <row r="212" spans="1:19" customHeight="1" ht="14.25">
@@ -11293,7 +10987,7 @@
       <c r="M212" s="108"/>
       <c r="N212" s="108"/>
       <c r="Q212" s="3" t="s">
-        <v>332</v>
+        <v>297</v>
       </c>
     </row>
     <row r="213" spans="1:19" customHeight="1" ht="14.25">
@@ -11312,7 +11006,7 @@
       <c r="M213" s="108"/>
       <c r="N213" s="108"/>
       <c r="Q213" s="3" t="s">
-        <v>333</v>
+        <v>298</v>
       </c>
     </row>
     <row r="214" spans="1:19" customHeight="1" ht="14.25">
@@ -11331,7 +11025,7 @@
       <c r="M214" s="108"/>
       <c r="N214" s="108"/>
       <c r="Q214" s="3" t="s">
-        <v>334</v>
+        <v>299</v>
       </c>
     </row>
     <row r="215" spans="1:19" customHeight="1" ht="14.25">
@@ -11350,7 +11044,7 @@
       <c r="M215" s="108"/>
       <c r="N215" s="108"/>
       <c r="Q215" s="3" t="s">
-        <v>335</v>
+        <v>300</v>
       </c>
     </row>
     <row r="216" spans="1:19" customHeight="1" ht="14.25">
@@ -11369,7 +11063,7 @@
       <c r="M216" s="108"/>
       <c r="N216" s="108"/>
       <c r="Q216" s="3" t="s">
-        <v>336</v>
+        <v>301</v>
       </c>
     </row>
     <row r="217" spans="1:19">
@@ -12551,7 +12245,7 @@
     </row>
     <row r="2" spans="1:14" customHeight="1" ht="18">
       <c r="A2" s="514" t="s">
-        <v>337</v>
+        <v>302</v>
       </c>
       <c r="B2" s="515"/>
       <c r="C2" s="515"/>
@@ -12568,28 +12262,28 @@
     </row>
     <row r="3" spans="1:14" customHeight="1" ht="15">
       <c r="A3" s="140" t="s">
-        <v>338</v>
+        <v>303</v>
       </c>
       <c r="B3" s="507" t="s">
-        <v>339</v>
+        <v>304</v>
       </c>
       <c r="C3" s="507"/>
       <c r="D3" s="507"/>
       <c r="E3" s="508"/>
       <c r="F3" s="512" t="s">
-        <v>340</v>
+        <v>305</v>
       </c>
       <c r="G3" s="509" t="s">
-        <v>341</v>
+        <v>306</v>
       </c>
       <c r="H3" s="508"/>
       <c r="I3" s="509" t="s">
-        <v>342</v>
+        <v>307</v>
       </c>
       <c r="J3" s="507"/>
       <c r="K3" s="508"/>
       <c r="L3" s="510" t="s">
-        <v>343</v>
+        <v>308</v>
       </c>
       <c r="M3" s="511"/>
     </row>
@@ -12606,36 +12300,26 @@
       <c r="J4" s="483"/>
       <c r="K4" s="484"/>
       <c r="L4" s="5" t="s">
-        <v>344</v>
+        <v>309</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>345</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:14" customHeight="1" ht="27">
-      <c r="A5" s="493" t="s">
-        <v>346</v>
-      </c>
+      <c r="A5" s="493"/>
       <c r="B5" s="468"/>
       <c r="C5" s="468"/>
       <c r="D5" s="468"/>
       <c r="E5" s="468"/>
-      <c r="F5" s="16">
-        <v>80</v>
-      </c>
-      <c r="G5" s="492" t="s">
-        <v>347</v>
-      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="492"/>
       <c r="H5" s="492"/>
       <c r="I5" s="496"/>
       <c r="J5" s="496"/>
       <c r="K5" s="496"/>
-      <c r="L5" s="9">
-        <v>123456</v>
-      </c>
-      <c r="M5" s="22" t="s">
-        <v>348</v>
-      </c>
+      <c r="L5" s="9"/>
+      <c r="M5" s="22"/>
     </row>
     <row r="6" spans="1:14" customHeight="1" ht="27">
       <c r="A6" s="493"/>
@@ -12729,38 +12413,24 @@
     </row>
     <row r="12" spans="1:14" customHeight="1" ht="12">
       <c r="A12" s="485" t="s">
-        <v>349</v>
+        <v>113</v>
       </c>
       <c r="B12" s="486"/>
-      <c r="C12" s="486" t="s">
-        <v>350</v>
-      </c>
-      <c r="D12" s="486" t="s">
-        <v>351</v>
-      </c>
+      <c r="C12" s="486"/>
+      <c r="D12" s="486"/>
       <c r="E12" s="486"/>
       <c r="F12" s="486"/>
-      <c r="G12" s="486" t="s">
-        <v>352</v>
-      </c>
+      <c r="G12" s="486"/>
       <c r="H12" s="486"/>
       <c r="I12" s="486"/>
-      <c r="J12" s="486">
-        <v>200000.0</v>
-      </c>
-      <c r="K12" s="486">
-        <v>30</v>
-      </c>
-      <c r="L12" s="486" t="s">
-        <v>353</v>
-      </c>
-      <c r="M12" s="487" t="s">
-        <v>354</v>
-      </c>
+      <c r="J12" s="486"/>
+      <c r="K12" s="486"/>
+      <c r="L12" s="486"/>
+      <c r="M12" s="487"/>
     </row>
     <row r="13" spans="1:14" customHeight="1" ht="18">
       <c r="A13" s="488" t="s">
-        <v>355</v>
+        <v>311</v>
       </c>
       <c r="B13" s="489"/>
       <c r="C13" s="489"/>
@@ -12777,7 +12447,7 @@
     </row>
     <row r="14" spans="1:14" customHeight="1" ht="12">
       <c r="A14" s="202" t="s">
-        <v>356</v>
+        <v>312</v>
       </c>
       <c r="B14" s="101"/>
       <c r="C14" s="101"/>
@@ -12794,33 +12464,33 @@
     </row>
     <row r="15" spans="1:14" customHeight="1" ht="18">
       <c r="A15" s="4" t="s">
-        <v>357</v>
+        <v>313</v>
       </c>
       <c r="B15" s="481" t="s">
-        <v>358</v>
+        <v>314</v>
       </c>
       <c r="C15" s="482"/>
       <c r="D15" s="494" t="s">
-        <v>359</v>
+        <v>315</v>
       </c>
       <c r="E15" s="481"/>
       <c r="F15" s="482"/>
       <c r="G15" s="494" t="s">
-        <v>360</v>
+        <v>316</v>
       </c>
       <c r="H15" s="481"/>
       <c r="I15" s="482"/>
       <c r="J15" s="498" t="s">
-        <v>361</v>
+        <v>317</v>
       </c>
       <c r="K15" s="519" t="s">
-        <v>362</v>
+        <v>318</v>
       </c>
       <c r="L15" s="473" t="s">
-        <v>363</v>
+        <v>319</v>
       </c>
       <c r="M15" s="517" t="s">
-        <v>364</v>
+        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:14" customHeight="1" ht="15">
@@ -12840,11 +12510,11 @@
     </row>
     <row r="17" spans="1:14" customHeight="1" ht="18.75">
       <c r="A17" s="521" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
       <c r="B17" s="522"/>
       <c r="C17" s="8" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="D17" s="495"/>
       <c r="E17" s="483"/>
@@ -13279,7 +12949,7 @@
     </row>
     <row r="46" spans="1:14" customHeight="1" ht="9.75">
       <c r="A46" s="476" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
       <c r="B46" s="477"/>
       <c r="C46" s="477"/>
@@ -13296,7 +12966,7 @@
     </row>
     <row r="47" spans="1:14" customHeight="1" ht="27.75">
       <c r="A47" s="445" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="B47" s="446"/>
       <c r="C47" s="447"/>
@@ -13306,7 +12976,7 @@
       <c r="G47" s="502"/>
       <c r="H47" s="503"/>
       <c r="I47" s="228" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="J47" s="229"/>
       <c r="K47" s="230"/>
@@ -13316,7 +12986,7 @@
     </row>
     <row r="48" spans="1:14" customHeight="1" ht="9">
       <c r="A48" s="500" t="s">
-        <v>365</v>
+        <v>321</v>
       </c>
       <c r="B48" s="500"/>
       <c r="C48" s="500"/>
@@ -13520,7 +13190,7 @@
     </row>
     <row r="2" spans="1:13" customHeight="1" ht="22.5">
       <c r="A2" s="571" t="s">
-        <v>366</v>
+        <v>322</v>
       </c>
       <c r="B2" s="572"/>
       <c r="C2" s="572"/>
@@ -13535,22 +13205,22 @@
     </row>
     <row r="3" spans="1:13" customHeight="1" ht="15">
       <c r="A3" s="555" t="s">
-        <v>367</v>
+        <v>323</v>
       </c>
       <c r="B3" s="556" t="s">
-        <v>368</v>
+        <v>324</v>
       </c>
       <c r="C3" s="556"/>
       <c r="D3" s="557"/>
       <c r="E3" s="507" t="s">
-        <v>369</v>
+        <v>325</v>
       </c>
       <c r="F3" s="508"/>
       <c r="G3" s="576" t="s">
-        <v>370</v>
+        <v>326</v>
       </c>
       <c r="H3" s="509" t="s">
-        <v>371</v>
+        <v>327</v>
       </c>
       <c r="I3" s="566"/>
       <c r="J3" s="566"/>
@@ -13575,10 +13245,10 @@
       <c r="C5" s="574"/>
       <c r="D5" s="575"/>
       <c r="E5" s="27" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="G5" s="520"/>
       <c r="H5" s="570"/>
@@ -13587,24 +13257,14 @@
       <c r="K5" s="432"/>
     </row>
     <row r="6" spans="1:13" customHeight="1" ht="27.75">
-      <c r="A6" s="563" t="s">
-        <v>372</v>
-      </c>
+      <c r="A6" s="563"/>
       <c r="B6" s="564"/>
       <c r="C6" s="564"/>
       <c r="D6" s="565"/>
-      <c r="E6" s="33" t="s">
-        <v>373</v>
-      </c>
-      <c r="F6" s="33" t="s">
-        <v>374</v>
-      </c>
-      <c r="G6" s="34">
-        <v>50</v>
-      </c>
-      <c r="H6" s="552" t="s">
-        <v>375</v>
-      </c>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="552"/>
       <c r="I6" s="553"/>
       <c r="J6" s="553"/>
       <c r="K6" s="554"/>
@@ -13675,33 +13335,21 @@
       <c r="K11" s="554"/>
     </row>
     <row r="12" spans="1:13" customHeight="1" ht="27.75">
-      <c r="A12" s="560" t="s">
-        <v>376</v>
-      </c>
+      <c r="A12" s="560"/>
       <c r="B12" s="561"/>
       <c r="C12" s="561"/>
       <c r="D12" s="562"/>
-      <c r="E12" s="33" t="s">
-        <v>348</v>
-      </c>
-      <c r="F12" s="33" t="s">
-        <v>377</v>
-      </c>
-      <c r="G12" s="35">
-        <v>50</v>
-      </c>
-      <c r="H12" s="525" t="s">
-        <v>378</v>
-      </c>
-      <c r="I12" s="526" t="s">
-        <v>379</v>
-      </c>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="525"/>
+      <c r="I12" s="526"/>
       <c r="J12" s="526"/>
       <c r="K12" s="527"/>
     </row>
     <row r="13" spans="1:13" customHeight="1" ht="11.25">
       <c r="A13" s="485" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
       <c r="B13" s="486"/>
       <c r="C13" s="486"/>
@@ -13716,7 +13364,7 @@
     </row>
     <row r="14" spans="1:13" customHeight="1" ht="18">
       <c r="A14" s="528" t="s">
-        <v>380</v>
+        <v>328</v>
       </c>
       <c r="B14" s="529"/>
       <c r="C14" s="529"/>
@@ -13731,25 +13379,25 @@
     </row>
     <row r="15" spans="1:13" customHeight="1" ht="18">
       <c r="A15" s="543" t="s">
-        <v>381</v>
+        <v>329</v>
       </c>
       <c r="B15" s="481" t="s">
-        <v>382</v>
+        <v>330</v>
       </c>
       <c r="C15" s="549"/>
       <c r="D15" s="550"/>
       <c r="E15" s="481" t="s">
-        <v>383</v>
+        <v>331</v>
       </c>
       <c r="F15" s="482"/>
       <c r="G15" s="519" t="s">
-        <v>370</v>
+        <v>326</v>
       </c>
       <c r="H15" s="498" t="s">
-        <v>384</v>
+        <v>332</v>
       </c>
       <c r="I15" s="494" t="s">
-        <v>385</v>
+        <v>333</v>
       </c>
       <c r="J15" s="549"/>
       <c r="K15" s="569"/>
@@ -13773,10 +13421,10 @@
       <c r="C17" s="431"/>
       <c r="D17" s="551"/>
       <c r="E17" s="27" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="G17" s="520"/>
       <c r="H17" s="499"/>
@@ -14059,7 +13707,7 @@
     </row>
     <row r="39" spans="1:13" customHeight="1" ht="13.5">
       <c r="A39" s="448" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
       <c r="B39" s="449"/>
       <c r="C39" s="449"/>
@@ -14074,7 +13722,7 @@
     </row>
     <row r="40" spans="1:13" customHeight="1" ht="22.5">
       <c r="A40" s="585" t="s">
-        <v>386</v>
+        <v>334</v>
       </c>
       <c r="B40" s="586"/>
       <c r="C40" s="586"/>
@@ -14089,26 +13737,26 @@
     </row>
     <row r="41" spans="1:13" customHeight="1" ht="33.75">
       <c r="A41" s="141" t="s">
-        <v>387</v>
+        <v>335</v>
       </c>
       <c r="B41" s="146" t="s">
-        <v>388</v>
+        <v>336</v>
       </c>
       <c r="C41" s="142" t="s">
-        <v>389</v>
+        <v>337</v>
       </c>
       <c r="D41" s="577" t="s">
-        <v>390</v>
+        <v>338</v>
       </c>
       <c r="E41" s="577"/>
       <c r="F41" s="577"/>
       <c r="G41" s="577"/>
       <c r="H41" s="578"/>
       <c r="I41" s="142" t="s">
-        <v>391</v>
+        <v>339</v>
       </c>
       <c r="J41" s="577" t="s">
-        <v>392</v>
+        <v>340</v>
       </c>
       <c r="K41" s="584"/>
     </row>
@@ -14116,7 +13764,7 @@
       <c r="A42" s="582"/>
       <c r="B42" s="583"/>
       <c r="C42" s="579" t="s">
-        <v>393</v>
+        <v>341</v>
       </c>
       <c r="D42" s="580"/>
       <c r="E42" s="580"/>
@@ -14207,7 +13855,7 @@
     </row>
     <row r="49" spans="1:13" customHeight="1" ht="11.25">
       <c r="A49" s="448" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
       <c r="B49" s="449"/>
       <c r="C49" s="449"/>
@@ -14222,7 +13870,7 @@
     </row>
     <row r="50" spans="1:13" customHeight="1" ht="28.5">
       <c r="A50" s="445" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="B50" s="447"/>
       <c r="C50" s="501"/>
@@ -14230,7 +13878,7 @@
       <c r="E50" s="502"/>
       <c r="F50" s="503"/>
       <c r="G50" s="588" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="H50" s="589"/>
       <c r="I50" s="501"/>
@@ -14241,7 +13889,7 @@
     </row>
     <row r="51" spans="1:13" customHeight="1" ht="9.75">
       <c r="K51" s="236" t="s">
-        <v>394</v>
+        <v>342</v>
       </c>
     </row>
     <row r="52" spans="1:13" customHeight="1" ht="3"/>
@@ -14411,11 +14059,11 @@
     </row>
     <row r="2" spans="1:14" customHeight="1" ht="13.5">
       <c r="A2" s="624" t="s">
-        <v>395</v>
+        <v>343</v>
       </c>
       <c r="B2" s="625"/>
       <c r="C2" s="603" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
       <c r="D2" s="603"/>
       <c r="E2" s="603"/>
@@ -14432,7 +14080,7 @@
       <c r="A3" s="39"/>
       <c r="B3" s="40"/>
       <c r="C3" s="607" t="s">
-        <v>397</v>
+        <v>345</v>
       </c>
       <c r="D3" s="607"/>
       <c r="E3" s="607"/>
@@ -14449,7 +14097,7 @@
       <c r="A4" s="39"/>
       <c r="B4" s="40"/>
       <c r="C4" s="607" t="s">
-        <v>398</v>
+        <v>346</v>
       </c>
       <c r="D4" s="607"/>
       <c r="E4" s="607"/>
@@ -14475,14 +14123,12 @@
       <c r="A6" s="39"/>
       <c r="B6" s="40"/>
       <c r="C6" s="607" t="s">
-        <v>399</v>
+        <v>347</v>
       </c>
       <c r="D6" s="607"/>
       <c r="E6" s="607"/>
       <c r="F6" s="608"/>
-      <c r="G6" s="629" t="s">
-        <v>400</v>
-      </c>
+      <c r="G6" s="629"/>
       <c r="H6" s="630"/>
       <c r="I6" s="630"/>
       <c r="J6" s="630"/>
@@ -14509,14 +14155,12 @@
       <c r="A8" s="39"/>
       <c r="B8" s="40"/>
       <c r="C8" s="607" t="s">
-        <v>401</v>
+        <v>348</v>
       </c>
       <c r="D8" s="607"/>
       <c r="E8" s="607"/>
       <c r="F8" s="608"/>
-      <c r="G8" s="632" t="s">
-        <v>400</v>
-      </c>
+      <c r="G8" s="632"/>
       <c r="H8" s="633"/>
       <c r="I8" s="633"/>
       <c r="J8" s="633"/>
@@ -14541,7 +14185,7 @@
       <c r="E10" s="607"/>
       <c r="F10" s="608"/>
       <c r="G10" s="592" t="s">
-        <v>402</v>
+        <v>349</v>
       </c>
       <c r="H10" s="592"/>
       <c r="I10" s="592"/>
@@ -14582,18 +14226,16 @@
     </row>
     <row r="13" spans="1:14" customHeight="1" ht="18">
       <c r="A13" s="622" t="s">
-        <v>403</v>
+        <v>350</v>
       </c>
       <c r="B13" s="623"/>
       <c r="C13" s="590" t="s">
-        <v>404</v>
+        <v>351</v>
       </c>
       <c r="D13" s="590"/>
       <c r="E13" s="549"/>
       <c r="F13" s="550"/>
-      <c r="G13" s="594" t="s">
-        <v>400</v>
-      </c>
+      <c r="G13" s="594"/>
       <c r="H13" s="595"/>
       <c r="I13" s="595"/>
       <c r="J13" s="595"/>
@@ -14609,7 +14251,7 @@
       <c r="E14" s="549"/>
       <c r="F14" s="550"/>
       <c r="G14" s="591" t="s">
-        <v>402</v>
+        <v>349</v>
       </c>
       <c r="H14" s="592"/>
       <c r="I14" s="592"/>
@@ -14667,14 +14309,12 @@
       <c r="A18" s="51"/>
       <c r="B18" s="52"/>
       <c r="C18" s="737" t="s">
-        <v>405</v>
+        <v>352</v>
       </c>
       <c r="D18" s="737"/>
       <c r="E18" s="738"/>
       <c r="F18" s="739"/>
-      <c r="G18" s="728" t="s">
-        <v>400</v>
-      </c>
+      <c r="G18" s="728"/>
       <c r="H18" s="729"/>
       <c r="I18" s="729"/>
       <c r="J18" s="729"/>
@@ -14690,7 +14330,7 @@
       <c r="E19" s="738"/>
       <c r="F19" s="739"/>
       <c r="G19" s="591" t="s">
-        <v>402</v>
+        <v>349</v>
       </c>
       <c r="H19" s="592"/>
       <c r="I19" s="592"/>
@@ -14708,7 +14348,7 @@
       <c r="F20" s="739"/>
       <c r="G20" s="56"/>
       <c r="H20" s="733" t="s">
-        <v>406</v>
+        <v>353</v>
       </c>
       <c r="I20" s="733"/>
       <c r="J20" s="246"/>
@@ -14724,7 +14364,7 @@
       <c r="E21" s="738"/>
       <c r="F21" s="739"/>
       <c r="G21" s="734" t="s">
-        <v>407</v>
+        <v>354</v>
       </c>
       <c r="H21" s="735"/>
       <c r="I21" s="735"/>
@@ -14741,7 +14381,7 @@
       <c r="E22" s="740"/>
       <c r="F22" s="741"/>
       <c r="G22" s="125" t="s">
-        <v>408</v>
+        <v>355</v>
       </c>
       <c r="H22" s="237"/>
       <c r="I22" s="685"/>
@@ -14752,18 +14392,16 @@
     </row>
     <row r="23" spans="1:14" customHeight="1" ht="18">
       <c r="A23" s="636" t="s">
-        <v>409</v>
+        <v>356</v>
       </c>
       <c r="B23" s="637"/>
       <c r="C23" s="618" t="s">
-        <v>410</v>
+        <v>357</v>
       </c>
       <c r="D23" s="618"/>
       <c r="E23" s="618"/>
       <c r="F23" s="619"/>
-      <c r="G23" s="594" t="s">
-        <v>400</v>
-      </c>
+      <c r="G23" s="594"/>
       <c r="H23" s="595"/>
       <c r="I23" s="595"/>
       <c r="J23" s="595"/>
@@ -14779,7 +14417,7 @@
       <c r="E24" s="610"/>
       <c r="F24" s="609"/>
       <c r="G24" s="591" t="s">
-        <v>402</v>
+        <v>349</v>
       </c>
       <c r="H24" s="592"/>
       <c r="I24" s="592"/>
@@ -14820,18 +14458,16 @@
     </row>
     <row r="27" spans="1:14" customHeight="1" ht="14.25">
       <c r="A27" s="636" t="s">
-        <v>411</v>
+        <v>358</v>
       </c>
       <c r="B27" s="637"/>
       <c r="C27" s="618" t="s">
-        <v>412</v>
+        <v>359</v>
       </c>
       <c r="D27" s="618"/>
       <c r="E27" s="618"/>
       <c r="F27" s="619"/>
-      <c r="G27" s="594" t="s">
-        <v>400</v>
-      </c>
+      <c r="G27" s="594"/>
       <c r="H27" s="595"/>
       <c r="I27" s="595"/>
       <c r="J27" s="595"/>
@@ -14847,7 +14483,7 @@
       <c r="E28" s="610"/>
       <c r="F28" s="609"/>
       <c r="G28" s="591" t="s">
-        <v>402</v>
+        <v>349</v>
       </c>
       <c r="H28" s="592"/>
       <c r="I28" s="592"/>
@@ -14887,18 +14523,16 @@
     </row>
     <row r="31" spans="1:14" customHeight="1" ht="18">
       <c r="A31" s="636" t="s">
-        <v>413</v>
+        <v>360</v>
       </c>
       <c r="B31" s="637"/>
       <c r="C31" s="618" t="s">
-        <v>414</v>
+        <v>361</v>
       </c>
       <c r="D31" s="618"/>
       <c r="E31" s="618"/>
       <c r="F31" s="619"/>
-      <c r="G31" s="594" t="s">
-        <v>400</v>
-      </c>
+      <c r="G31" s="594"/>
       <c r="H31" s="595"/>
       <c r="I31" s="595"/>
       <c r="J31" s="595"/>
@@ -14914,7 +14548,7 @@
       <c r="E32" s="610"/>
       <c r="F32" s="609"/>
       <c r="G32" s="672" t="s">
-        <v>415</v>
+        <v>362</v>
       </c>
       <c r="H32" s="673"/>
       <c r="I32" s="673"/>
@@ -14942,14 +14576,12 @@
       <c r="A34" s="49"/>
       <c r="B34" s="50"/>
       <c r="C34" s="610" t="s">
-        <v>416</v>
+        <v>363</v>
       </c>
       <c r="D34" s="610"/>
       <c r="E34" s="610"/>
       <c r="F34" s="609"/>
-      <c r="G34" s="674" t="s">
-        <v>400</v>
-      </c>
+      <c r="G34" s="674"/>
       <c r="H34" s="675"/>
       <c r="I34" s="675"/>
       <c r="J34" s="675"/>
@@ -14965,7 +14597,7 @@
       <c r="E35" s="610"/>
       <c r="F35" s="609"/>
       <c r="G35" s="672" t="s">
-        <v>415</v>
+        <v>362</v>
       </c>
       <c r="H35" s="673"/>
       <c r="I35" s="673"/>
@@ -14990,18 +14622,16 @@
     </row>
     <row r="37" spans="1:14" customHeight="1" ht="18">
       <c r="A37" s="636" t="s">
-        <v>417</v>
+        <v>364</v>
       </c>
       <c r="B37" s="637"/>
       <c r="C37" s="613" t="s">
-        <v>418</v>
+        <v>365</v>
       </c>
       <c r="D37" s="613"/>
       <c r="E37" s="613"/>
       <c r="F37" s="614"/>
-      <c r="G37" s="594" t="s">
-        <v>400</v>
-      </c>
+      <c r="G37" s="594"/>
       <c r="H37" s="595"/>
       <c r="I37" s="595"/>
       <c r="J37" s="595"/>
@@ -15017,7 +14647,7 @@
       <c r="E38" s="590"/>
       <c r="F38" s="615"/>
       <c r="G38" s="591" t="s">
-        <v>419</v>
+        <v>366</v>
       </c>
       <c r="H38" s="592"/>
       <c r="I38" s="592"/>
@@ -15058,11 +14688,11 @@
     </row>
     <row r="41" spans="1:14" customHeight="1" ht="28.5">
       <c r="A41" s="611" t="s">
-        <v>420</v>
+        <v>367</v>
       </c>
       <c r="B41" s="612"/>
       <c r="C41" s="610" t="s">
-        <v>421</v>
+        <v>368</v>
       </c>
       <c r="D41" s="610"/>
       <c r="E41" s="610"/>
@@ -15092,18 +14722,16 @@
     </row>
     <row r="43" spans="1:14" customHeight="1" ht="13.5">
       <c r="A43" s="64" t="s">
-        <v>422</v>
+        <v>369</v>
       </c>
       <c r="B43" s="65"/>
       <c r="C43" s="610" t="s">
-        <v>423</v>
+        <v>370</v>
       </c>
       <c r="D43" s="610"/>
       <c r="E43" s="610"/>
       <c r="F43" s="609"/>
-      <c r="G43" s="632" t="s">
-        <v>400</v>
-      </c>
+      <c r="G43" s="632"/>
       <c r="H43" s="633"/>
       <c r="I43" s="633"/>
       <c r="J43" s="633"/>
@@ -15119,7 +14747,7 @@
       <c r="E44" s="610"/>
       <c r="F44" s="609"/>
       <c r="G44" s="187" t="s">
-        <v>424</v>
+        <v>371</v>
       </c>
       <c r="H44" s="239"/>
       <c r="I44" s="118"/>
@@ -15130,18 +14758,16 @@
     </row>
     <row r="45" spans="1:14" customHeight="1" ht="13.5">
       <c r="A45" s="64" t="s">
-        <v>425</v>
+        <v>372</v>
       </c>
       <c r="B45" s="65"/>
       <c r="C45" s="609" t="s">
-        <v>426</v>
+        <v>373</v>
       </c>
       <c r="D45" s="609"/>
       <c r="E45" s="609"/>
       <c r="F45" s="609"/>
-      <c r="G45" s="632" t="s">
-        <v>400</v>
-      </c>
+      <c r="G45" s="632"/>
       <c r="H45" s="633"/>
       <c r="I45" s="633"/>
       <c r="J45" s="633"/>
@@ -15157,7 +14783,7 @@
       <c r="E46" s="609"/>
       <c r="F46" s="609"/>
       <c r="G46" s="188" t="s">
-        <v>427</v>
+        <v>374</v>
       </c>
       <c r="H46" s="240"/>
       <c r="I46" s="118"/>
@@ -15169,18 +14795,16 @@
     </row>
     <row r="47" spans="1:14" customHeight="1" ht="13.5">
       <c r="A47" s="64" t="s">
-        <v>428</v>
+        <v>375</v>
       </c>
       <c r="B47" s="65"/>
       <c r="C47" s="610" t="s">
-        <v>429</v>
+        <v>376</v>
       </c>
       <c r="D47" s="610"/>
       <c r="E47" s="115"/>
       <c r="F47" s="116"/>
-      <c r="G47" s="632" t="s">
-        <v>400</v>
-      </c>
+      <c r="G47" s="632"/>
       <c r="H47" s="633"/>
       <c r="I47" s="633"/>
       <c r="J47" s="633"/>
@@ -15196,7 +14820,7 @@
       <c r="E48" s="652"/>
       <c r="F48" s="653"/>
       <c r="G48" s="189" t="s">
-        <v>427</v>
+        <v>374</v>
       </c>
       <c r="H48" s="241"/>
       <c r="I48" s="120"/>
@@ -15224,11 +14848,11 @@
     </row>
     <row r="50" spans="1:14" customHeight="1" ht="23.25">
       <c r="A50" s="725" t="s">
-        <v>430</v>
+        <v>377</v>
       </c>
       <c r="B50" s="726"/>
       <c r="C50" s="185" t="s">
-        <v>431</v>
+        <v>378</v>
       </c>
       <c r="D50" s="185"/>
       <c r="E50" s="185"/>
@@ -15243,17 +14867,17 @@
     </row>
     <row r="51" spans="1:14" customHeight="1" ht="18">
       <c r="A51" s="648" t="s">
-        <v>432</v>
+        <v>379</v>
       </c>
       <c r="B51" s="649"/>
       <c r="C51" s="649"/>
       <c r="D51" s="649"/>
       <c r="E51" s="650"/>
       <c r="F51" s="177" t="s">
-        <v>433</v>
+        <v>380</v>
       </c>
       <c r="G51" s="657" t="s">
-        <v>434</v>
+        <v>381</v>
       </c>
       <c r="H51" s="577"/>
       <c r="I51" s="584"/>
@@ -15263,19 +14887,13 @@
       <c r="M51" s="644"/>
     </row>
     <row r="52" spans="1:14" customHeight="1" ht="24">
-      <c r="A52" s="665" t="s">
-        <v>435</v>
-      </c>
+      <c r="A52" s="665"/>
       <c r="B52" s="666"/>
       <c r="C52" s="668"/>
       <c r="D52" s="668"/>
       <c r="E52" s="669"/>
-      <c r="F52" s="72" t="s">
-        <v>436</v>
-      </c>
-      <c r="G52" s="658" t="s">
-        <v>437</v>
-      </c>
+      <c r="F52" s="72"/>
+      <c r="G52" s="658"/>
       <c r="H52" s="659"/>
       <c r="I52" s="660"/>
       <c r="J52" s="642"/>
@@ -15284,19 +14902,13 @@
       <c r="M52" s="644"/>
     </row>
     <row r="53" spans="1:14" customHeight="1" ht="24">
-      <c r="A53" s="665" t="s">
-        <v>438</v>
-      </c>
+      <c r="A53" s="665"/>
       <c r="B53" s="666"/>
       <c r="C53" s="666"/>
       <c r="D53" s="666"/>
       <c r="E53" s="667"/>
-      <c r="F53" s="72" t="s">
-        <v>439</v>
-      </c>
-      <c r="G53" s="658" t="s">
-        <v>440</v>
-      </c>
+      <c r="F53" s="72"/>
+      <c r="G53" s="658"/>
       <c r="H53" s="659"/>
       <c r="I53" s="660"/>
       <c r="J53" s="642"/>
@@ -15305,19 +14917,13 @@
       <c r="M53" s="644"/>
     </row>
     <row r="54" spans="1:14" customHeight="1" ht="24">
-      <c r="A54" s="661" t="s">
-        <v>441</v>
-      </c>
+      <c r="A54" s="661"/>
       <c r="B54" s="662"/>
       <c r="C54" s="663"/>
       <c r="D54" s="663"/>
       <c r="E54" s="664"/>
-      <c r="F54" s="193" t="s">
-        <v>442</v>
-      </c>
-      <c r="G54" s="645" t="s">
-        <v>443</v>
-      </c>
+      <c r="F54" s="193"/>
+      <c r="G54" s="645"/>
       <c r="H54" s="646"/>
       <c r="I54" s="647"/>
       <c r="J54" s="642"/>
@@ -15327,11 +14933,11 @@
     </row>
     <row r="55" spans="1:14" customHeight="1" ht="39.75">
       <c r="A55" s="624" t="s">
-        <v>444</v>
+        <v>382</v>
       </c>
       <c r="B55" s="625"/>
       <c r="C55" s="670" t="s">
-        <v>445</v>
+        <v>383</v>
       </c>
       <c r="D55" s="670"/>
       <c r="E55" s="670"/>
@@ -15356,7 +14962,7 @@
       <c r="I56" s="243"/>
       <c r="J56" s="192"/>
       <c r="K56" s="605" t="s">
-        <v>446</v>
+        <v>384</v>
       </c>
       <c r="L56" s="605"/>
       <c r="M56" s="176"/>
@@ -15406,7 +15012,7 @@
     <row r="60" spans="1:14" customHeight="1" ht="25.5">
       <c r="A60" s="75"/>
       <c r="B60" s="677" t="s">
-        <v>447</v>
+        <v>385</v>
       </c>
       <c r="C60" s="678"/>
       <c r="D60" s="679"/>
@@ -15421,12 +15027,10 @@
     <row r="61" spans="1:14" customHeight="1" ht="20.25">
       <c r="A61" s="75"/>
       <c r="B61" s="712" t="s">
-        <v>448</v>
+        <v>386</v>
       </c>
       <c r="C61" s="713"/>
-      <c r="D61" s="131" t="s">
-        <v>449</v>
-      </c>
+      <c r="D61" s="131"/>
       <c r="F61" s="719"/>
       <c r="G61" s="720"/>
       <c r="H61" s="720"/>
@@ -15438,12 +15042,10 @@
     <row r="62" spans="1:14" customHeight="1" ht="9">
       <c r="A62" s="75"/>
       <c r="B62" s="701" t="s">
-        <v>450</v>
+        <v>387</v>
       </c>
       <c r="C62" s="702"/>
-      <c r="D62" s="680">
-        <v>123123</v>
-      </c>
+      <c r="D62" s="680"/>
       <c r="F62" s="722"/>
       <c r="G62" s="723"/>
       <c r="H62" s="723"/>
@@ -15458,7 +15060,7 @@
       <c r="C63" s="715"/>
       <c r="D63" s="681"/>
       <c r="F63" s="682" t="s">
-        <v>451</v>
+        <v>388</v>
       </c>
       <c r="G63" s="683"/>
       <c r="H63" s="683"/>
@@ -15470,12 +15072,10 @@
     <row r="64" spans="1:14" customHeight="1" ht="10.5">
       <c r="A64" s="75"/>
       <c r="B64" s="701" t="s">
-        <v>452</v>
+        <v>389</v>
       </c>
       <c r="C64" s="702"/>
-      <c r="D64" s="680" t="s">
-        <v>453</v>
-      </c>
+      <c r="D64" s="680"/>
       <c r="F64" s="77"/>
       <c r="G64" s="178"/>
       <c r="H64" s="178"/>
@@ -15491,14 +15091,14 @@
       <c r="C65" s="704"/>
       <c r="D65" s="705"/>
       <c r="F65" s="698" t="s">
-        <v>454</v>
+        <v>390</v>
       </c>
       <c r="G65" s="699"/>
       <c r="H65" s="699"/>
       <c r="I65" s="700"/>
       <c r="J65" s="78"/>
       <c r="K65" s="696" t="s">
-        <v>455</v>
+        <v>391</v>
       </c>
       <c r="L65" s="697"/>
       <c r="M65" s="76"/>
@@ -15520,7 +15120,7 @@
     </row>
     <row r="67" spans="1:14" customHeight="1" ht="28.5">
       <c r="A67" s="693" t="s">
-        <v>456</v>
+        <v>392</v>
       </c>
       <c r="B67" s="694"/>
       <c r="C67" s="694"/>
@@ -15555,7 +15155,7 @@
       <c r="C69" s="227"/>
       <c r="D69" s="227"/>
       <c r="E69" s="687" t="s">
-        <v>457</v>
+        <v>393</v>
       </c>
       <c r="F69" s="688"/>
       <c r="G69" s="688"/>
@@ -15583,7 +15183,7 @@
     </row>
     <row r="71" spans="1:14" customHeight="1" ht="10.5">
       <c r="A71" s="686" t="s">
-        <v>458</v>
+        <v>394</v>
       </c>
       <c r="B71" s="686"/>
       <c r="C71" s="686"/>
@@ -15762,45 +15362,45 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>459</v>
+        <v>395</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>460</v>
+        <v>396</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>461</v>
+        <v>397</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>462</v>
+        <v>398</v>
       </c>
       <c r="B2" t="s">
-        <v>463</v>
+        <v>399</v>
       </c>
       <c r="C2" t="s">
-        <v>464</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>465</v>
+        <v>401</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>466</v>
+        <v>402</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="B4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="B5" t="s">
-        <v>467</v>
+        <v>403</v>
       </c>
     </row>
   </sheetData>

</xml_diff>